<commit_message>
recalculate htse, ft boundaries
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A94DB64-9635-D541-AD57-9E1F129A7F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897E15E-B96D-2040-8521-526F9D8AEAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="6" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="35840" yWindow="-1100" windowWidth="38400" windowHeight="23500" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
-    <sheet name="MACRS" sheetId="1" r:id="rId1"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId2"/>
-    <sheet name="HTSE" sheetId="2" r:id="rId3"/>
-    <sheet name="FT" sheetId="11" r:id="rId4"/>
-    <sheet name="Boundaries" sheetId="10" r:id="rId5"/>
+    <sheet name="Boundaries" sheetId="10" r:id="rId1"/>
+    <sheet name="MACRS" sheetId="1" r:id="rId2"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId3"/>
+    <sheet name="HTSE" sheetId="2" r:id="rId4"/>
+    <sheet name="FT" sheetId="11" r:id="rId5"/>
     <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
     <sheet name="Tax rates" sheetId="12" r:id="rId7"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="211">
   <si>
     <t>Source</t>
   </si>
@@ -614,6 +614,66 @@
   </si>
   <si>
     <t>arizona</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Capacity (MWe)</t>
+  </si>
+  <si>
+    <t>HTSE (MWe)</t>
+  </si>
+  <si>
+    <t>FT (kg-H2)</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Days FT prod. for sto max cap.</t>
+  </si>
+  <si>
+    <t>Max elec. Price</t>
+  </si>
+  <si>
+    <t>Braidwood</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Davis-Besse</t>
+  </si>
+  <si>
+    <t>South Texas Project</t>
+  </si>
+  <si>
+    <t>HTSE Steps</t>
+  </si>
+  <si>
+    <t>FT Steps</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>H2 Storage</t>
+  </si>
+  <si>
+    <t>Location elec. Prices</t>
+  </si>
+  <si>
+    <t>Prairie-Island</t>
+  </si>
+  <si>
+    <t>6 units</t>
+  </si>
+  <si>
+    <t>18 units</t>
   </si>
 </sst>
 </file>
@@ -623,7 +683,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,8 +735,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,6 +753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -874,7 +947,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -911,10 +984,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2321,6 +2402,1785 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
+  <dimension ref="A1:L65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5">
+        <v>14.9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <f>-A12+14.9</f>
+        <v>-45.1</v>
+      </c>
+      <c r="C12" s="34">
+        <f>B12*25.13</f>
+        <v>-1133.3630000000001</v>
+      </c>
+      <c r="D12" s="34">
+        <f>ABS(C12)*48</f>
+        <v>54401.423999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>360</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B16" si="0">-A13+14.9</f>
+        <v>-345.1</v>
+      </c>
+      <c r="C13" s="34">
+        <f>B13*25.13</f>
+        <v>-8672.3629999999994</v>
+      </c>
+      <c r="D13" s="34">
+        <f t="shared" ref="D13:D16" si="1">ABS(C13)*48</f>
+        <v>416273.424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>720</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>-705.1</v>
+      </c>
+      <c r="C14" s="34">
+        <f>B14*25.13</f>
+        <v>-17719.163</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="1"/>
+        <v>850519.82400000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1080</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>-1065.0999999999999</v>
+      </c>
+      <c r="C15" s="34">
+        <f>B15*25.13</f>
+        <v>-26765.962999999996</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="1"/>
+        <v>1284766.2239999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1440</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>-1425.1</v>
+      </c>
+      <c r="C16" s="34">
+        <f>B16*25.13</f>
+        <v>-35812.762999999999</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="1"/>
+        <v>1719012.6239999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21">
+        <v>720</v>
+      </c>
+      <c r="C21">
+        <f>MAX(-B21+$B$15, -1000+$B$15)</f>
+        <v>-1785.1</v>
+      </c>
+      <c r="D21">
+        <f>-100+$B$5</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E21">
+        <f>C21*25.13</f>
+        <v>-44859.562999999995</v>
+      </c>
+      <c r="F21">
+        <f>D21*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22">
+        <v>360</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C23" si="2">MAX(-B22+$B$15, -1000+$B$15)</f>
+        <v>-1425.1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:D23" si="3">-100+$B$5</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:F22" si="4">C22*25.13</f>
+        <v>-35812.762999999999</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23">
+        <f>18*60</f>
+        <v>1080</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>-2065.1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E23">
+        <f>C23*25.13</f>
+        <v>-51895.962999999996</v>
+      </c>
+      <c r="F23">
+        <f>D23*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="37">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="37">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" s="37">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" s="37">
+        <v>6</v>
+      </c>
+      <c r="I26" s="39">
+        <v>7</v>
+      </c>
+      <c r="J26" s="37">
+        <v>8</v>
+      </c>
+      <c r="K26" s="39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>A21</f>
+        <v>Ref</v>
+      </c>
+      <c r="B27" s="38">
+        <f>$C21+B$26*ABS($C21-$D21)/9</f>
+        <v>-1785.1</v>
+      </c>
+      <c r="C27" s="40">
+        <f t="shared" ref="C27:K27" si="5">$C21+C$26*ABS($C21-$D21)/9</f>
+        <v>-1596.211111111111</v>
+      </c>
+      <c r="D27" s="38">
+        <f t="shared" si="5"/>
+        <v>-1407.3222222222221</v>
+      </c>
+      <c r="E27" s="40">
+        <f t="shared" si="5"/>
+        <v>-1218.4333333333334</v>
+      </c>
+      <c r="F27" s="38">
+        <f t="shared" si="5"/>
+        <v>-1029.5444444444443</v>
+      </c>
+      <c r="G27" s="40">
+        <f t="shared" si="5"/>
+        <v>-840.65555555555545</v>
+      </c>
+      <c r="H27" s="38">
+        <f t="shared" si="5"/>
+        <v>-651.76666666666665</v>
+      </c>
+      <c r="I27" s="40">
+        <f t="shared" si="5"/>
+        <v>-462.87777777777774</v>
+      </c>
+      <c r="J27" s="38">
+        <f t="shared" si="5"/>
+        <v>-273.98888888888882</v>
+      </c>
+      <c r="K27" s="40">
+        <f t="shared" si="5"/>
+        <v>-85.099999999999909</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f t="shared" ref="A28:A29" si="6">A22</f>
+        <v>6 units</v>
+      </c>
+      <c r="B28" s="38">
+        <f>$C22+B$26*ABS($C22-$D22)/9</f>
+        <v>-1425.1</v>
+      </c>
+      <c r="C28" s="40">
+        <f t="shared" ref="C28:K28" si="7">$C22+C$26*ABS($C22-$D22)/9</f>
+        <v>-1276.211111111111</v>
+      </c>
+      <c r="D28" s="38">
+        <f t="shared" si="7"/>
+        <v>-1127.3222222222221</v>
+      </c>
+      <c r="E28" s="40">
+        <f t="shared" si="7"/>
+        <v>-978.43333333333317</v>
+      </c>
+      <c r="F28" s="38">
+        <f t="shared" si="7"/>
+        <v>-829.54444444444437</v>
+      </c>
+      <c r="G28" s="40">
+        <f t="shared" si="7"/>
+        <v>-680.65555555555545</v>
+      </c>
+      <c r="H28" s="38">
+        <f t="shared" si="7"/>
+        <v>-531.76666666666654</v>
+      </c>
+      <c r="I28" s="40">
+        <f t="shared" si="7"/>
+        <v>-382.87777777777774</v>
+      </c>
+      <c r="J28" s="38">
+        <f t="shared" si="7"/>
+        <v>-233.98888888888882</v>
+      </c>
+      <c r="K28" s="40">
+        <f t="shared" si="7"/>
+        <v>-85.099999999999909</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f t="shared" si="6"/>
+        <v>18 units</v>
+      </c>
+      <c r="B29" s="38">
+        <f>$C23+B$26*ABS($C23-$D23)/9</f>
+        <v>-2065.1</v>
+      </c>
+      <c r="C29" s="40">
+        <f t="shared" ref="C29:K29" si="8">$C23+C$26*ABS($C23-$D23)/9</f>
+        <v>-1845.1</v>
+      </c>
+      <c r="D29" s="38">
+        <f t="shared" si="8"/>
+        <v>-1625.1</v>
+      </c>
+      <c r="E29" s="40">
+        <f t="shared" si="8"/>
+        <v>-1405.1</v>
+      </c>
+      <c r="F29" s="38">
+        <f t="shared" si="8"/>
+        <v>-1185.0999999999999</v>
+      </c>
+      <c r="G29" s="40">
+        <f t="shared" si="8"/>
+        <v>-965.09999999999991</v>
+      </c>
+      <c r="H29" s="38">
+        <f t="shared" si="8"/>
+        <v>-745.09999999999991</v>
+      </c>
+      <c r="I29" s="40">
+        <f t="shared" si="8"/>
+        <v>-525.09999999999991</v>
+      </c>
+      <c r="J29" s="38">
+        <f t="shared" si="8"/>
+        <v>-305.09999999999991</v>
+      </c>
+      <c r="K29" s="40">
+        <f t="shared" si="8"/>
+        <v>-85.099999999999909</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="37">
+        <v>0</v>
+      </c>
+      <c r="C32" s="39">
+        <v>1</v>
+      </c>
+      <c r="D32" s="37">
+        <v>2</v>
+      </c>
+      <c r="E32" s="39">
+        <v>3</v>
+      </c>
+      <c r="F32" s="37">
+        <v>4</v>
+      </c>
+      <c r="G32" s="39">
+        <v>5</v>
+      </c>
+      <c r="H32" s="37">
+        <v>6</v>
+      </c>
+      <c r="I32" s="39">
+        <v>7</v>
+      </c>
+      <c r="J32" s="37">
+        <v>8</v>
+      </c>
+      <c r="K32" s="39">
+        <v>9</v>
+      </c>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>A21</f>
+        <v>Ref</v>
+      </c>
+      <c r="B33" s="38">
+        <f>$E21+B$32*ABS($E21-$F21)/9</f>
+        <v>-44859.562999999995</v>
+      </c>
+      <c r="C33" s="40">
+        <f t="shared" ref="C33:K33" si="9">$E21+C$32*ABS($E21-$F21)/9</f>
+        <v>-40112.785222222214</v>
+      </c>
+      <c r="D33" s="38">
+        <f t="shared" si="9"/>
+        <v>-35366.00744444444</v>
+      </c>
+      <c r="E33" s="40">
+        <f t="shared" si="9"/>
+        <v>-30619.229666666666</v>
+      </c>
+      <c r="F33" s="38">
+        <f t="shared" si="9"/>
+        <v>-25872.451888888885</v>
+      </c>
+      <c r="G33" s="40">
+        <f t="shared" si="9"/>
+        <v>-21125.674111111108</v>
+      </c>
+      <c r="H33" s="38">
+        <f t="shared" si="9"/>
+        <v>-16378.896333333334</v>
+      </c>
+      <c r="I33" s="40">
+        <f t="shared" si="9"/>
+        <v>-11632.118555555557</v>
+      </c>
+      <c r="J33" s="38">
+        <f t="shared" si="9"/>
+        <v>-6885.3407777777757</v>
+      </c>
+      <c r="K33" s="40">
+        <f t="shared" si="9"/>
+        <v>-2138.5630000000019</v>
+      </c>
+      <c r="L33" s="39"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A35" si="10">A22</f>
+        <v>6 units</v>
+      </c>
+      <c r="B34" s="38">
+        <f>$E22+B$32*ABS($E22-$F22)/9</f>
+        <v>-35812.762999999999</v>
+      </c>
+      <c r="C34" s="40">
+        <f t="shared" ref="C34:K34" si="11">$E22+C$32*ABS($E22-$F22)/9</f>
+        <v>-32071.185222222222</v>
+      </c>
+      <c r="D34" s="38">
+        <f t="shared" si="11"/>
+        <v>-28329.607444444446</v>
+      </c>
+      <c r="E34" s="40">
+        <f t="shared" si="11"/>
+        <v>-24588.029666666669</v>
+      </c>
+      <c r="F34" s="38">
+        <f t="shared" si="11"/>
+        <v>-20846.451888888889</v>
+      </c>
+      <c r="G34" s="40">
+        <f t="shared" si="11"/>
+        <v>-17104.874111111109</v>
+      </c>
+      <c r="H34" s="38">
+        <f t="shared" si="11"/>
+        <v>-13363.296333333335</v>
+      </c>
+      <c r="I34" s="40">
+        <f t="shared" si="11"/>
+        <v>-9621.7185555555589</v>
+      </c>
+      <c r="J34" s="38">
+        <f t="shared" si="11"/>
+        <v>-5880.1407777777786</v>
+      </c>
+      <c r="K34" s="40">
+        <f t="shared" si="11"/>
+        <v>-2138.5630000000019</v>
+      </c>
+      <c r="L34" s="40"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f t="shared" si="10"/>
+        <v>18 units</v>
+      </c>
+      <c r="B35" s="38">
+        <f>$E23+B$32*ABS($E23-$F23)/9</f>
+        <v>-51895.962999999996</v>
+      </c>
+      <c r="C35" s="40">
+        <f>$E23+C$32*ABS($E23-$F23)/9</f>
+        <v>-46367.362999999998</v>
+      </c>
+      <c r="D35" s="38">
+        <f t="shared" ref="C35:K35" si="12">$E23+D$32*ABS($E23-$F23)/9</f>
+        <v>-40838.762999999999</v>
+      </c>
+      <c r="E35" s="40">
+        <f t="shared" si="12"/>
+        <v>-35310.163</v>
+      </c>
+      <c r="F35" s="38">
+        <f t="shared" si="12"/>
+        <v>-29781.562999999998</v>
+      </c>
+      <c r="G35" s="40">
+        <f t="shared" si="12"/>
+        <v>-24252.963</v>
+      </c>
+      <c r="H35" s="38">
+        <f t="shared" si="12"/>
+        <v>-18724.362999999998</v>
+      </c>
+      <c r="I35" s="40">
+        <f t="shared" si="12"/>
+        <v>-13195.763000000006</v>
+      </c>
+      <c r="J35" s="38">
+        <f t="shared" si="12"/>
+        <v>-7667.1630000000005</v>
+      </c>
+      <c r="K35" s="40">
+        <f t="shared" si="12"/>
+        <v>-2138.5630000000019</v>
+      </c>
+      <c r="L35" s="39"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="39"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39" t="str">
+        <f>A21</f>
+        <v>Ref</v>
+      </c>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39" t="str">
+        <f>A22</f>
+        <v>6 units</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39" t="str">
+        <f>A23</f>
+        <v>18 units</v>
+      </c>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="F39" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" t="s">
+        <v>195</v>
+      </c>
+      <c r="I39" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="41">
+        <f t="shared" ref="B40:B42" si="13">ROUNDUP(C40*$B$44/$C$44,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C40" s="41">
+        <v>934</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" s="40">
+        <f>ABS($E$21)*24*B40</f>
+        <v>2153259.0239999997</v>
+      </c>
+      <c r="F40" s="40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="40">
+        <f>ABS($E$22)*24*$B40</f>
+        <v>1719012.6239999998</v>
+      </c>
+      <c r="H40" s="40">
+        <v>0</v>
+      </c>
+      <c r="I40" s="40">
+        <f>ABS($E$23)*24*$B40</f>
+        <v>2491006.2239999999</v>
+      </c>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="39"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="41">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="C41" s="41">
+        <v>4231</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="40">
+        <f>ABS($E$21)*24*B41</f>
+        <v>7536406.5839999989</v>
+      </c>
+      <c r="F41" s="40">
+        <v>0</v>
+      </c>
+      <c r="G41" s="40">
+        <f t="shared" ref="G41:G44" si="14">ABS($E$22)*24*$B41</f>
+        <v>6016544.1839999994</v>
+      </c>
+      <c r="H41" s="40">
+        <v>0</v>
+      </c>
+      <c r="I41" s="40">
+        <f t="shared" ref="I41:I44" si="15">ABS($E$23)*24*$B41</f>
+        <v>8718521.784</v>
+      </c>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="39"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" s="41">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="C42" s="41">
+        <v>934</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="40">
+        <f>ABS($E$21)*24*B42</f>
+        <v>2153259.0239999997</v>
+      </c>
+      <c r="F42" s="40">
+        <v>0</v>
+      </c>
+      <c r="G42" s="40">
+        <f t="shared" si="14"/>
+        <v>1719012.6239999998</v>
+      </c>
+      <c r="H42" s="40">
+        <v>0</v>
+      </c>
+      <c r="I42" s="40">
+        <f t="shared" si="15"/>
+        <v>2491006.2239999999</v>
+      </c>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="39"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" s="41">
+        <f>ROUNDUP(C43*$B$44/$C$44,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="41">
+        <v>97</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="40">
+        <f>ABS($E$21)*24*B43</f>
+        <v>1076629.5119999999</v>
+      </c>
+      <c r="F43" s="40">
+        <v>0</v>
+      </c>
+      <c r="G43" s="40">
+        <f t="shared" si="14"/>
+        <v>859506.31199999992</v>
+      </c>
+      <c r="H43" s="40">
+        <v>0</v>
+      </c>
+      <c r="I43" s="40">
+        <f t="shared" si="15"/>
+        <v>1245503.112</v>
+      </c>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="41">
+        <v>14</v>
+      </c>
+      <c r="C44" s="41">
+        <v>8997</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" s="40">
+        <f>ABS($E$21)*24*B44</f>
+        <v>15072813.167999998</v>
+      </c>
+      <c r="F44" s="40">
+        <v>0</v>
+      </c>
+      <c r="G44" s="40">
+        <f t="shared" si="14"/>
+        <v>12033088.367999999</v>
+      </c>
+      <c r="H44" s="40">
+        <v>0</v>
+      </c>
+      <c r="I44" s="40">
+        <f t="shared" si="15"/>
+        <v>17437043.568</v>
+      </c>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="41">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="41">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46" s="41">
+        <v>5</v>
+      </c>
+      <c r="H46">
+        <v>6</v>
+      </c>
+      <c r="I46" s="41">
+        <v>7</v>
+      </c>
+      <c r="J46">
+        <v>8</v>
+      </c>
+      <c r="K46" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="str">
+        <f>A40</f>
+        <v>Braidwood</v>
+      </c>
+      <c r="B47" s="40">
+        <f>$D40+B$46*ABS($E40-$D40)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="40">
+        <f t="shared" ref="C47:K47" si="16">$D40+C$46*ABS($E40-$D40)/9</f>
+        <v>239251.00266666664</v>
+      </c>
+      <c r="D47" s="40">
+        <f t="shared" si="16"/>
+        <v>478502.00533333328</v>
+      </c>
+      <c r="E47" s="40">
+        <f t="shared" si="16"/>
+        <v>717753.00799999991</v>
+      </c>
+      <c r="F47" s="40">
+        <f t="shared" si="16"/>
+        <v>957004.01066666655</v>
+      </c>
+      <c r="G47" s="40">
+        <f t="shared" si="16"/>
+        <v>1196255.0133333332</v>
+      </c>
+      <c r="H47" s="40">
+        <f t="shared" si="16"/>
+        <v>1435506.0159999998</v>
+      </c>
+      <c r="I47" s="40">
+        <f t="shared" si="16"/>
+        <v>1674757.0186666665</v>
+      </c>
+      <c r="J47" s="40">
+        <f t="shared" si="16"/>
+        <v>1914008.0213333331</v>
+      </c>
+      <c r="K47" s="40">
+        <f t="shared" si="16"/>
+        <v>2153259.0239999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f t="shared" ref="A48:A51" si="17">A41</f>
+        <v>Cooper</v>
+      </c>
+      <c r="B48" s="40">
+        <f t="shared" ref="B48:K51" si="18">$D41+B$46*ABS($E41-$D41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="40">
+        <f t="shared" si="18"/>
+        <v>837378.50933333323</v>
+      </c>
+      <c r="D48" s="40">
+        <f t="shared" si="18"/>
+        <v>1674757.0186666665</v>
+      </c>
+      <c r="E48" s="40">
+        <f t="shared" si="18"/>
+        <v>2512135.5279999995</v>
+      </c>
+      <c r="F48" s="40">
+        <f t="shared" si="18"/>
+        <v>3349514.0373333329</v>
+      </c>
+      <c r="G48" s="40">
+        <f t="shared" si="18"/>
+        <v>4186892.5466666659</v>
+      </c>
+      <c r="H48" s="40">
+        <f t="shared" si="18"/>
+        <v>5024271.0559999989</v>
+      </c>
+      <c r="I48" s="40">
+        <f t="shared" si="18"/>
+        <v>5861649.5653333329</v>
+      </c>
+      <c r="J48" s="40">
+        <f t="shared" si="18"/>
+        <v>6699028.0746666659</v>
+      </c>
+      <c r="K48" s="40">
+        <f t="shared" si="18"/>
+        <v>7536406.5839999979</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f t="shared" si="17"/>
+        <v>Davis-Besse</v>
+      </c>
+      <c r="B49" s="40">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="C49" s="40">
+        <f t="shared" si="18"/>
+        <v>239251.00266666664</v>
+      </c>
+      <c r="D49" s="40">
+        <f t="shared" si="18"/>
+        <v>478502.00533333328</v>
+      </c>
+      <c r="E49" s="40">
+        <f t="shared" si="18"/>
+        <v>717753.00799999991</v>
+      </c>
+      <c r="F49" s="40">
+        <f t="shared" si="18"/>
+        <v>957004.01066666655</v>
+      </c>
+      <c r="G49" s="40">
+        <f t="shared" si="18"/>
+        <v>1196255.0133333332</v>
+      </c>
+      <c r="H49" s="40">
+        <f t="shared" si="18"/>
+        <v>1435506.0159999998</v>
+      </c>
+      <c r="I49" s="40">
+        <f t="shared" si="18"/>
+        <v>1674757.0186666665</v>
+      </c>
+      <c r="J49" s="40">
+        <f t="shared" si="18"/>
+        <v>1914008.0213333331</v>
+      </c>
+      <c r="K49" s="40">
+        <f t="shared" si="18"/>
+        <v>2153259.0239999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="str">
+        <f t="shared" si="17"/>
+        <v>Prairie-Island</v>
+      </c>
+      <c r="B50" s="40">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="C50" s="40">
+        <f t="shared" si="18"/>
+        <v>119625.50133333332</v>
+      </c>
+      <c r="D50" s="40">
+        <f t="shared" si="18"/>
+        <v>239251.00266666664</v>
+      </c>
+      <c r="E50" s="40">
+        <f t="shared" si="18"/>
+        <v>358876.50399999996</v>
+      </c>
+      <c r="F50" s="40">
+        <f t="shared" si="18"/>
+        <v>478502.00533333328</v>
+      </c>
+      <c r="G50" s="40">
+        <f t="shared" si="18"/>
+        <v>598127.5066666666</v>
+      </c>
+      <c r="H50" s="40">
+        <f t="shared" si="18"/>
+        <v>717753.00799999991</v>
+      </c>
+      <c r="I50" s="40">
+        <f t="shared" si="18"/>
+        <v>837378.50933333323</v>
+      </c>
+      <c r="J50" s="40">
+        <f t="shared" si="18"/>
+        <v>957004.01066666655</v>
+      </c>
+      <c r="K50" s="40">
+        <f t="shared" si="18"/>
+        <v>1076629.5119999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f t="shared" si="17"/>
+        <v>South Texas Project</v>
+      </c>
+      <c r="B51" s="40">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="C51" s="40">
+        <f>$D44+C$46*ABS($E44-$D44)/9</f>
+        <v>1674757.0186666665</v>
+      </c>
+      <c r="D51" s="40">
+        <f t="shared" si="18"/>
+        <v>3349514.0373333329</v>
+      </c>
+      <c r="E51" s="40">
+        <f t="shared" si="18"/>
+        <v>5024271.0559999989</v>
+      </c>
+      <c r="F51" s="40">
+        <f t="shared" si="18"/>
+        <v>6699028.0746666659</v>
+      </c>
+      <c r="G51" s="40">
+        <f t="shared" si="18"/>
+        <v>8373785.0933333319</v>
+      </c>
+      <c r="H51" s="40">
+        <f t="shared" si="18"/>
+        <v>10048542.111999998</v>
+      </c>
+      <c r="I51" s="40">
+        <f t="shared" si="18"/>
+        <v>11723299.130666666</v>
+      </c>
+      <c r="J51" s="40">
+        <f t="shared" si="18"/>
+        <v>13398056.149333332</v>
+      </c>
+      <c r="K51" s="40">
+        <f t="shared" si="18"/>
+        <v>15072813.167999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" s="41">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53" s="41">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53" s="41">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>6</v>
+      </c>
+      <c r="I53" s="41">
+        <v>7</v>
+      </c>
+      <c r="J53">
+        <v>8</v>
+      </c>
+      <c r="K53" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="str">
+        <f>A47</f>
+        <v>Braidwood</v>
+      </c>
+      <c r="B54" s="40">
+        <f>$F40+B$46*ABS($G40-$F40)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="40">
+        <f t="shared" ref="C54:K54" si="19">$F40+C$46*ABS($G40-$F40)/9</f>
+        <v>191001.40266666666</v>
+      </c>
+      <c r="D54" s="40">
+        <f t="shared" si="19"/>
+        <v>382002.80533333332</v>
+      </c>
+      <c r="E54" s="40">
+        <f t="shared" si="19"/>
+        <v>573004.20799999998</v>
+      </c>
+      <c r="F54" s="40">
+        <f t="shared" si="19"/>
+        <v>764005.61066666665</v>
+      </c>
+      <c r="G54" s="40">
+        <f t="shared" si="19"/>
+        <v>955007.01333333319</v>
+      </c>
+      <c r="H54" s="40">
+        <f t="shared" si="19"/>
+        <v>1146008.416</v>
+      </c>
+      <c r="I54" s="40">
+        <f t="shared" si="19"/>
+        <v>1337009.8186666665</v>
+      </c>
+      <c r="J54" s="40">
+        <f t="shared" si="19"/>
+        <v>1528011.2213333333</v>
+      </c>
+      <c r="K54" s="40">
+        <f t="shared" si="19"/>
+        <v>1719012.6239999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="str">
+        <f t="shared" ref="A55:A58" si="20">A48</f>
+        <v>Cooper</v>
+      </c>
+      <c r="B55" s="40">
+        <f t="shared" ref="B55:K58" si="21">$F41+B$46*ABS($G41-$F41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="40">
+        <f t="shared" si="21"/>
+        <v>668504.90933333326</v>
+      </c>
+      <c r="D55" s="40">
+        <f t="shared" si="21"/>
+        <v>1337009.8186666665</v>
+      </c>
+      <c r="E55" s="40">
+        <f t="shared" si="21"/>
+        <v>2005514.7279999997</v>
+      </c>
+      <c r="F55" s="40">
+        <f t="shared" si="21"/>
+        <v>2674019.637333333</v>
+      </c>
+      <c r="G55" s="40">
+        <f t="shared" si="21"/>
+        <v>3342524.5466666664</v>
+      </c>
+      <c r="H55" s="40">
+        <f t="shared" si="21"/>
+        <v>4011029.4559999993</v>
+      </c>
+      <c r="I55" s="40">
+        <f t="shared" si="21"/>
+        <v>4679534.3653333327</v>
+      </c>
+      <c r="J55" s="40">
+        <f t="shared" si="21"/>
+        <v>5348039.2746666661</v>
+      </c>
+      <c r="K55" s="40">
+        <f t="shared" si="21"/>
+        <v>6016544.1839999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="str">
+        <f t="shared" si="20"/>
+        <v>Davis-Besse</v>
+      </c>
+      <c r="B56" s="40">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="C56" s="40">
+        <f t="shared" si="21"/>
+        <v>191001.40266666666</v>
+      </c>
+      <c r="D56" s="40">
+        <f t="shared" si="21"/>
+        <v>382002.80533333332</v>
+      </c>
+      <c r="E56" s="40">
+        <f t="shared" si="21"/>
+        <v>573004.20799999998</v>
+      </c>
+      <c r="F56" s="40">
+        <f t="shared" si="21"/>
+        <v>764005.61066666665</v>
+      </c>
+      <c r="G56" s="40">
+        <f t="shared" si="21"/>
+        <v>955007.01333333319</v>
+      </c>
+      <c r="H56" s="40">
+        <f t="shared" si="21"/>
+        <v>1146008.416</v>
+      </c>
+      <c r="I56" s="40">
+        <f t="shared" si="21"/>
+        <v>1337009.8186666665</v>
+      </c>
+      <c r="J56" s="40">
+        <f t="shared" si="21"/>
+        <v>1528011.2213333333</v>
+      </c>
+      <c r="K56" s="40">
+        <f t="shared" si="21"/>
+        <v>1719012.6239999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f t="shared" si="20"/>
+        <v>Prairie-Island</v>
+      </c>
+      <c r="B57" s="40">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="C57" s="40">
+        <f t="shared" si="21"/>
+        <v>95500.701333333331</v>
+      </c>
+      <c r="D57" s="40">
+        <f t="shared" si="21"/>
+        <v>191001.40266666666</v>
+      </c>
+      <c r="E57" s="40">
+        <f t="shared" si="21"/>
+        <v>286502.10399999999</v>
+      </c>
+      <c r="F57" s="40">
+        <f t="shared" si="21"/>
+        <v>382002.80533333332</v>
+      </c>
+      <c r="G57" s="40">
+        <f t="shared" si="21"/>
+        <v>477503.5066666666</v>
+      </c>
+      <c r="H57" s="40">
+        <f t="shared" si="21"/>
+        <v>573004.20799999998</v>
+      </c>
+      <c r="I57" s="40">
+        <f t="shared" si="21"/>
+        <v>668504.90933333326</v>
+      </c>
+      <c r="J57" s="40">
+        <f t="shared" si="21"/>
+        <v>764005.61066666665</v>
+      </c>
+      <c r="K57" s="40">
+        <f t="shared" si="21"/>
+        <v>859506.31199999992</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="str">
+        <f t="shared" si="20"/>
+        <v>South Texas Project</v>
+      </c>
+      <c r="B58" s="40">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="C58" s="40">
+        <f t="shared" si="21"/>
+        <v>1337009.8186666665</v>
+      </c>
+      <c r="D58" s="40">
+        <f t="shared" si="21"/>
+        <v>2674019.637333333</v>
+      </c>
+      <c r="E58" s="40">
+        <f t="shared" si="21"/>
+        <v>4011029.4559999993</v>
+      </c>
+      <c r="F58" s="40">
+        <f t="shared" si="21"/>
+        <v>5348039.2746666661</v>
+      </c>
+      <c r="G58" s="40">
+        <f t="shared" si="21"/>
+        <v>6685049.0933333328</v>
+      </c>
+      <c r="H58" s="40">
+        <f t="shared" si="21"/>
+        <v>8022058.9119999986</v>
+      </c>
+      <c r="I58" s="40">
+        <f t="shared" si="21"/>
+        <v>9359068.7306666654</v>
+      </c>
+      <c r="J58" s="40">
+        <f t="shared" si="21"/>
+        <v>10696078.549333332</v>
+      </c>
+      <c r="K58" s="40">
+        <f t="shared" si="21"/>
+        <v>12033088.367999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60" s="41">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="41">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60" s="41">
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>6</v>
+      </c>
+      <c r="I60" s="41">
+        <v>7</v>
+      </c>
+      <c r="J60">
+        <v>8</v>
+      </c>
+      <c r="K60" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f>A54</f>
+        <v>Braidwood</v>
+      </c>
+      <c r="B61" s="40">
+        <f>$H40+B$46*ABS($I40-$H40)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C61" s="40">
+        <f t="shared" ref="C61:K61" si="22">$H40+C$46*ABS($I40-$H40)/9</f>
+        <v>276778.46933333331</v>
+      </c>
+      <c r="D61" s="40">
+        <f t="shared" si="22"/>
+        <v>553556.93866666663</v>
+      </c>
+      <c r="E61" s="40">
+        <f t="shared" si="22"/>
+        <v>830335.40800000005</v>
+      </c>
+      <c r="F61" s="40">
+        <f t="shared" si="22"/>
+        <v>1107113.8773333333</v>
+      </c>
+      <c r="G61" s="40">
+        <f t="shared" si="22"/>
+        <v>1383892.3466666667</v>
+      </c>
+      <c r="H61" s="40">
+        <f t="shared" si="22"/>
+        <v>1660670.8160000001</v>
+      </c>
+      <c r="I61" s="40">
+        <f t="shared" si="22"/>
+        <v>1937449.2853333333</v>
+      </c>
+      <c r="J61" s="40">
+        <f t="shared" si="22"/>
+        <v>2214227.7546666665</v>
+      </c>
+      <c r="K61" s="40">
+        <f t="shared" si="22"/>
+        <v>2491006.2239999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="str">
+        <f t="shared" ref="A62:A65" si="23">A55</f>
+        <v>Cooper</v>
+      </c>
+      <c r="B62" s="40">
+        <f t="shared" ref="B62:K65" si="24">$H41+B$46*ABS($I41-$H41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C62" s="40">
+        <f t="shared" si="24"/>
+        <v>968724.64266666665</v>
+      </c>
+      <c r="D62" s="40">
+        <f t="shared" si="24"/>
+        <v>1937449.2853333333</v>
+      </c>
+      <c r="E62" s="40">
+        <f t="shared" si="24"/>
+        <v>2906173.9279999998</v>
+      </c>
+      <c r="F62" s="40">
+        <f t="shared" si="24"/>
+        <v>3874898.5706666666</v>
+      </c>
+      <c r="G62" s="40">
+        <f t="shared" si="24"/>
+        <v>4843623.2133333338</v>
+      </c>
+      <c r="H62" s="40">
+        <f t="shared" si="24"/>
+        <v>5812347.8559999997</v>
+      </c>
+      <c r="I62" s="40">
+        <f t="shared" si="24"/>
+        <v>6781072.4986666664</v>
+      </c>
+      <c r="J62" s="40">
+        <f t="shared" si="24"/>
+        <v>7749797.1413333332</v>
+      </c>
+      <c r="K62" s="40">
+        <f t="shared" si="24"/>
+        <v>8718521.784</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="str">
+        <f t="shared" si="23"/>
+        <v>Davis-Besse</v>
+      </c>
+      <c r="B63" s="40">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="C63" s="40">
+        <f t="shared" si="24"/>
+        <v>276778.46933333331</v>
+      </c>
+      <c r="D63" s="40">
+        <f t="shared" si="24"/>
+        <v>553556.93866666663</v>
+      </c>
+      <c r="E63" s="40">
+        <f t="shared" si="24"/>
+        <v>830335.40800000005</v>
+      </c>
+      <c r="F63" s="40">
+        <f t="shared" si="24"/>
+        <v>1107113.8773333333</v>
+      </c>
+      <c r="G63" s="40">
+        <f t="shared" si="24"/>
+        <v>1383892.3466666667</v>
+      </c>
+      <c r="H63" s="40">
+        <f t="shared" si="24"/>
+        <v>1660670.8160000001</v>
+      </c>
+      <c r="I63" s="40">
+        <f t="shared" si="24"/>
+        <v>1937449.2853333333</v>
+      </c>
+      <c r="J63" s="40">
+        <f t="shared" si="24"/>
+        <v>2214227.7546666665</v>
+      </c>
+      <c r="K63" s="40">
+        <f t="shared" si="24"/>
+        <v>2491006.2239999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f t="shared" si="23"/>
+        <v>Prairie-Island</v>
+      </c>
+      <c r="B64" s="40">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="C64" s="40">
+        <f t="shared" si="24"/>
+        <v>138389.23466666666</v>
+      </c>
+      <c r="D64" s="40">
+        <f t="shared" si="24"/>
+        <v>276778.46933333331</v>
+      </c>
+      <c r="E64" s="40">
+        <f t="shared" si="24"/>
+        <v>415167.70400000003</v>
+      </c>
+      <c r="F64" s="40">
+        <f t="shared" si="24"/>
+        <v>553556.93866666663</v>
+      </c>
+      <c r="G64" s="40">
+        <f t="shared" si="24"/>
+        <v>691946.17333333334</v>
+      </c>
+      <c r="H64" s="40">
+        <f t="shared" si="24"/>
+        <v>830335.40800000005</v>
+      </c>
+      <c r="I64" s="40">
+        <f t="shared" si="24"/>
+        <v>968724.64266666665</v>
+      </c>
+      <c r="J64" s="40">
+        <f t="shared" si="24"/>
+        <v>1107113.8773333333</v>
+      </c>
+      <c r="K64" s="40">
+        <f t="shared" si="24"/>
+        <v>1245503.112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f t="shared" si="23"/>
+        <v>South Texas Project</v>
+      </c>
+      <c r="B65" s="40">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="C65" s="40">
+        <f t="shared" si="24"/>
+        <v>1937449.2853333333</v>
+      </c>
+      <c r="D65" s="40">
+        <f t="shared" si="24"/>
+        <v>3874898.5706666666</v>
+      </c>
+      <c r="E65" s="40">
+        <f t="shared" si="24"/>
+        <v>5812347.8559999997</v>
+      </c>
+      <c r="F65" s="40">
+        <f t="shared" si="24"/>
+        <v>7749797.1413333332</v>
+      </c>
+      <c r="G65" s="40">
+        <f t="shared" si="24"/>
+        <v>9687246.4266666677</v>
+      </c>
+      <c r="H65" s="40">
+        <f t="shared" si="24"/>
+        <v>11624695.711999999</v>
+      </c>
+      <c r="I65" s="40">
+        <f t="shared" si="24"/>
+        <v>13562144.997333333</v>
+      </c>
+      <c r="J65" s="40">
+        <f t="shared" si="24"/>
+        <v>15499594.282666666</v>
+      </c>
+      <c r="K65" s="40">
+        <f t="shared" si="24"/>
+        <v>17437043.568</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17762179-2135-43B7-98DA-D4A6A7868310}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -2346,10 +4206,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="35"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2477,7 +4337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -2517,26 +4377,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2608,15 +4468,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2694,22 +4554,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2723,11 +4583,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -2768,7 +4628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -2943,7 +4803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D919D22-7A01-ED42-B8B2-84358A3D7717}">
   <dimension ref="A1:P25"/>
   <sheetViews>
@@ -3450,230 +5310,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5">
-        <v>14.9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>60</v>
-      </c>
-      <c r="B12">
-        <f>-A12+14.9</f>
-        <v>-45.1</v>
-      </c>
-      <c r="C12" s="35">
-        <f>B12*25.13</f>
-        <v>-1133.3630000000001</v>
-      </c>
-      <c r="D12" s="35">
-        <f>ABS(C12)*48</f>
-        <v>54401.423999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>360</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ref="B13:B16" si="0">-A13+14.9</f>
-        <v>-345.1</v>
-      </c>
-      <c r="C13" s="35">
-        <f>B13*25.13</f>
-        <v>-8672.3629999999994</v>
-      </c>
-      <c r="D13" s="35">
-        <f t="shared" ref="D13:D16" si="1">ABS(C13)*48</f>
-        <v>416273.424</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>720</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>-705.1</v>
-      </c>
-      <c r="C14" s="35">
-        <f>B14*25.13</f>
-        <v>-17719.163</v>
-      </c>
-      <c r="D14" s="35">
-        <f t="shared" si="1"/>
-        <v>850519.82400000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1080</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>-1065.0999999999999</v>
-      </c>
-      <c r="C15" s="35">
-        <f>B15*25.13</f>
-        <v>-26765.962999999996</v>
-      </c>
-      <c r="D15" s="35">
-        <f t="shared" si="1"/>
-        <v>1284766.2239999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1440</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>-1425.1</v>
-      </c>
-      <c r="C16" s="35">
-        <f>B16*25.13</f>
-        <v>-35812.762999999999</v>
-      </c>
-      <c r="D16" s="35">
-        <f t="shared" si="1"/>
-        <v>1719012.6239999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
@@ -3810,7 +5446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Calculate smr total capacity for SA cases
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897E15E-B96D-2040-8521-526F9D8AEAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41FB75-9BC8-8843-BCF2-ADBD1CAB561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-1100" windowWidth="38400" windowHeight="23500" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-460" yWindow="600" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="Boundaries" sheetId="10" r:id="rId1"/>
-    <sheet name="MACRS" sheetId="1" r:id="rId2"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId3"/>
-    <sheet name="HTSE" sheetId="2" r:id="rId4"/>
-    <sheet name="FT" sheetId="11" r:id="rId5"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
-    <sheet name="Tax rates" sheetId="12" r:id="rId7"/>
+    <sheet name="SMR" sheetId="13" r:id="rId2"/>
+    <sheet name="MACRS" sheetId="1" r:id="rId3"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId4"/>
+    <sheet name="HTSE" sheetId="2" r:id="rId5"/>
+    <sheet name="FT" sheetId="11" r:id="rId6"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId7"/>
+    <sheet name="Tax rates" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="222">
   <si>
     <t>Source</t>
   </si>
@@ -661,6 +662,12 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
     <t>H2 Storage</t>
   </si>
   <si>
@@ -674,6 +681,33 @@
   </si>
   <si>
     <t>18 units</t>
+  </si>
+  <si>
+    <t>Find Abdalla's report citation</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>CAPEX ($/MWe)</t>
+  </si>
+  <si>
+    <t>720MWe ((2020)$ USD)</t>
+  </si>
+  <si>
+    <t>OPEX ($/MWh)</t>
+  </si>
+  <si>
+    <t>SA Capacity</t>
+  </si>
+  <si>
+    <t># modules</t>
+  </si>
+  <si>
+    <t>Unit capacity (MWe)</t>
+  </si>
+  <si>
+    <t>Total capacity (MWe)</t>
   </si>
 </sst>
 </file>
@@ -947,7 +981,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -985,17 +1019,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2405,7 +2438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
@@ -2612,7 +2645,7 @@
         <v>1719012.6239999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>181</v>
       </c>
@@ -2620,27 +2653,27 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" t="s">
         <v>195</v>
       </c>
@@ -2654,7 +2687,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>205</v>
       </c>
@@ -2678,9 +2711,9 @@
         <v>-2138.5629999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B22">
         <v>360</v>
@@ -2702,9 +2735,9 @@
         <v>-2138.5629999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B23">
         <f>18*60</f>
@@ -2727,684 +2760,623 @@
         <v>-2138.5629999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B26" s="35">
         <v>0</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="35">
         <v>2</v>
       </c>
       <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="35">
         <v>4</v>
       </c>
       <c r="G26">
         <v>5</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="35">
         <v>6</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26">
         <v>7</v>
       </c>
-      <c r="J26" s="37">
+      <c r="J26" s="35">
         <v>8</v>
       </c>
-      <c r="K26" s="39">
+      <c r="K26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>A21</f>
         <v>Ref</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="36">
         <f>$C21+B$26*ABS($C21-$D21)/9</f>
         <v>-1785.1</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="34">
         <f t="shared" ref="C27:K27" si="5">$C21+C$26*ABS($C21-$D21)/9</f>
         <v>-1596.211111111111</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="36">
         <f t="shared" si="5"/>
         <v>-1407.3222222222221</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="34">
         <f t="shared" si="5"/>
         <v>-1218.4333333333334</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="36">
         <f t="shared" si="5"/>
         <v>-1029.5444444444443</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="34">
         <f t="shared" si="5"/>
         <v>-840.65555555555545</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="36">
         <f t="shared" si="5"/>
         <v>-651.76666666666665</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="34">
         <f t="shared" si="5"/>
         <v>-462.87777777777774</v>
       </c>
-      <c r="J27" s="38">
+      <c r="J27" s="36">
         <f t="shared" si="5"/>
         <v>-273.98888888888882</v>
       </c>
-      <c r="K27" s="40">
+      <c r="K27" s="34">
         <f t="shared" si="5"/>
         <v>-85.099999999999909</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" ref="A28:A29" si="6">A22</f>
         <v>6 units</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="36">
         <f>$C22+B$26*ABS($C22-$D22)/9</f>
         <v>-1425.1</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="34">
         <f t="shared" ref="C28:K28" si="7">$C22+C$26*ABS($C22-$D22)/9</f>
         <v>-1276.211111111111</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="36">
         <f t="shared" si="7"/>
         <v>-1127.3222222222221</v>
       </c>
-      <c r="E28" s="40">
+      <c r="E28" s="34">
         <f t="shared" si="7"/>
         <v>-978.43333333333317</v>
       </c>
-      <c r="F28" s="38">
+      <c r="F28" s="36">
         <f t="shared" si="7"/>
         <v>-829.54444444444437</v>
       </c>
-      <c r="G28" s="40">
+      <c r="G28" s="34">
         <f t="shared" si="7"/>
         <v>-680.65555555555545</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="36">
         <f t="shared" si="7"/>
         <v>-531.76666666666654</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="34">
         <f t="shared" si="7"/>
         <v>-382.87777777777774</v>
       </c>
-      <c r="J28" s="38">
+      <c r="J28" s="36">
         <f t="shared" si="7"/>
         <v>-233.98888888888882</v>
       </c>
-      <c r="K28" s="40">
+      <c r="K28" s="34">
         <f t="shared" si="7"/>
         <v>-85.099999999999909</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f t="shared" si="6"/>
         <v>18 units</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="36">
         <f>$C23+B$26*ABS($C23-$D23)/9</f>
         <v>-2065.1</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="34">
         <f t="shared" ref="C29:K29" si="8">$C23+C$26*ABS($C23-$D23)/9</f>
         <v>-1845.1</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="36">
         <f t="shared" si="8"/>
         <v>-1625.1</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="34">
         <f t="shared" si="8"/>
         <v>-1405.1</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="36">
         <f t="shared" si="8"/>
         <v>-1185.0999999999999</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="34">
         <f t="shared" si="8"/>
         <v>-965.09999999999991</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="36">
         <f t="shared" si="8"/>
         <v>-745.09999999999991</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="34">
         <f t="shared" si="8"/>
         <v>-525.09999999999991</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J29" s="36">
         <f t="shared" si="8"/>
         <v>-305.09999999999991</v>
       </c>
-      <c r="K29" s="40">
+      <c r="K29" s="34">
         <f t="shared" si="8"/>
         <v>-85.099999999999909</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>204</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B32" s="37">
+      <c r="B32" s="35">
         <v>0</v>
       </c>
-      <c r="C32" s="39">
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="37">
+      <c r="D32" s="35">
         <v>2</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32">
         <v>3</v>
       </c>
-      <c r="F32" s="37">
+      <c r="F32" s="35">
         <v>4</v>
       </c>
-      <c r="G32" s="39">
+      <c r="G32">
         <v>5</v>
       </c>
-      <c r="H32" s="37">
+      <c r="H32" s="35">
         <v>6</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32">
         <v>7</v>
       </c>
-      <c r="J32" s="37">
+      <c r="J32" s="35">
         <v>8</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32">
         <v>9</v>
       </c>
-      <c r="L32" s="39"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>A21</f>
         <v>Ref</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="36">
         <f>$E21+B$32*ABS($E21-$F21)/9</f>
         <v>-44859.562999999995</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="34">
         <f t="shared" ref="C33:K33" si="9">$E21+C$32*ABS($E21-$F21)/9</f>
         <v>-40112.785222222214</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="36">
         <f t="shared" si="9"/>
         <v>-35366.00744444444</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="34">
         <f t="shared" si="9"/>
         <v>-30619.229666666666</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="36">
         <f t="shared" si="9"/>
         <v>-25872.451888888885</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G33" s="34">
         <f t="shared" si="9"/>
         <v>-21125.674111111108</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="36">
         <f t="shared" si="9"/>
         <v>-16378.896333333334</v>
       </c>
-      <c r="I33" s="40">
+      <c r="I33" s="34">
         <f t="shared" si="9"/>
         <v>-11632.118555555557</v>
       </c>
-      <c r="J33" s="38">
+      <c r="J33" s="36">
         <f t="shared" si="9"/>
         <v>-6885.3407777777757</v>
       </c>
-      <c r="K33" s="40">
+      <c r="K33" s="34">
         <f t="shared" si="9"/>
         <v>-2138.5630000000019</v>
       </c>
-      <c r="L33" s="39"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f t="shared" ref="A34:A35" si="10">A22</f>
         <v>6 units</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="36">
         <f>$E22+B$32*ABS($E22-$F22)/9</f>
         <v>-35812.762999999999</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="34">
         <f t="shared" ref="C34:K34" si="11">$E22+C$32*ABS($E22-$F22)/9</f>
         <v>-32071.185222222222</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="36">
         <f t="shared" si="11"/>
         <v>-28329.607444444446</v>
       </c>
-      <c r="E34" s="40">
+      <c r="E34" s="34">
         <f t="shared" si="11"/>
         <v>-24588.029666666669</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="36">
         <f t="shared" si="11"/>
         <v>-20846.451888888889</v>
       </c>
-      <c r="G34" s="40">
+      <c r="G34" s="34">
         <f t="shared" si="11"/>
         <v>-17104.874111111109</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="36">
         <f t="shared" si="11"/>
         <v>-13363.296333333335</v>
       </c>
-      <c r="I34" s="40">
+      <c r="I34" s="34">
         <f t="shared" si="11"/>
         <v>-9621.7185555555589</v>
       </c>
-      <c r="J34" s="38">
+      <c r="J34" s="36">
         <f t="shared" si="11"/>
         <v>-5880.1407777777786</v>
       </c>
-      <c r="K34" s="40">
+      <c r="K34" s="34">
         <f t="shared" si="11"/>
         <v>-2138.5630000000019</v>
       </c>
-      <c r="L34" s="40"/>
+      <c r="L34" s="34"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f t="shared" si="10"/>
         <v>18 units</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="36">
         <f>$E23+B$32*ABS($E23-$F23)/9</f>
         <v>-51895.962999999996</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="34">
         <f>$E23+C$32*ABS($E23-$F23)/9</f>
         <v>-46367.362999999998</v>
       </c>
-      <c r="D35" s="38">
-        <f t="shared" ref="C35:K35" si="12">$E23+D$32*ABS($E23-$F23)/9</f>
+      <c r="D35" s="36">
+        <f t="shared" ref="D35:K35" si="12">$E23+D$32*ABS($E23-$F23)/9</f>
         <v>-40838.762999999999</v>
       </c>
-      <c r="E35" s="40">
+      <c r="E35" s="34">
         <f t="shared" si="12"/>
         <v>-35310.163</v>
       </c>
-      <c r="F35" s="38">
+      <c r="F35" s="36">
         <f t="shared" si="12"/>
         <v>-29781.562999999998</v>
       </c>
-      <c r="G35" s="40">
+      <c r="G35" s="34">
         <f t="shared" si="12"/>
         <v>-24252.963</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="36">
         <f t="shared" si="12"/>
         <v>-18724.362999999998</v>
       </c>
-      <c r="I35" s="40">
+      <c r="I35" s="34">
         <f t="shared" si="12"/>
         <v>-13195.763000000006</v>
       </c>
-      <c r="J35" s="38">
+      <c r="J35" s="36">
         <f t="shared" si="12"/>
         <v>-7667.1630000000005</v>
       </c>
-      <c r="K35" s="40">
+      <c r="K35" s="34">
         <f t="shared" si="12"/>
         <v>-2138.5630000000019</v>
       </c>
-      <c r="L35" s="39"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="39"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39" t="str">
+      <c r="A38" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" t="str">
         <f>A21</f>
         <v>Ref</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39" t="str">
+      <c r="F38" t="str">
         <f>A22</f>
         <v>6 units</v>
       </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39" t="str">
+      <c r="H38" t="str">
         <f>A23</f>
         <v>18 units</v>
       </c>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>207</v>
-      </c>
-      <c r="B39" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="37" t="s">
         <v>198</v>
       </c>
       <c r="D39" t="s">
         <v>195</v>
       </c>
-      <c r="E39" s="39" t="s">
+      <c r="E39" t="s">
         <v>196</v>
       </c>
       <c r="F39" t="s">
         <v>195</v>
       </c>
-      <c r="G39" s="39" t="s">
+      <c r="G39" t="s">
         <v>196</v>
       </c>
       <c r="H39" t="s">
         <v>195</v>
       </c>
-      <c r="I39" s="39" t="s">
+      <c r="I39" t="s">
         <v>196</v>
       </c>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>199</v>
       </c>
-      <c r="B40" s="41">
+      <c r="B40" s="37">
         <f t="shared" ref="B40:B42" si="13">ROUNDUP(C40*$B$44/$C$44,0)</f>
         <v>2</v>
       </c>
-      <c r="C40" s="41">
+      <c r="C40" s="37">
         <v>934</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40" s="40">
+      <c r="E40" s="34">
         <f>ABS($E$21)*24*B40</f>
         <v>2153259.0239999997</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F40" s="34">
         <v>0</v>
       </c>
-      <c r="G40" s="40">
+      <c r="G40" s="34">
         <f>ABS($E$22)*24*$B40</f>
         <v>1719012.6239999998</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H40" s="34">
         <v>0</v>
       </c>
-      <c r="I40" s="40">
+      <c r="I40" s="34">
         <f>ABS($E$23)*24*$B40</f>
         <v>2491006.2239999999</v>
       </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="39"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>200</v>
       </c>
-      <c r="B41" s="41">
+      <c r="B41" s="37">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="37">
         <v>4231</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41" s="40">
+      <c r="E41" s="34">
         <f>ABS($E$21)*24*B41</f>
         <v>7536406.5839999989</v>
       </c>
-      <c r="F41" s="40">
+      <c r="F41" s="34">
         <v>0</v>
       </c>
-      <c r="G41" s="40">
+      <c r="G41" s="34">
         <f t="shared" ref="G41:G44" si="14">ABS($E$22)*24*$B41</f>
         <v>6016544.1839999994</v>
       </c>
-      <c r="H41" s="40">
+      <c r="H41" s="34">
         <v>0</v>
       </c>
-      <c r="I41" s="40">
+      <c r="I41" s="34">
         <f t="shared" ref="I41:I44" si="15">ABS($E$23)*24*$B41</f>
         <v>8718521.784</v>
       </c>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="39"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>201</v>
       </c>
-      <c r="B42" s="41">
+      <c r="B42" s="37">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="C42" s="41">
+      <c r="C42" s="37">
         <v>934</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
-      <c r="E42" s="40">
+      <c r="E42" s="34">
         <f>ABS($E$21)*24*B42</f>
         <v>2153259.0239999997</v>
       </c>
-      <c r="F42" s="40">
+      <c r="F42" s="34">
         <v>0</v>
       </c>
-      <c r="G42" s="40">
+      <c r="G42" s="34">
         <f t="shared" si="14"/>
         <v>1719012.6239999998</v>
       </c>
-      <c r="H42" s="40">
+      <c r="H42" s="34">
         <v>0</v>
       </c>
-      <c r="I42" s="40">
+      <c r="I42" s="34">
         <f t="shared" si="15"/>
         <v>2491006.2239999999</v>
       </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="39"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>208</v>
-      </c>
-      <c r="B43" s="41">
+        <v>210</v>
+      </c>
+      <c r="B43" s="37">
         <f>ROUNDUP(C43*$B$44/$C$44,0)</f>
         <v>1</v>
       </c>
-      <c r="C43" s="41">
+      <c r="C43" s="37">
         <v>97</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
-      <c r="E43" s="40">
+      <c r="E43" s="34">
         <f>ABS($E$21)*24*B43</f>
         <v>1076629.5119999999</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="34">
         <v>0</v>
       </c>
-      <c r="G43" s="40">
+      <c r="G43" s="34">
         <f t="shared" si="14"/>
         <v>859506.31199999992</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="34">
         <v>0</v>
       </c>
-      <c r="I43" s="40">
+      <c r="I43" s="34">
         <f t="shared" si="15"/>
         <v>1245503.112</v>
       </c>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>202</v>
       </c>
-      <c r="B44" s="41">
+      <c r="B44" s="37">
         <v>14</v>
       </c>
-      <c r="C44" s="41">
+      <c r="C44" s="37">
         <v>8997</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44" s="40">
+      <c r="E44" s="34">
         <f>ABS($E$21)*24*B44</f>
         <v>15072813.167999998</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="34">
         <v>0</v>
       </c>
-      <c r="G44" s="40">
+      <c r="G44" s="34">
         <f t="shared" si="14"/>
         <v>12033088.367999999</v>
       </c>
-      <c r="H44" s="40">
+      <c r="H44" s="34">
         <v>0</v>
       </c>
-      <c r="I44" s="40">
+      <c r="I44" s="34">
         <f t="shared" si="15"/>
         <v>17437043.568</v>
       </c>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="39" t="s">
+      <c r="A46" t="s">
         <v>205</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
-      <c r="C46" s="41">
+      <c r="C46" s="37">
         <v>1</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="E46" s="41">
+      <c r="E46" s="37">
         <v>3</v>
       </c>
       <c r="F46">
         <v>4</v>
       </c>
-      <c r="G46" s="41">
+      <c r="G46" s="37">
         <v>5</v>
       </c>
       <c r="H46">
         <v>6</v>
       </c>
-      <c r="I46" s="41">
+      <c r="I46" s="37">
         <v>7</v>
       </c>
       <c r="J46">
         <v>8</v>
       </c>
-      <c r="K46" s="41">
+      <c r="K46" s="37">
         <v>9</v>
       </c>
     </row>
@@ -3413,43 +3385,43 @@
         <f>A40</f>
         <v>Braidwood</v>
       </c>
-      <c r="B47" s="40">
+      <c r="B47" s="34">
         <f>$D40+B$46*ABS($E40-$D40)/9</f>
         <v>0</v>
       </c>
-      <c r="C47" s="40">
+      <c r="C47" s="34">
         <f t="shared" ref="C47:K47" si="16">$D40+C$46*ABS($E40-$D40)/9</f>
         <v>239251.00266666664</v>
       </c>
-      <c r="D47" s="40">
+      <c r="D47" s="34">
         <f t="shared" si="16"/>
         <v>478502.00533333328</v>
       </c>
-      <c r="E47" s="40">
+      <c r="E47" s="34">
         <f t="shared" si="16"/>
         <v>717753.00799999991</v>
       </c>
-      <c r="F47" s="40">
+      <c r="F47" s="34">
         <f t="shared" si="16"/>
         <v>957004.01066666655</v>
       </c>
-      <c r="G47" s="40">
+      <c r="G47" s="34">
         <f t="shared" si="16"/>
         <v>1196255.0133333332</v>
       </c>
-      <c r="H47" s="40">
+      <c r="H47" s="34">
         <f t="shared" si="16"/>
         <v>1435506.0159999998</v>
       </c>
-      <c r="I47" s="40">
+      <c r="I47" s="34">
         <f t="shared" si="16"/>
         <v>1674757.0186666665</v>
       </c>
-      <c r="J47" s="40">
+      <c r="J47" s="34">
         <f t="shared" si="16"/>
         <v>1914008.0213333331</v>
       </c>
-      <c r="K47" s="40">
+      <c r="K47" s="34">
         <f t="shared" si="16"/>
         <v>2153259.0239999997</v>
       </c>
@@ -3459,43 +3431,43 @@
         <f t="shared" ref="A48:A51" si="17">A41</f>
         <v>Cooper</v>
       </c>
-      <c r="B48" s="40">
+      <c r="B48" s="34">
         <f t="shared" ref="B48:K51" si="18">$D41+B$46*ABS($E41-$D41)/9</f>
         <v>0</v>
       </c>
-      <c r="C48" s="40">
+      <c r="C48" s="34">
         <f t="shared" si="18"/>
         <v>837378.50933333323</v>
       </c>
-      <c r="D48" s="40">
+      <c r="D48" s="34">
         <f t="shared" si="18"/>
         <v>1674757.0186666665</v>
       </c>
-      <c r="E48" s="40">
+      <c r="E48" s="34">
         <f t="shared" si="18"/>
         <v>2512135.5279999995</v>
       </c>
-      <c r="F48" s="40">
+      <c r="F48" s="34">
         <f t="shared" si="18"/>
         <v>3349514.0373333329</v>
       </c>
-      <c r="G48" s="40">
+      <c r="G48" s="34">
         <f t="shared" si="18"/>
         <v>4186892.5466666659</v>
       </c>
-      <c r="H48" s="40">
+      <c r="H48" s="34">
         <f t="shared" si="18"/>
         <v>5024271.0559999989</v>
       </c>
-      <c r="I48" s="40">
+      <c r="I48" s="34">
         <f t="shared" si="18"/>
         <v>5861649.5653333329</v>
       </c>
-      <c r="J48" s="40">
+      <c r="J48" s="34">
         <f t="shared" si="18"/>
         <v>6699028.0746666659</v>
       </c>
-      <c r="K48" s="40">
+      <c r="K48" s="34">
         <f t="shared" si="18"/>
         <v>7536406.5839999979</v>
       </c>
@@ -3505,43 +3477,43 @@
         <f t="shared" si="17"/>
         <v>Davis-Besse</v>
       </c>
-      <c r="B49" s="40">
+      <c r="B49" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="C49" s="40">
+      <c r="C49" s="34">
         <f t="shared" si="18"/>
         <v>239251.00266666664</v>
       </c>
-      <c r="D49" s="40">
+      <c r="D49" s="34">
         <f t="shared" si="18"/>
         <v>478502.00533333328</v>
       </c>
-      <c r="E49" s="40">
+      <c r="E49" s="34">
         <f t="shared" si="18"/>
         <v>717753.00799999991</v>
       </c>
-      <c r="F49" s="40">
+      <c r="F49" s="34">
         <f t="shared" si="18"/>
         <v>957004.01066666655</v>
       </c>
-      <c r="G49" s="40">
+      <c r="G49" s="34">
         <f t="shared" si="18"/>
         <v>1196255.0133333332</v>
       </c>
-      <c r="H49" s="40">
+      <c r="H49" s="34">
         <f t="shared" si="18"/>
         <v>1435506.0159999998</v>
       </c>
-      <c r="I49" s="40">
+      <c r="I49" s="34">
         <f t="shared" si="18"/>
         <v>1674757.0186666665</v>
       </c>
-      <c r="J49" s="40">
+      <c r="J49" s="34">
         <f t="shared" si="18"/>
         <v>1914008.0213333331</v>
       </c>
-      <c r="K49" s="40">
+      <c r="K49" s="34">
         <f t="shared" si="18"/>
         <v>2153259.0239999997</v>
       </c>
@@ -3551,43 +3523,43 @@
         <f t="shared" si="17"/>
         <v>Prairie-Island</v>
       </c>
-      <c r="B50" s="40">
+      <c r="B50" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="34">
         <f t="shared" si="18"/>
         <v>119625.50133333332</v>
       </c>
-      <c r="D50" s="40">
+      <c r="D50" s="34">
         <f t="shared" si="18"/>
         <v>239251.00266666664</v>
       </c>
-      <c r="E50" s="40">
+      <c r="E50" s="34">
         <f t="shared" si="18"/>
         <v>358876.50399999996</v>
       </c>
-      <c r="F50" s="40">
+      <c r="F50" s="34">
         <f t="shared" si="18"/>
         <v>478502.00533333328</v>
       </c>
-      <c r="G50" s="40">
+      <c r="G50" s="34">
         <f t="shared" si="18"/>
         <v>598127.5066666666</v>
       </c>
-      <c r="H50" s="40">
+      <c r="H50" s="34">
         <f t="shared" si="18"/>
         <v>717753.00799999991</v>
       </c>
-      <c r="I50" s="40">
+      <c r="I50" s="34">
         <f t="shared" si="18"/>
         <v>837378.50933333323</v>
       </c>
-      <c r="J50" s="40">
+      <c r="J50" s="34">
         <f t="shared" si="18"/>
         <v>957004.01066666655</v>
       </c>
-      <c r="K50" s="40">
+      <c r="K50" s="34">
         <f t="shared" si="18"/>
         <v>1076629.5119999999</v>
       </c>
@@ -3597,79 +3569,79 @@
         <f t="shared" si="17"/>
         <v>South Texas Project</v>
       </c>
-      <c r="B51" s="40">
+      <c r="B51" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="C51" s="40">
+      <c r="C51" s="34">
         <f>$D44+C$46*ABS($E44-$D44)/9</f>
         <v>1674757.0186666665</v>
       </c>
-      <c r="D51" s="40">
+      <c r="D51" s="34">
         <f t="shared" si="18"/>
         <v>3349514.0373333329</v>
       </c>
-      <c r="E51" s="40">
+      <c r="E51" s="34">
         <f t="shared" si="18"/>
         <v>5024271.0559999989</v>
       </c>
-      <c r="F51" s="40">
+      <c r="F51" s="34">
         <f t="shared" si="18"/>
         <v>6699028.0746666659</v>
       </c>
-      <c r="G51" s="40">
+      <c r="G51" s="34">
         <f t="shared" si="18"/>
         <v>8373785.0933333319</v>
       </c>
-      <c r="H51" s="40">
+      <c r="H51" s="34">
         <f t="shared" si="18"/>
         <v>10048542.111999998</v>
       </c>
-      <c r="I51" s="40">
+      <c r="I51" s="34">
         <f t="shared" si="18"/>
         <v>11723299.130666666</v>
       </c>
-      <c r="J51" s="40">
+      <c r="J51" s="34">
         <f t="shared" si="18"/>
         <v>13398056.149333332</v>
       </c>
-      <c r="K51" s="40">
+      <c r="K51" s="34">
         <f t="shared" si="18"/>
         <v>15072813.167999996</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="39" t="s">
-        <v>209</v>
+      <c r="A53" t="s">
+        <v>211</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
-      <c r="C53" s="41">
+      <c r="C53" s="37">
         <v>1</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
-      <c r="E53" s="41">
+      <c r="E53" s="37">
         <v>3</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
-      <c r="G53" s="41">
+      <c r="G53" s="37">
         <v>5</v>
       </c>
       <c r="H53">
         <v>6</v>
       </c>
-      <c r="I53" s="41">
+      <c r="I53" s="37">
         <v>7</v>
       </c>
       <c r="J53">
         <v>8</v>
       </c>
-      <c r="K53" s="41">
+      <c r="K53" s="37">
         <v>9</v>
       </c>
     </row>
@@ -3678,43 +3650,43 @@
         <f>A47</f>
         <v>Braidwood</v>
       </c>
-      <c r="B54" s="40">
+      <c r="B54" s="34">
         <f>$F40+B$46*ABS($G40-$F40)/9</f>
         <v>0</v>
       </c>
-      <c r="C54" s="40">
+      <c r="C54" s="34">
         <f t="shared" ref="C54:K54" si="19">$F40+C$46*ABS($G40-$F40)/9</f>
         <v>191001.40266666666</v>
       </c>
-      <c r="D54" s="40">
+      <c r="D54" s="34">
         <f t="shared" si="19"/>
         <v>382002.80533333332</v>
       </c>
-      <c r="E54" s="40">
+      <c r="E54" s="34">
         <f t="shared" si="19"/>
         <v>573004.20799999998</v>
       </c>
-      <c r="F54" s="40">
+      <c r="F54" s="34">
         <f t="shared" si="19"/>
         <v>764005.61066666665</v>
       </c>
-      <c r="G54" s="40">
+      <c r="G54" s="34">
         <f t="shared" si="19"/>
         <v>955007.01333333319</v>
       </c>
-      <c r="H54" s="40">
+      <c r="H54" s="34">
         <f t="shared" si="19"/>
         <v>1146008.416</v>
       </c>
-      <c r="I54" s="40">
+      <c r="I54" s="34">
         <f t="shared" si="19"/>
         <v>1337009.8186666665</v>
       </c>
-      <c r="J54" s="40">
+      <c r="J54" s="34">
         <f t="shared" si="19"/>
         <v>1528011.2213333333</v>
       </c>
-      <c r="K54" s="40">
+      <c r="K54" s="34">
         <f t="shared" si="19"/>
         <v>1719012.6239999998</v>
       </c>
@@ -3724,43 +3696,43 @@
         <f t="shared" ref="A55:A58" si="20">A48</f>
         <v>Cooper</v>
       </c>
-      <c r="B55" s="40">
+      <c r="B55" s="34">
         <f t="shared" ref="B55:K58" si="21">$F41+B$46*ABS($G41-$F41)/9</f>
         <v>0</v>
       </c>
-      <c r="C55" s="40">
+      <c r="C55" s="34">
         <f t="shared" si="21"/>
         <v>668504.90933333326</v>
       </c>
-      <c r="D55" s="40">
+      <c r="D55" s="34">
         <f t="shared" si="21"/>
         <v>1337009.8186666665</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="34">
         <f t="shared" si="21"/>
         <v>2005514.7279999997</v>
       </c>
-      <c r="F55" s="40">
+      <c r="F55" s="34">
         <f t="shared" si="21"/>
         <v>2674019.637333333</v>
       </c>
-      <c r="G55" s="40">
+      <c r="G55" s="34">
         <f t="shared" si="21"/>
         <v>3342524.5466666664</v>
       </c>
-      <c r="H55" s="40">
+      <c r="H55" s="34">
         <f t="shared" si="21"/>
         <v>4011029.4559999993</v>
       </c>
-      <c r="I55" s="40">
+      <c r="I55" s="34">
         <f t="shared" si="21"/>
         <v>4679534.3653333327</v>
       </c>
-      <c r="J55" s="40">
+      <c r="J55" s="34">
         <f t="shared" si="21"/>
         <v>5348039.2746666661</v>
       </c>
-      <c r="K55" s="40">
+      <c r="K55" s="34">
         <f t="shared" si="21"/>
         <v>6016544.1839999994</v>
       </c>
@@ -3770,43 +3742,43 @@
         <f t="shared" si="20"/>
         <v>Davis-Besse</v>
       </c>
-      <c r="B56" s="40">
+      <c r="B56" s="34">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="C56" s="40">
+      <c r="C56" s="34">
         <f t="shared" si="21"/>
         <v>191001.40266666666</v>
       </c>
-      <c r="D56" s="40">
+      <c r="D56" s="34">
         <f t="shared" si="21"/>
         <v>382002.80533333332</v>
       </c>
-      <c r="E56" s="40">
+      <c r="E56" s="34">
         <f t="shared" si="21"/>
         <v>573004.20799999998</v>
       </c>
-      <c r="F56" s="40">
+      <c r="F56" s="34">
         <f t="shared" si="21"/>
         <v>764005.61066666665</v>
       </c>
-      <c r="G56" s="40">
+      <c r="G56" s="34">
         <f t="shared" si="21"/>
         <v>955007.01333333319</v>
       </c>
-      <c r="H56" s="40">
+      <c r="H56" s="34">
         <f t="shared" si="21"/>
         <v>1146008.416</v>
       </c>
-      <c r="I56" s="40">
+      <c r="I56" s="34">
         <f t="shared" si="21"/>
         <v>1337009.8186666665</v>
       </c>
-      <c r="J56" s="40">
+      <c r="J56" s="34">
         <f t="shared" si="21"/>
         <v>1528011.2213333333</v>
       </c>
-      <c r="K56" s="40">
+      <c r="K56" s="34">
         <f t="shared" si="21"/>
         <v>1719012.6239999998</v>
       </c>
@@ -3816,43 +3788,43 @@
         <f t="shared" si="20"/>
         <v>Prairie-Island</v>
       </c>
-      <c r="B57" s="40">
+      <c r="B57" s="34">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="C57" s="40">
+      <c r="C57" s="34">
         <f t="shared" si="21"/>
         <v>95500.701333333331</v>
       </c>
-      <c r="D57" s="40">
+      <c r="D57" s="34">
         <f t="shared" si="21"/>
         <v>191001.40266666666</v>
       </c>
-      <c r="E57" s="40">
+      <c r="E57" s="34">
         <f t="shared" si="21"/>
         <v>286502.10399999999</v>
       </c>
-      <c r="F57" s="40">
+      <c r="F57" s="34">
         <f t="shared" si="21"/>
         <v>382002.80533333332</v>
       </c>
-      <c r="G57" s="40">
+      <c r="G57" s="34">
         <f t="shared" si="21"/>
         <v>477503.5066666666</v>
       </c>
-      <c r="H57" s="40">
+      <c r="H57" s="34">
         <f t="shared" si="21"/>
         <v>573004.20799999998</v>
       </c>
-      <c r="I57" s="40">
+      <c r="I57" s="34">
         <f t="shared" si="21"/>
         <v>668504.90933333326</v>
       </c>
-      <c r="J57" s="40">
+      <c r="J57" s="34">
         <f t="shared" si="21"/>
         <v>764005.61066666665</v>
       </c>
-      <c r="K57" s="40">
+      <c r="K57" s="34">
         <f t="shared" si="21"/>
         <v>859506.31199999992</v>
       </c>
@@ -3862,79 +3834,79 @@
         <f t="shared" si="20"/>
         <v>South Texas Project</v>
       </c>
-      <c r="B58" s="40">
+      <c r="B58" s="34">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="C58" s="40">
+      <c r="C58" s="34">
         <f t="shared" si="21"/>
         <v>1337009.8186666665</v>
       </c>
-      <c r="D58" s="40">
+      <c r="D58" s="34">
         <f t="shared" si="21"/>
         <v>2674019.637333333</v>
       </c>
-      <c r="E58" s="40">
+      <c r="E58" s="34">
         <f t="shared" si="21"/>
         <v>4011029.4559999993</v>
       </c>
-      <c r="F58" s="40">
+      <c r="F58" s="34">
         <f t="shared" si="21"/>
         <v>5348039.2746666661</v>
       </c>
-      <c r="G58" s="40">
+      <c r="G58" s="34">
         <f t="shared" si="21"/>
         <v>6685049.0933333328</v>
       </c>
-      <c r="H58" s="40">
+      <c r="H58" s="34">
         <f t="shared" si="21"/>
         <v>8022058.9119999986</v>
       </c>
-      <c r="I58" s="40">
+      <c r="I58" s="34">
         <f t="shared" si="21"/>
         <v>9359068.7306666654</v>
       </c>
-      <c r="J58" s="40">
+      <c r="J58" s="34">
         <f t="shared" si="21"/>
         <v>10696078.549333332</v>
       </c>
-      <c r="K58" s="40">
+      <c r="K58" s="34">
         <f t="shared" si="21"/>
         <v>12033088.367999999</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="39" t="s">
-        <v>210</v>
+      <c r="A60" t="s">
+        <v>212</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
-      <c r="C60" s="41">
+      <c r="C60" s="37">
         <v>1</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
-      <c r="E60" s="41">
+      <c r="E60" s="37">
         <v>3</v>
       </c>
       <c r="F60">
         <v>4</v>
       </c>
-      <c r="G60" s="41">
+      <c r="G60" s="37">
         <v>5</v>
       </c>
       <c r="H60">
         <v>6</v>
       </c>
-      <c r="I60" s="41">
+      <c r="I60" s="37">
         <v>7</v>
       </c>
       <c r="J60">
         <v>8</v>
       </c>
-      <c r="K60" s="41">
+      <c r="K60" s="37">
         <v>9</v>
       </c>
     </row>
@@ -3943,43 +3915,43 @@
         <f>A54</f>
         <v>Braidwood</v>
       </c>
-      <c r="B61" s="40">
+      <c r="B61" s="34">
         <f>$H40+B$46*ABS($I40-$H40)/9</f>
         <v>0</v>
       </c>
-      <c r="C61" s="40">
+      <c r="C61" s="34">
         <f t="shared" ref="C61:K61" si="22">$H40+C$46*ABS($I40-$H40)/9</f>
         <v>276778.46933333331</v>
       </c>
-      <c r="D61" s="40">
+      <c r="D61" s="34">
         <f t="shared" si="22"/>
         <v>553556.93866666663</v>
       </c>
-      <c r="E61" s="40">
+      <c r="E61" s="34">
         <f t="shared" si="22"/>
         <v>830335.40800000005</v>
       </c>
-      <c r="F61" s="40">
+      <c r="F61" s="34">
         <f t="shared" si="22"/>
         <v>1107113.8773333333</v>
       </c>
-      <c r="G61" s="40">
+      <c r="G61" s="34">
         <f t="shared" si="22"/>
         <v>1383892.3466666667</v>
       </c>
-      <c r="H61" s="40">
+      <c r="H61" s="34">
         <f t="shared" si="22"/>
         <v>1660670.8160000001</v>
       </c>
-      <c r="I61" s="40">
+      <c r="I61" s="34">
         <f t="shared" si="22"/>
         <v>1937449.2853333333</v>
       </c>
-      <c r="J61" s="40">
+      <c r="J61" s="34">
         <f t="shared" si="22"/>
         <v>2214227.7546666665</v>
       </c>
-      <c r="K61" s="40">
+      <c r="K61" s="34">
         <f t="shared" si="22"/>
         <v>2491006.2239999999</v>
       </c>
@@ -3989,43 +3961,43 @@
         <f t="shared" ref="A62:A65" si="23">A55</f>
         <v>Cooper</v>
       </c>
-      <c r="B62" s="40">
+      <c r="B62" s="34">
         <f t="shared" ref="B62:K65" si="24">$H41+B$46*ABS($I41-$H41)/9</f>
         <v>0</v>
       </c>
-      <c r="C62" s="40">
+      <c r="C62" s="34">
         <f t="shared" si="24"/>
         <v>968724.64266666665</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="34">
         <f t="shared" si="24"/>
         <v>1937449.2853333333</v>
       </c>
-      <c r="E62" s="40">
+      <c r="E62" s="34">
         <f t="shared" si="24"/>
         <v>2906173.9279999998</v>
       </c>
-      <c r="F62" s="40">
+      <c r="F62" s="34">
         <f t="shared" si="24"/>
         <v>3874898.5706666666</v>
       </c>
-      <c r="G62" s="40">
+      <c r="G62" s="34">
         <f t="shared" si="24"/>
         <v>4843623.2133333338</v>
       </c>
-      <c r="H62" s="40">
+      <c r="H62" s="34">
         <f t="shared" si="24"/>
         <v>5812347.8559999997</v>
       </c>
-      <c r="I62" s="40">
+      <c r="I62" s="34">
         <f t="shared" si="24"/>
         <v>6781072.4986666664</v>
       </c>
-      <c r="J62" s="40">
+      <c r="J62" s="34">
         <f t="shared" si="24"/>
         <v>7749797.1413333332</v>
       </c>
-      <c r="K62" s="40">
+      <c r="K62" s="34">
         <f t="shared" si="24"/>
         <v>8718521.784</v>
       </c>
@@ -4035,43 +4007,43 @@
         <f t="shared" si="23"/>
         <v>Davis-Besse</v>
       </c>
-      <c r="B63" s="40">
+      <c r="B63" s="34">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="C63" s="40">
+      <c r="C63" s="34">
         <f t="shared" si="24"/>
         <v>276778.46933333331</v>
       </c>
-      <c r="D63" s="40">
+      <c r="D63" s="34">
         <f t="shared" si="24"/>
         <v>553556.93866666663</v>
       </c>
-      <c r="E63" s="40">
+      <c r="E63" s="34">
         <f t="shared" si="24"/>
         <v>830335.40800000005</v>
       </c>
-      <c r="F63" s="40">
+      <c r="F63" s="34">
         <f t="shared" si="24"/>
         <v>1107113.8773333333</v>
       </c>
-      <c r="G63" s="40">
+      <c r="G63" s="34">
         <f t="shared" si="24"/>
         <v>1383892.3466666667</v>
       </c>
-      <c r="H63" s="40">
+      <c r="H63" s="34">
         <f t="shared" si="24"/>
         <v>1660670.8160000001</v>
       </c>
-      <c r="I63" s="40">
+      <c r="I63" s="34">
         <f t="shared" si="24"/>
         <v>1937449.2853333333</v>
       </c>
-      <c r="J63" s="40">
+      <c r="J63" s="34">
         <f t="shared" si="24"/>
         <v>2214227.7546666665</v>
       </c>
-      <c r="K63" s="40">
+      <c r="K63" s="34">
         <f t="shared" si="24"/>
         <v>2491006.2239999999</v>
       </c>
@@ -4081,43 +4053,43 @@
         <f t="shared" si="23"/>
         <v>Prairie-Island</v>
       </c>
-      <c r="B64" s="40">
+      <c r="B64" s="34">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="C64" s="40">
+      <c r="C64" s="34">
         <f t="shared" si="24"/>
         <v>138389.23466666666</v>
       </c>
-      <c r="D64" s="40">
+      <c r="D64" s="34">
         <f t="shared" si="24"/>
         <v>276778.46933333331</v>
       </c>
-      <c r="E64" s="40">
+      <c r="E64" s="34">
         <f t="shared" si="24"/>
         <v>415167.70400000003</v>
       </c>
-      <c r="F64" s="40">
+      <c r="F64" s="34">
         <f t="shared" si="24"/>
         <v>553556.93866666663</v>
       </c>
-      <c r="G64" s="40">
+      <c r="G64" s="34">
         <f t="shared" si="24"/>
         <v>691946.17333333334</v>
       </c>
-      <c r="H64" s="40">
+      <c r="H64" s="34">
         <f t="shared" si="24"/>
         <v>830335.40800000005</v>
       </c>
-      <c r="I64" s="40">
+      <c r="I64" s="34">
         <f t="shared" si="24"/>
         <v>968724.64266666665</v>
       </c>
-      <c r="J64" s="40">
+      <c r="J64" s="34">
         <f t="shared" si="24"/>
         <v>1107113.8773333333</v>
       </c>
-      <c r="K64" s="40">
+      <c r="K64" s="34">
         <f t="shared" si="24"/>
         <v>1245503.112</v>
       </c>
@@ -4127,43 +4099,43 @@
         <f t="shared" si="23"/>
         <v>South Texas Project</v>
       </c>
-      <c r="B65" s="40">
+      <c r="B65" s="34">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="C65" s="40">
+      <c r="C65" s="34">
         <f t="shared" si="24"/>
         <v>1937449.2853333333</v>
       </c>
-      <c r="D65" s="40">
+      <c r="D65" s="34">
         <f t="shared" si="24"/>
         <v>3874898.5706666666</v>
       </c>
-      <c r="E65" s="40">
+      <c r="E65" s="34">
         <f t="shared" si="24"/>
         <v>5812347.8559999997</v>
       </c>
-      <c r="F65" s="40">
+      <c r="F65" s="34">
         <f t="shared" si="24"/>
         <v>7749797.1413333332</v>
       </c>
-      <c r="G65" s="40">
+      <c r="G65" s="34">
         <f t="shared" si="24"/>
         <v>9687246.4266666677</v>
       </c>
-      <c r="H65" s="40">
+      <c r="H65" s="34">
         <f t="shared" si="24"/>
         <v>11624695.711999999</v>
       </c>
-      <c r="I65" s="40">
+      <c r="I65" s="34">
         <f t="shared" si="24"/>
         <v>13562144.997333333</v>
       </c>
-      <c r="J65" s="40">
+      <c r="J65" s="34">
         <f t="shared" si="24"/>
         <v>15499594.282666666</v>
       </c>
-      <c r="K65" s="40">
+      <c r="K65" s="34">
         <f t="shared" si="24"/>
         <v>17437043.568</v>
       </c>
@@ -4181,6 +4153,128 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7BA3C-274B-4147-8CC3-A303BF1014EB}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>40</v>
+      </c>
+      <c r="K3">
+        <v>80</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="38">
+        <v>1802460</v>
+      </c>
+      <c r="C4" s="38">
+        <v>5569000</v>
+      </c>
+      <c r="D4" s="38">
+        <v>24646000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4">
+        <f>H3*$H$2</f>
+        <v>720</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:L4" si="0">I3*$H$2</f>
+        <v>240</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="38">
+        <v>3.71</v>
+      </c>
+      <c r="C5" s="38">
+        <v>23.2</v>
+      </c>
+      <c r="D5" s="38">
+        <v>55.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17762179-2135-43B7-98DA-D4A6A7868310}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -4206,10 +4300,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="40"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -4337,7 +4431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -4377,26 +4471,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4468,15 +4562,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4554,22 +4648,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4583,11 +4677,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -4628,7 +4722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4803,7 +4897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D919D22-7A01-ED42-B8B2-84358A3D7717}">
   <dimension ref="A1:P25"/>
   <sheetViews>
@@ -5310,7 +5404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -5442,7 +5536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
   <dimension ref="A1:E10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix mistake in htse, ft, h2 sto cap calculations
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41FB75-9BC8-8843-BCF2-ADBD1CAB561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC12F5-D4F6-1549-84CD-EAF3D73E4F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-460" yWindow="600" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="37140" yWindow="1460" windowWidth="35980" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
-    <sheet name="Boundaries" sheetId="10" r:id="rId1"/>
-    <sheet name="SMR" sheetId="13" r:id="rId2"/>
+    <sheet name="SMR" sheetId="13" r:id="rId1"/>
+    <sheet name="Boundaries" sheetId="10" r:id="rId2"/>
     <sheet name="MACRS" sheetId="1" r:id="rId3"/>
     <sheet name="Transfer_rates" sheetId="4" r:id="rId4"/>
     <sheet name="HTSE" sheetId="2" r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="215">
   <si>
     <t>Source</t>
   </si>
@@ -497,15 +497,6 @@
     <t>Federal corporate tax rate</t>
   </si>
   <si>
-    <t>HTSE Lower (MWe)</t>
-  </si>
-  <si>
-    <t>FT Lower (kg-H2)</t>
-  </si>
-  <si>
-    <t>H2 storage Upper (kg-h2)</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -584,15 +575,6 @@
     <t>Depreciation schedule</t>
   </si>
   <si>
-    <t>SMR Capacity (MWe)</t>
-  </si>
-  <si>
-    <t>Storage max capacity (FT prod)</t>
-  </si>
-  <si>
-    <t>48h</t>
-  </si>
-  <si>
     <t>Case name</t>
   </si>
   <si>
@@ -641,18 +623,6 @@
     <t>Max elec. Price</t>
   </si>
   <si>
-    <t>Braidwood</t>
-  </si>
-  <si>
-    <t>Cooper</t>
-  </si>
-  <si>
-    <t>Davis-Besse</t>
-  </si>
-  <si>
-    <t>South Texas Project</t>
-  </si>
-  <si>
     <t>HTSE Steps</t>
   </si>
   <si>
@@ -674,9 +644,6 @@
     <t>Location elec. Prices</t>
   </si>
   <si>
-    <t>Prairie-Island</t>
-  </si>
-  <si>
     <t>6 units</t>
   </si>
   <si>
@@ -708,6 +675,18 @@
   </si>
   <si>
     <t>Total capacity (MWe)</t>
+  </si>
+  <si>
+    <t>20MWe</t>
+  </si>
+  <si>
+    <t>40MWe</t>
+  </si>
+  <si>
+    <t>80MWe</t>
+  </si>
+  <si>
+    <t>100MWe</t>
   </si>
 </sst>
 </file>
@@ -777,7 +756,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,12 +766,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1019,8 +992,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1029,6 +1000,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2435,1729 +2408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:L65"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5">
-        <v>14.9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>60</v>
-      </c>
-      <c r="B12">
-        <f>-A12+14.9</f>
-        <v>-45.1</v>
-      </c>
-      <c r="C12" s="34">
-        <f>B12*25.13</f>
-        <v>-1133.3630000000001</v>
-      </c>
-      <c r="D12" s="34">
-        <f>ABS(C12)*48</f>
-        <v>54401.423999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>360</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ref="B13:B16" si="0">-A13+14.9</f>
-        <v>-345.1</v>
-      </c>
-      <c r="C13" s="34">
-        <f>B13*25.13</f>
-        <v>-8672.3629999999994</v>
-      </c>
-      <c r="D13" s="34">
-        <f t="shared" ref="D13:D16" si="1">ABS(C13)*48</f>
-        <v>416273.424</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>720</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>-705.1</v>
-      </c>
-      <c r="C14" s="34">
-        <f>B14*25.13</f>
-        <v>-17719.163</v>
-      </c>
-      <c r="D14" s="34">
-        <f t="shared" si="1"/>
-        <v>850519.82400000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1080</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>-1065.0999999999999</v>
-      </c>
-      <c r="C15" s="34">
-        <f>B15*25.13</f>
-        <v>-26765.962999999996</v>
-      </c>
-      <c r="D15" s="34">
-        <f t="shared" si="1"/>
-        <v>1284766.2239999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1440</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>-1425.1</v>
-      </c>
-      <c r="C16" s="34">
-        <f>B16*25.13</f>
-        <v>-35812.762999999999</v>
-      </c>
-      <c r="D16" s="34">
-        <f t="shared" si="1"/>
-        <v>1719012.6239999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" t="s">
-        <v>196</v>
-      </c>
-      <c r="E20" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21">
-        <v>720</v>
-      </c>
-      <c r="C21">
-        <f>MAX(-B21+$B$15, -1000+$B$15)</f>
-        <v>-1785.1</v>
-      </c>
-      <c r="D21">
-        <f>-100+$B$5</f>
-        <v>-85.1</v>
-      </c>
-      <c r="E21">
-        <f>C21*25.13</f>
-        <v>-44859.562999999995</v>
-      </c>
-      <c r="F21">
-        <f>D21*25.13</f>
-        <v>-2138.5629999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B22">
-        <v>360</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:C23" si="2">MAX(-B22+$B$15, -1000+$B$15)</f>
-        <v>-1425.1</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22:D23" si="3">-100+$B$5</f>
-        <v>-85.1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ref="E22:F22" si="4">C22*25.13</f>
-        <v>-35812.762999999999</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>-2138.5629999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23">
-        <f>18*60</f>
-        <v>1080</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>-2065.1</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
-        <v>-85.1</v>
-      </c>
-      <c r="E23">
-        <f>C23*25.13</f>
-        <v>-51895.962999999996</v>
-      </c>
-      <c r="F23">
-        <f>D23*25.13</f>
-        <v>-2138.5629999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B26" s="35">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="35">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
-      </c>
-      <c r="F26" s="35">
-        <v>4</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
-      </c>
-      <c r="H26" s="35">
-        <v>6</v>
-      </c>
-      <c r="I26">
-        <v>7</v>
-      </c>
-      <c r="J26" s="35">
-        <v>8</v>
-      </c>
-      <c r="K26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
-        <f>A21</f>
-        <v>Ref</v>
-      </c>
-      <c r="B27" s="36">
-        <f>$C21+B$26*ABS($C21-$D21)/9</f>
-        <v>-1785.1</v>
-      </c>
-      <c r="C27" s="34">
-        <f t="shared" ref="C27:K27" si="5">$C21+C$26*ABS($C21-$D21)/9</f>
-        <v>-1596.211111111111</v>
-      </c>
-      <c r="D27" s="36">
-        <f t="shared" si="5"/>
-        <v>-1407.3222222222221</v>
-      </c>
-      <c r="E27" s="34">
-        <f t="shared" si="5"/>
-        <v>-1218.4333333333334</v>
-      </c>
-      <c r="F27" s="36">
-        <f t="shared" si="5"/>
-        <v>-1029.5444444444443</v>
-      </c>
-      <c r="G27" s="34">
-        <f t="shared" si="5"/>
-        <v>-840.65555555555545</v>
-      </c>
-      <c r="H27" s="36">
-        <f t="shared" si="5"/>
-        <v>-651.76666666666665</v>
-      </c>
-      <c r="I27" s="34">
-        <f t="shared" si="5"/>
-        <v>-462.87777777777774</v>
-      </c>
-      <c r="J27" s="36">
-        <f t="shared" si="5"/>
-        <v>-273.98888888888882</v>
-      </c>
-      <c r="K27" s="34">
-        <f t="shared" si="5"/>
-        <v>-85.099999999999909</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
-        <f t="shared" ref="A28:A29" si="6">A22</f>
-        <v>6 units</v>
-      </c>
-      <c r="B28" s="36">
-        <f>$C22+B$26*ABS($C22-$D22)/9</f>
-        <v>-1425.1</v>
-      </c>
-      <c r="C28" s="34">
-        <f t="shared" ref="C28:K28" si="7">$C22+C$26*ABS($C22-$D22)/9</f>
-        <v>-1276.211111111111</v>
-      </c>
-      <c r="D28" s="36">
-        <f t="shared" si="7"/>
-        <v>-1127.3222222222221</v>
-      </c>
-      <c r="E28" s="34">
-        <f t="shared" si="7"/>
-        <v>-978.43333333333317</v>
-      </c>
-      <c r="F28" s="36">
-        <f t="shared" si="7"/>
-        <v>-829.54444444444437</v>
-      </c>
-      <c r="G28" s="34">
-        <f t="shared" si="7"/>
-        <v>-680.65555555555545</v>
-      </c>
-      <c r="H28" s="36">
-        <f t="shared" si="7"/>
-        <v>-531.76666666666654</v>
-      </c>
-      <c r="I28" s="34">
-        <f t="shared" si="7"/>
-        <v>-382.87777777777774</v>
-      </c>
-      <c r="J28" s="36">
-        <f t="shared" si="7"/>
-        <v>-233.98888888888882</v>
-      </c>
-      <c r="K28" s="34">
-        <f t="shared" si="7"/>
-        <v>-85.099999999999909</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="str">
-        <f t="shared" si="6"/>
-        <v>18 units</v>
-      </c>
-      <c r="B29" s="36">
-        <f>$C23+B$26*ABS($C23-$D23)/9</f>
-        <v>-2065.1</v>
-      </c>
-      <c r="C29" s="34">
-        <f t="shared" ref="C29:K29" si="8">$C23+C$26*ABS($C23-$D23)/9</f>
-        <v>-1845.1</v>
-      </c>
-      <c r="D29" s="36">
-        <f t="shared" si="8"/>
-        <v>-1625.1</v>
-      </c>
-      <c r="E29" s="34">
-        <f t="shared" si="8"/>
-        <v>-1405.1</v>
-      </c>
-      <c r="F29" s="36">
-        <f t="shared" si="8"/>
-        <v>-1185.0999999999999</v>
-      </c>
-      <c r="G29" s="34">
-        <f t="shared" si="8"/>
-        <v>-965.09999999999991</v>
-      </c>
-      <c r="H29" s="36">
-        <f t="shared" si="8"/>
-        <v>-745.09999999999991</v>
-      </c>
-      <c r="I29" s="34">
-        <f t="shared" si="8"/>
-        <v>-525.09999999999991</v>
-      </c>
-      <c r="J29" s="36">
-        <f t="shared" si="8"/>
-        <v>-305.09999999999991</v>
-      </c>
-      <c r="K29" s="34">
-        <f t="shared" si="8"/>
-        <v>-85.099999999999909</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B32" s="35">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="35">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32" s="35">
-        <v>4</v>
-      </c>
-      <c r="G32">
-        <v>5</v>
-      </c>
-      <c r="H32" s="35">
-        <v>6</v>
-      </c>
-      <c r="I32">
-        <v>7</v>
-      </c>
-      <c r="J32" s="35">
-        <v>8</v>
-      </c>
-      <c r="K32">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <f>A21</f>
-        <v>Ref</v>
-      </c>
-      <c r="B33" s="36">
-        <f>$E21+B$32*ABS($E21-$F21)/9</f>
-        <v>-44859.562999999995</v>
-      </c>
-      <c r="C33" s="34">
-        <f t="shared" ref="C33:K33" si="9">$E21+C$32*ABS($E21-$F21)/9</f>
-        <v>-40112.785222222214</v>
-      </c>
-      <c r="D33" s="36">
-        <f t="shared" si="9"/>
-        <v>-35366.00744444444</v>
-      </c>
-      <c r="E33" s="34">
-        <f t="shared" si="9"/>
-        <v>-30619.229666666666</v>
-      </c>
-      <c r="F33" s="36">
-        <f t="shared" si="9"/>
-        <v>-25872.451888888885</v>
-      </c>
-      <c r="G33" s="34">
-        <f t="shared" si="9"/>
-        <v>-21125.674111111108</v>
-      </c>
-      <c r="H33" s="36">
-        <f t="shared" si="9"/>
-        <v>-16378.896333333334</v>
-      </c>
-      <c r="I33" s="34">
-        <f t="shared" si="9"/>
-        <v>-11632.118555555557</v>
-      </c>
-      <c r="J33" s="36">
-        <f t="shared" si="9"/>
-        <v>-6885.3407777777757</v>
-      </c>
-      <c r="K33" s="34">
-        <f t="shared" si="9"/>
-        <v>-2138.5630000000019</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f t="shared" ref="A34:A35" si="10">A22</f>
-        <v>6 units</v>
-      </c>
-      <c r="B34" s="36">
-        <f>$E22+B$32*ABS($E22-$F22)/9</f>
-        <v>-35812.762999999999</v>
-      </c>
-      <c r="C34" s="34">
-        <f t="shared" ref="C34:K34" si="11">$E22+C$32*ABS($E22-$F22)/9</f>
-        <v>-32071.185222222222</v>
-      </c>
-      <c r="D34" s="36">
-        <f t="shared" si="11"/>
-        <v>-28329.607444444446</v>
-      </c>
-      <c r="E34" s="34">
-        <f t="shared" si="11"/>
-        <v>-24588.029666666669</v>
-      </c>
-      <c r="F34" s="36">
-        <f t="shared" si="11"/>
-        <v>-20846.451888888889</v>
-      </c>
-      <c r="G34" s="34">
-        <f t="shared" si="11"/>
-        <v>-17104.874111111109</v>
-      </c>
-      <c r="H34" s="36">
-        <f t="shared" si="11"/>
-        <v>-13363.296333333335</v>
-      </c>
-      <c r="I34" s="34">
-        <f t="shared" si="11"/>
-        <v>-9621.7185555555589</v>
-      </c>
-      <c r="J34" s="36">
-        <f t="shared" si="11"/>
-        <v>-5880.1407777777786</v>
-      </c>
-      <c r="K34" s="34">
-        <f t="shared" si="11"/>
-        <v>-2138.5630000000019</v>
-      </c>
-      <c r="L34" s="34"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <f t="shared" si="10"/>
-        <v>18 units</v>
-      </c>
-      <c r="B35" s="36">
-        <f>$E23+B$32*ABS($E23-$F23)/9</f>
-        <v>-51895.962999999996</v>
-      </c>
-      <c r="C35" s="34">
-        <f>$E23+C$32*ABS($E23-$F23)/9</f>
-        <v>-46367.362999999998</v>
-      </c>
-      <c r="D35" s="36">
-        <f t="shared" ref="D35:K35" si="12">$E23+D$32*ABS($E23-$F23)/9</f>
-        <v>-40838.762999999999</v>
-      </c>
-      <c r="E35" s="34">
-        <f t="shared" si="12"/>
-        <v>-35310.163</v>
-      </c>
-      <c r="F35" s="36">
-        <f t="shared" si="12"/>
-        <v>-29781.562999999998</v>
-      </c>
-      <c r="G35" s="34">
-        <f t="shared" si="12"/>
-        <v>-24252.963</v>
-      </c>
-      <c r="H35" s="36">
-        <f t="shared" si="12"/>
-        <v>-18724.362999999998</v>
-      </c>
-      <c r="I35" s="34">
-        <f t="shared" si="12"/>
-        <v>-13195.763000000006</v>
-      </c>
-      <c r="J35" s="36">
-        <f t="shared" si="12"/>
-        <v>-7667.1630000000005</v>
-      </c>
-      <c r="K35" s="34">
-        <f t="shared" si="12"/>
-        <v>-2138.5630000000019</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" t="str">
-        <f>A21</f>
-        <v>Ref</v>
-      </c>
-      <c r="F38" t="str">
-        <f>A22</f>
-        <v>6 units</v>
-      </c>
-      <c r="H38" t="str">
-        <f>A23</f>
-        <v>18 units</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>209</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="D39" t="s">
-        <v>195</v>
-      </c>
-      <c r="E39" t="s">
-        <v>196</v>
-      </c>
-      <c r="F39" t="s">
-        <v>195</v>
-      </c>
-      <c r="G39" t="s">
-        <v>196</v>
-      </c>
-      <c r="H39" t="s">
-        <v>195</v>
-      </c>
-      <c r="I39" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>199</v>
-      </c>
-      <c r="B40" s="37">
-        <f t="shared" ref="B40:B42" si="13">ROUNDUP(C40*$B$44/$C$44,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C40" s="37">
-        <v>934</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" s="34">
-        <f>ABS($E$21)*24*B40</f>
-        <v>2153259.0239999997</v>
-      </c>
-      <c r="F40" s="34">
-        <v>0</v>
-      </c>
-      <c r="G40" s="34">
-        <f>ABS($E$22)*24*$B40</f>
-        <v>1719012.6239999998</v>
-      </c>
-      <c r="H40" s="34">
-        <v>0</v>
-      </c>
-      <c r="I40" s="34">
-        <f>ABS($E$23)*24*$B40</f>
-        <v>2491006.2239999999</v>
-      </c>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>200</v>
-      </c>
-      <c r="B41" s="37">
-        <f t="shared" si="13"/>
-        <v>7</v>
-      </c>
-      <c r="C41" s="37">
-        <v>4231</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" s="34">
-        <f>ABS($E$21)*24*B41</f>
-        <v>7536406.5839999989</v>
-      </c>
-      <c r="F41" s="34">
-        <v>0</v>
-      </c>
-      <c r="G41" s="34">
-        <f t="shared" ref="G41:G44" si="14">ABS($E$22)*24*$B41</f>
-        <v>6016544.1839999994</v>
-      </c>
-      <c r="H41" s="34">
-        <v>0</v>
-      </c>
-      <c r="I41" s="34">
-        <f t="shared" ref="I41:I44" si="15">ABS($E$23)*24*$B41</f>
-        <v>8718521.784</v>
-      </c>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>201</v>
-      </c>
-      <c r="B42" s="37">
-        <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="C42" s="37">
-        <v>934</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" s="34">
-        <f>ABS($E$21)*24*B42</f>
-        <v>2153259.0239999997</v>
-      </c>
-      <c r="F42" s="34">
-        <v>0</v>
-      </c>
-      <c r="G42" s="34">
-        <f t="shared" si="14"/>
-        <v>1719012.6239999998</v>
-      </c>
-      <c r="H42" s="34">
-        <v>0</v>
-      </c>
-      <c r="I42" s="34">
-        <f t="shared" si="15"/>
-        <v>2491006.2239999999</v>
-      </c>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>210</v>
-      </c>
-      <c r="B43" s="37">
-        <f>ROUNDUP(C43*$B$44/$C$44,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C43" s="37">
-        <v>97</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" s="34">
-        <f>ABS($E$21)*24*B43</f>
-        <v>1076629.5119999999</v>
-      </c>
-      <c r="F43" s="34">
-        <v>0</v>
-      </c>
-      <c r="G43" s="34">
-        <f t="shared" si="14"/>
-        <v>859506.31199999992</v>
-      </c>
-      <c r="H43" s="34">
-        <v>0</v>
-      </c>
-      <c r="I43" s="34">
-        <f t="shared" si="15"/>
-        <v>1245503.112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>202</v>
-      </c>
-      <c r="B44" s="37">
-        <v>14</v>
-      </c>
-      <c r="C44" s="37">
-        <v>8997</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44" s="34">
-        <f>ABS($E$21)*24*B44</f>
-        <v>15072813.167999998</v>
-      </c>
-      <c r="F44" s="34">
-        <v>0</v>
-      </c>
-      <c r="G44" s="34">
-        <f t="shared" si="14"/>
-        <v>12033088.367999999</v>
-      </c>
-      <c r="H44" s="34">
-        <v>0</v>
-      </c>
-      <c r="I44" s="34">
-        <f t="shared" si="15"/>
-        <v>17437043.568</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>205</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" s="37">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="E46" s="37">
-        <v>3</v>
-      </c>
-      <c r="F46">
-        <v>4</v>
-      </c>
-      <c r="G46" s="37">
-        <v>5</v>
-      </c>
-      <c r="H46">
-        <v>6</v>
-      </c>
-      <c r="I46" s="37">
-        <v>7</v>
-      </c>
-      <c r="J46">
-        <v>8</v>
-      </c>
-      <c r="K46" s="37">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" t="str">
-        <f>A40</f>
-        <v>Braidwood</v>
-      </c>
-      <c r="B47" s="34">
-        <f>$D40+B$46*ABS($E40-$D40)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="34">
-        <f t="shared" ref="C47:K47" si="16">$D40+C$46*ABS($E40-$D40)/9</f>
-        <v>239251.00266666664</v>
-      </c>
-      <c r="D47" s="34">
-        <f t="shared" si="16"/>
-        <v>478502.00533333328</v>
-      </c>
-      <c r="E47" s="34">
-        <f t="shared" si="16"/>
-        <v>717753.00799999991</v>
-      </c>
-      <c r="F47" s="34">
-        <f t="shared" si="16"/>
-        <v>957004.01066666655</v>
-      </c>
-      <c r="G47" s="34">
-        <f t="shared" si="16"/>
-        <v>1196255.0133333332</v>
-      </c>
-      <c r="H47" s="34">
-        <f t="shared" si="16"/>
-        <v>1435506.0159999998</v>
-      </c>
-      <c r="I47" s="34">
-        <f t="shared" si="16"/>
-        <v>1674757.0186666665</v>
-      </c>
-      <c r="J47" s="34">
-        <f t="shared" si="16"/>
-        <v>1914008.0213333331</v>
-      </c>
-      <c r="K47" s="34">
-        <f t="shared" si="16"/>
-        <v>2153259.0239999997</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <f t="shared" ref="A48:A51" si="17">A41</f>
-        <v>Cooper</v>
-      </c>
-      <c r="B48" s="34">
-        <f t="shared" ref="B48:K51" si="18">$D41+B$46*ABS($E41-$D41)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="34">
-        <f t="shared" si="18"/>
-        <v>837378.50933333323</v>
-      </c>
-      <c r="D48" s="34">
-        <f t="shared" si="18"/>
-        <v>1674757.0186666665</v>
-      </c>
-      <c r="E48" s="34">
-        <f t="shared" si="18"/>
-        <v>2512135.5279999995</v>
-      </c>
-      <c r="F48" s="34">
-        <f t="shared" si="18"/>
-        <v>3349514.0373333329</v>
-      </c>
-      <c r="G48" s="34">
-        <f t="shared" si="18"/>
-        <v>4186892.5466666659</v>
-      </c>
-      <c r="H48" s="34">
-        <f t="shared" si="18"/>
-        <v>5024271.0559999989</v>
-      </c>
-      <c r="I48" s="34">
-        <f t="shared" si="18"/>
-        <v>5861649.5653333329</v>
-      </c>
-      <c r="J48" s="34">
-        <f t="shared" si="18"/>
-        <v>6699028.0746666659</v>
-      </c>
-      <c r="K48" s="34">
-        <f t="shared" si="18"/>
-        <v>7536406.5839999979</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f t="shared" si="17"/>
-        <v>Davis-Besse</v>
-      </c>
-      <c r="B49" s="34">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="C49" s="34">
-        <f t="shared" si="18"/>
-        <v>239251.00266666664</v>
-      </c>
-      <c r="D49" s="34">
-        <f t="shared" si="18"/>
-        <v>478502.00533333328</v>
-      </c>
-      <c r="E49" s="34">
-        <f t="shared" si="18"/>
-        <v>717753.00799999991</v>
-      </c>
-      <c r="F49" s="34">
-        <f t="shared" si="18"/>
-        <v>957004.01066666655</v>
-      </c>
-      <c r="G49" s="34">
-        <f t="shared" si="18"/>
-        <v>1196255.0133333332</v>
-      </c>
-      <c r="H49" s="34">
-        <f t="shared" si="18"/>
-        <v>1435506.0159999998</v>
-      </c>
-      <c r="I49" s="34">
-        <f t="shared" si="18"/>
-        <v>1674757.0186666665</v>
-      </c>
-      <c r="J49" s="34">
-        <f t="shared" si="18"/>
-        <v>1914008.0213333331</v>
-      </c>
-      <c r="K49" s="34">
-        <f t="shared" si="18"/>
-        <v>2153259.0239999997</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="17"/>
-        <v>Prairie-Island</v>
-      </c>
-      <c r="B50" s="34">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="C50" s="34">
-        <f t="shared" si="18"/>
-        <v>119625.50133333332</v>
-      </c>
-      <c r="D50" s="34">
-        <f t="shared" si="18"/>
-        <v>239251.00266666664</v>
-      </c>
-      <c r="E50" s="34">
-        <f t="shared" si="18"/>
-        <v>358876.50399999996</v>
-      </c>
-      <c r="F50" s="34">
-        <f t="shared" si="18"/>
-        <v>478502.00533333328</v>
-      </c>
-      <c r="G50" s="34">
-        <f t="shared" si="18"/>
-        <v>598127.5066666666</v>
-      </c>
-      <c r="H50" s="34">
-        <f t="shared" si="18"/>
-        <v>717753.00799999991</v>
-      </c>
-      <c r="I50" s="34">
-        <f t="shared" si="18"/>
-        <v>837378.50933333323</v>
-      </c>
-      <c r="J50" s="34">
-        <f t="shared" si="18"/>
-        <v>957004.01066666655</v>
-      </c>
-      <c r="K50" s="34">
-        <f t="shared" si="18"/>
-        <v>1076629.5119999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="str">
-        <f t="shared" si="17"/>
-        <v>South Texas Project</v>
-      </c>
-      <c r="B51" s="34">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="C51" s="34">
-        <f>$D44+C$46*ABS($E44-$D44)/9</f>
-        <v>1674757.0186666665</v>
-      </c>
-      <c r="D51" s="34">
-        <f t="shared" si="18"/>
-        <v>3349514.0373333329</v>
-      </c>
-      <c r="E51" s="34">
-        <f t="shared" si="18"/>
-        <v>5024271.0559999989</v>
-      </c>
-      <c r="F51" s="34">
-        <f t="shared" si="18"/>
-        <v>6699028.0746666659</v>
-      </c>
-      <c r="G51" s="34">
-        <f t="shared" si="18"/>
-        <v>8373785.0933333319</v>
-      </c>
-      <c r="H51" s="34">
-        <f t="shared" si="18"/>
-        <v>10048542.111999998</v>
-      </c>
-      <c r="I51" s="34">
-        <f t="shared" si="18"/>
-        <v>11723299.130666666</v>
-      </c>
-      <c r="J51" s="34">
-        <f t="shared" si="18"/>
-        <v>13398056.149333332</v>
-      </c>
-      <c r="K51" s="34">
-        <f t="shared" si="18"/>
-        <v>15072813.167999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>211</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53" s="37">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-      <c r="E53" s="37">
-        <v>3</v>
-      </c>
-      <c r="F53">
-        <v>4</v>
-      </c>
-      <c r="G53" s="37">
-        <v>5</v>
-      </c>
-      <c r="H53">
-        <v>6</v>
-      </c>
-      <c r="I53" s="37">
-        <v>7</v>
-      </c>
-      <c r="J53">
-        <v>8</v>
-      </c>
-      <c r="K53" s="37">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" t="str">
-        <f>A47</f>
-        <v>Braidwood</v>
-      </c>
-      <c r="B54" s="34">
-        <f>$F40+B$46*ABS($G40-$F40)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="34">
-        <f t="shared" ref="C54:K54" si="19">$F40+C$46*ABS($G40-$F40)/9</f>
-        <v>191001.40266666666</v>
-      </c>
-      <c r="D54" s="34">
-        <f t="shared" si="19"/>
-        <v>382002.80533333332</v>
-      </c>
-      <c r="E54" s="34">
-        <f t="shared" si="19"/>
-        <v>573004.20799999998</v>
-      </c>
-      <c r="F54" s="34">
-        <f t="shared" si="19"/>
-        <v>764005.61066666665</v>
-      </c>
-      <c r="G54" s="34">
-        <f t="shared" si="19"/>
-        <v>955007.01333333319</v>
-      </c>
-      <c r="H54" s="34">
-        <f t="shared" si="19"/>
-        <v>1146008.416</v>
-      </c>
-      <c r="I54" s="34">
-        <f t="shared" si="19"/>
-        <v>1337009.8186666665</v>
-      </c>
-      <c r="J54" s="34">
-        <f t="shared" si="19"/>
-        <v>1528011.2213333333</v>
-      </c>
-      <c r="K54" s="34">
-        <f t="shared" si="19"/>
-        <v>1719012.6239999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" t="str">
-        <f t="shared" ref="A55:A58" si="20">A48</f>
-        <v>Cooper</v>
-      </c>
-      <c r="B55" s="34">
-        <f t="shared" ref="B55:K58" si="21">$F41+B$46*ABS($G41-$F41)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C55" s="34">
-        <f t="shared" si="21"/>
-        <v>668504.90933333326</v>
-      </c>
-      <c r="D55" s="34">
-        <f t="shared" si="21"/>
-        <v>1337009.8186666665</v>
-      </c>
-      <c r="E55" s="34">
-        <f t="shared" si="21"/>
-        <v>2005514.7279999997</v>
-      </c>
-      <c r="F55" s="34">
-        <f t="shared" si="21"/>
-        <v>2674019.637333333</v>
-      </c>
-      <c r="G55" s="34">
-        <f t="shared" si="21"/>
-        <v>3342524.5466666664</v>
-      </c>
-      <c r="H55" s="34">
-        <f t="shared" si="21"/>
-        <v>4011029.4559999993</v>
-      </c>
-      <c r="I55" s="34">
-        <f t="shared" si="21"/>
-        <v>4679534.3653333327</v>
-      </c>
-      <c r="J55" s="34">
-        <f t="shared" si="21"/>
-        <v>5348039.2746666661</v>
-      </c>
-      <c r="K55" s="34">
-        <f t="shared" si="21"/>
-        <v>6016544.1839999994</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f t="shared" si="20"/>
-        <v>Davis-Besse</v>
-      </c>
-      <c r="B56" s="34">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="C56" s="34">
-        <f t="shared" si="21"/>
-        <v>191001.40266666666</v>
-      </c>
-      <c r="D56" s="34">
-        <f t="shared" si="21"/>
-        <v>382002.80533333332</v>
-      </c>
-      <c r="E56" s="34">
-        <f t="shared" si="21"/>
-        <v>573004.20799999998</v>
-      </c>
-      <c r="F56" s="34">
-        <f t="shared" si="21"/>
-        <v>764005.61066666665</v>
-      </c>
-      <c r="G56" s="34">
-        <f t="shared" si="21"/>
-        <v>955007.01333333319</v>
-      </c>
-      <c r="H56" s="34">
-        <f t="shared" si="21"/>
-        <v>1146008.416</v>
-      </c>
-      <c r="I56" s="34">
-        <f t="shared" si="21"/>
-        <v>1337009.8186666665</v>
-      </c>
-      <c r="J56" s="34">
-        <f t="shared" si="21"/>
-        <v>1528011.2213333333</v>
-      </c>
-      <c r="K56" s="34">
-        <f t="shared" si="21"/>
-        <v>1719012.6239999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" t="str">
-        <f t="shared" si="20"/>
-        <v>Prairie-Island</v>
-      </c>
-      <c r="B57" s="34">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="C57" s="34">
-        <f t="shared" si="21"/>
-        <v>95500.701333333331</v>
-      </c>
-      <c r="D57" s="34">
-        <f t="shared" si="21"/>
-        <v>191001.40266666666</v>
-      </c>
-      <c r="E57" s="34">
-        <f t="shared" si="21"/>
-        <v>286502.10399999999</v>
-      </c>
-      <c r="F57" s="34">
-        <f t="shared" si="21"/>
-        <v>382002.80533333332</v>
-      </c>
-      <c r="G57" s="34">
-        <f t="shared" si="21"/>
-        <v>477503.5066666666</v>
-      </c>
-      <c r="H57" s="34">
-        <f t="shared" si="21"/>
-        <v>573004.20799999998</v>
-      </c>
-      <c r="I57" s="34">
-        <f t="shared" si="21"/>
-        <v>668504.90933333326</v>
-      </c>
-      <c r="J57" s="34">
-        <f t="shared" si="21"/>
-        <v>764005.61066666665</v>
-      </c>
-      <c r="K57" s="34">
-        <f t="shared" si="21"/>
-        <v>859506.31199999992</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" t="str">
-        <f t="shared" si="20"/>
-        <v>South Texas Project</v>
-      </c>
-      <c r="B58" s="34">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="C58" s="34">
-        <f t="shared" si="21"/>
-        <v>1337009.8186666665</v>
-      </c>
-      <c r="D58" s="34">
-        <f t="shared" si="21"/>
-        <v>2674019.637333333</v>
-      </c>
-      <c r="E58" s="34">
-        <f t="shared" si="21"/>
-        <v>4011029.4559999993</v>
-      </c>
-      <c r="F58" s="34">
-        <f t="shared" si="21"/>
-        <v>5348039.2746666661</v>
-      </c>
-      <c r="G58" s="34">
-        <f t="shared" si="21"/>
-        <v>6685049.0933333328</v>
-      </c>
-      <c r="H58" s="34">
-        <f t="shared" si="21"/>
-        <v>8022058.9119999986</v>
-      </c>
-      <c r="I58" s="34">
-        <f t="shared" si="21"/>
-        <v>9359068.7306666654</v>
-      </c>
-      <c r="J58" s="34">
-        <f t="shared" si="21"/>
-        <v>10696078.549333332</v>
-      </c>
-      <c r="K58" s="34">
-        <f t="shared" si="21"/>
-        <v>12033088.367999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>212</v>
-      </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="C60" s="37">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60" s="37">
-        <v>3</v>
-      </c>
-      <c r="F60">
-        <v>4</v>
-      </c>
-      <c r="G60" s="37">
-        <v>5</v>
-      </c>
-      <c r="H60">
-        <v>6</v>
-      </c>
-      <c r="I60" s="37">
-        <v>7</v>
-      </c>
-      <c r="J60">
-        <v>8</v>
-      </c>
-      <c r="K60" s="37">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" t="str">
-        <f>A54</f>
-        <v>Braidwood</v>
-      </c>
-      <c r="B61" s="34">
-        <f>$H40+B$46*ABS($I40-$H40)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C61" s="34">
-        <f t="shared" ref="C61:K61" si="22">$H40+C$46*ABS($I40-$H40)/9</f>
-        <v>276778.46933333331</v>
-      </c>
-      <c r="D61" s="34">
-        <f t="shared" si="22"/>
-        <v>553556.93866666663</v>
-      </c>
-      <c r="E61" s="34">
-        <f t="shared" si="22"/>
-        <v>830335.40800000005</v>
-      </c>
-      <c r="F61" s="34">
-        <f t="shared" si="22"/>
-        <v>1107113.8773333333</v>
-      </c>
-      <c r="G61" s="34">
-        <f t="shared" si="22"/>
-        <v>1383892.3466666667</v>
-      </c>
-      <c r="H61" s="34">
-        <f t="shared" si="22"/>
-        <v>1660670.8160000001</v>
-      </c>
-      <c r="I61" s="34">
-        <f t="shared" si="22"/>
-        <v>1937449.2853333333</v>
-      </c>
-      <c r="J61" s="34">
-        <f t="shared" si="22"/>
-        <v>2214227.7546666665</v>
-      </c>
-      <c r="K61" s="34">
-        <f t="shared" si="22"/>
-        <v>2491006.2239999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
-        <f t="shared" ref="A62:A65" si="23">A55</f>
-        <v>Cooper</v>
-      </c>
-      <c r="B62" s="34">
-        <f t="shared" ref="B62:K65" si="24">$H41+B$46*ABS($I41-$H41)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C62" s="34">
-        <f t="shared" si="24"/>
-        <v>968724.64266666665</v>
-      </c>
-      <c r="D62" s="34">
-        <f t="shared" si="24"/>
-        <v>1937449.2853333333</v>
-      </c>
-      <c r="E62" s="34">
-        <f t="shared" si="24"/>
-        <v>2906173.9279999998</v>
-      </c>
-      <c r="F62" s="34">
-        <f t="shared" si="24"/>
-        <v>3874898.5706666666</v>
-      </c>
-      <c r="G62" s="34">
-        <f t="shared" si="24"/>
-        <v>4843623.2133333338</v>
-      </c>
-      <c r="H62" s="34">
-        <f t="shared" si="24"/>
-        <v>5812347.8559999997</v>
-      </c>
-      <c r="I62" s="34">
-        <f t="shared" si="24"/>
-        <v>6781072.4986666664</v>
-      </c>
-      <c r="J62" s="34">
-        <f t="shared" si="24"/>
-        <v>7749797.1413333332</v>
-      </c>
-      <c r="K62" s="34">
-        <f t="shared" si="24"/>
-        <v>8718521.784</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" t="str">
-        <f t="shared" si="23"/>
-        <v>Davis-Besse</v>
-      </c>
-      <c r="B63" s="34">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="C63" s="34">
-        <f t="shared" si="24"/>
-        <v>276778.46933333331</v>
-      </c>
-      <c r="D63" s="34">
-        <f t="shared" si="24"/>
-        <v>553556.93866666663</v>
-      </c>
-      <c r="E63" s="34">
-        <f t="shared" si="24"/>
-        <v>830335.40800000005</v>
-      </c>
-      <c r="F63" s="34">
-        <f t="shared" si="24"/>
-        <v>1107113.8773333333</v>
-      </c>
-      <c r="G63" s="34">
-        <f t="shared" si="24"/>
-        <v>1383892.3466666667</v>
-      </c>
-      <c r="H63" s="34">
-        <f t="shared" si="24"/>
-        <v>1660670.8160000001</v>
-      </c>
-      <c r="I63" s="34">
-        <f t="shared" si="24"/>
-        <v>1937449.2853333333</v>
-      </c>
-      <c r="J63" s="34">
-        <f t="shared" si="24"/>
-        <v>2214227.7546666665</v>
-      </c>
-      <c r="K63" s="34">
-        <f t="shared" si="24"/>
-        <v>2491006.2239999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" t="str">
-        <f t="shared" si="23"/>
-        <v>Prairie-Island</v>
-      </c>
-      <c r="B64" s="34">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="C64" s="34">
-        <f t="shared" si="24"/>
-        <v>138389.23466666666</v>
-      </c>
-      <c r="D64" s="34">
-        <f t="shared" si="24"/>
-        <v>276778.46933333331</v>
-      </c>
-      <c r="E64" s="34">
-        <f t="shared" si="24"/>
-        <v>415167.70400000003</v>
-      </c>
-      <c r="F64" s="34">
-        <f t="shared" si="24"/>
-        <v>553556.93866666663</v>
-      </c>
-      <c r="G64" s="34">
-        <f t="shared" si="24"/>
-        <v>691946.17333333334</v>
-      </c>
-      <c r="H64" s="34">
-        <f t="shared" si="24"/>
-        <v>830335.40800000005</v>
-      </c>
-      <c r="I64" s="34">
-        <f t="shared" si="24"/>
-        <v>968724.64266666665</v>
-      </c>
-      <c r="J64" s="34">
-        <f t="shared" si="24"/>
-        <v>1107113.8773333333</v>
-      </c>
-      <c r="K64" s="34">
-        <f t="shared" si="24"/>
-        <v>1245503.112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f t="shared" si="23"/>
-        <v>South Texas Project</v>
-      </c>
-      <c r="B65" s="34">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="C65" s="34">
-        <f t="shared" si="24"/>
-        <v>1937449.2853333333</v>
-      </c>
-      <c r="D65" s="34">
-        <f t="shared" si="24"/>
-        <v>3874898.5706666666</v>
-      </c>
-      <c r="E65" s="34">
-        <f t="shared" si="24"/>
-        <v>5812347.8559999997</v>
-      </c>
-      <c r="F65" s="34">
-        <f t="shared" si="24"/>
-        <v>7749797.1413333332</v>
-      </c>
-      <c r="G65" s="34">
-        <f t="shared" si="24"/>
-        <v>9687246.4266666677</v>
-      </c>
-      <c r="H65" s="34">
-        <f t="shared" si="24"/>
-        <v>11624695.711999999</v>
-      </c>
-      <c r="I65" s="34">
-        <f t="shared" si="24"/>
-        <v>13562144.997333333</v>
-      </c>
-      <c r="J65" s="34">
-        <f t="shared" si="24"/>
-        <v>15499594.282666666</v>
-      </c>
-      <c r="K65" s="34">
-        <f t="shared" si="24"/>
-        <v>17437043.568</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7BA3C-274B-4147-8CC3-A303BF1014EB}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4172,15 +2427,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G2" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="H2">
         <v>12</v>
@@ -4188,19 +2443,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="G3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -4220,19 +2475,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B4" s="38">
+        <v>204</v>
+      </c>
+      <c r="B4" s="36">
         <v>1802460</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <v>5569000</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="36">
         <v>24646000</v>
       </c>
       <c r="G4" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="H4">
         <f>H3*$H$2</f>
@@ -4257,19 +2512,1921 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="38">
+        <v>206</v>
+      </c>
+      <c r="B5" s="36">
         <v>3.71</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>23.2</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <v>55.69</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
+  <dimension ref="A1:L66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:K51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5">
+        <v>14.9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14">
+        <v>720</v>
+      </c>
+      <c r="C14">
+        <f>MAX(-B14+$B$5, -1000+$B$5)</f>
+        <v>-705.1</v>
+      </c>
+      <c r="D14">
+        <f>-100+$B$5</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E14">
+        <f>C14*25.13</f>
+        <v>-17719.163</v>
+      </c>
+      <c r="F14">
+        <f>D14*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15">
+        <v>240</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:C18" si="0">MAX(-B15+$B$5, -1000+$B$5)</f>
+        <v>-225.1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D18" si="1">-100+$B$5</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:F15" si="2">C15*25.13</f>
+        <v>-5656.7629999999999</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16">
+        <v>480</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-465.1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E16">
+        <f>C16*25.13</f>
+        <v>-11687.963</v>
+      </c>
+      <c r="F16">
+        <f>D16*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17">
+        <v>960</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-945.1</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E18" si="3">C17*25.13</f>
+        <v>-23750.363000000001</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F18" si="4">D17*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18">
+        <v>1200</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-985.1</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>-2138.5629999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="39">
+        <v>0</v>
+      </c>
+      <c r="C23" s="39">
+        <v>1</v>
+      </c>
+      <c r="D23" s="39">
+        <v>2</v>
+      </c>
+      <c r="E23" s="39">
+        <v>3</v>
+      </c>
+      <c r="F23" s="39">
+        <v>4</v>
+      </c>
+      <c r="G23" s="39">
+        <v>5</v>
+      </c>
+      <c r="H23" s="39">
+        <v>6</v>
+      </c>
+      <c r="I23" s="39">
+        <v>7</v>
+      </c>
+      <c r="J23" s="39">
+        <v>8</v>
+      </c>
+      <c r="K23" s="39">
+        <v>9</v>
+      </c>
+      <c r="L23" s="39"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>A14</f>
+        <v>Ref</v>
+      </c>
+      <c r="B24" s="40">
+        <f>$C14+B$23*ABS($C14-$D14)/9</f>
+        <v>-705.1</v>
+      </c>
+      <c r="C24" s="40">
+        <f t="shared" ref="C24:K24" si="5">$C14+C$23*ABS($C14-$D14)/9</f>
+        <v>-636.21111111111111</v>
+      </c>
+      <c r="D24" s="40">
+        <f t="shared" si="5"/>
+        <v>-567.32222222222231</v>
+      </c>
+      <c r="E24" s="40">
+        <f t="shared" si="5"/>
+        <v>-498.43333333333339</v>
+      </c>
+      <c r="F24" s="40">
+        <f t="shared" si="5"/>
+        <v>-429.54444444444448</v>
+      </c>
+      <c r="G24" s="40">
+        <f t="shared" si="5"/>
+        <v>-360.65555555555557</v>
+      </c>
+      <c r="H24" s="40">
+        <f t="shared" si="5"/>
+        <v>-291.76666666666671</v>
+      </c>
+      <c r="I24" s="40">
+        <f t="shared" si="5"/>
+        <v>-222.87777777777779</v>
+      </c>
+      <c r="J24" s="40">
+        <f t="shared" si="5"/>
+        <v>-153.98888888888894</v>
+      </c>
+      <c r="K24" s="40">
+        <f t="shared" si="5"/>
+        <v>-85.100000000000023</v>
+      </c>
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>A15</f>
+        <v>20MWe</v>
+      </c>
+      <c r="B25" s="40">
+        <f>$C15+B$23*ABS($C15-$D15)/9</f>
+        <v>-225.1</v>
+      </c>
+      <c r="C25" s="40">
+        <f t="shared" ref="C25:K25" si="6">$C15+C$23*ABS($C15-$D15)/9</f>
+        <v>-209.54444444444445</v>
+      </c>
+      <c r="D25" s="40">
+        <f t="shared" si="6"/>
+        <v>-193.98888888888888</v>
+      </c>
+      <c r="E25" s="40">
+        <f t="shared" si="6"/>
+        <v>-178.43333333333334</v>
+      </c>
+      <c r="F25" s="40">
+        <f t="shared" si="6"/>
+        <v>-162.87777777777777</v>
+      </c>
+      <c r="G25" s="40">
+        <f t="shared" si="6"/>
+        <v>-147.32222222222222</v>
+      </c>
+      <c r="H25" s="40">
+        <f t="shared" si="6"/>
+        <v>-131.76666666666665</v>
+      </c>
+      <c r="I25" s="40">
+        <f t="shared" si="6"/>
+        <v>-116.21111111111111</v>
+      </c>
+      <c r="J25" s="40">
+        <f t="shared" si="6"/>
+        <v>-100.65555555555555</v>
+      </c>
+      <c r="K25" s="40">
+        <f t="shared" si="6"/>
+        <v>-85.1</v>
+      </c>
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>A16</f>
+        <v>40MWe</v>
+      </c>
+      <c r="B26" s="40">
+        <f>$C16+B$23*ABS($C16-$D16)/9</f>
+        <v>-465.1</v>
+      </c>
+      <c r="C26" s="40">
+        <f>$C16+C$23*ABS($C16-$D16)/9</f>
+        <v>-422.87777777777779</v>
+      </c>
+      <c r="D26" s="40">
+        <f>$C16+D$23*ABS($C16-$D16)/9</f>
+        <v>-380.65555555555557</v>
+      </c>
+      <c r="E26" s="40">
+        <f>$C16+E$23*ABS($C16-$D16)/9</f>
+        <v>-338.43333333333334</v>
+      </c>
+      <c r="F26" s="40">
+        <f>$C16+F$23*ABS($C16-$D16)/9</f>
+        <v>-296.21111111111111</v>
+      </c>
+      <c r="G26" s="40">
+        <f>$C16+G$23*ABS($C16-$D16)/9</f>
+        <v>-253.98888888888891</v>
+      </c>
+      <c r="H26" s="40">
+        <f>$C16+H$23*ABS($C16-$D16)/9</f>
+        <v>-211.76666666666668</v>
+      </c>
+      <c r="I26" s="40">
+        <f>$C16+I$23*ABS($C16-$D16)/9</f>
+        <v>-169.54444444444448</v>
+      </c>
+      <c r="J26" s="40">
+        <f>$C16+J$23*ABS($C16-$D16)/9</f>
+        <v>-127.32222222222225</v>
+      </c>
+      <c r="K26" s="40">
+        <f>$C16+K$23*ABS($C16-$D16)/9</f>
+        <v>-85.100000000000023</v>
+      </c>
+      <c r="L26" s="39"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f t="shared" ref="A27:A28" si="7">A17</f>
+        <v>80MWe</v>
+      </c>
+      <c r="B27" s="40">
+        <f>$C17+B$23*ABS($C17-$D17)/9</f>
+        <v>-945.1</v>
+      </c>
+      <c r="C27" s="40">
+        <f>$C17+C$23*ABS($C17-$D17)/9</f>
+        <v>-849.54444444444448</v>
+      </c>
+      <c r="D27" s="40">
+        <f>$C17+D$23*ABS($C17-$D17)/9</f>
+        <v>-753.98888888888894</v>
+      </c>
+      <c r="E27" s="40">
+        <f>$C17+E$23*ABS($C17-$D17)/9</f>
+        <v>-658.43333333333339</v>
+      </c>
+      <c r="F27" s="40">
+        <f>$C17+F$23*ABS($C17-$D17)/9</f>
+        <v>-562.87777777777774</v>
+      </c>
+      <c r="G27" s="40">
+        <f>$C17+G$23*ABS($C17-$D17)/9</f>
+        <v>-467.32222222222225</v>
+      </c>
+      <c r="H27" s="40">
+        <f>$C17+H$23*ABS($C17-$D17)/9</f>
+        <v>-371.76666666666665</v>
+      </c>
+      <c r="I27" s="40">
+        <f>$C17+I$23*ABS($C17-$D17)/9</f>
+        <v>-276.21111111111111</v>
+      </c>
+      <c r="J27" s="40">
+        <f>$C17+J$23*ABS($C17-$D17)/9</f>
+        <v>-180.65555555555557</v>
+      </c>
+      <c r="K27" s="40">
+        <f>$C17+K$23*ABS($C17-$D17)/9</f>
+        <v>-85.100000000000023</v>
+      </c>
+      <c r="L27" s="39"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f t="shared" si="7"/>
+        <v>100MWe</v>
+      </c>
+      <c r="B28" s="40">
+        <f t="shared" ref="B28:K28" si="8">$C18+B$23*ABS($C18-$D18)/9</f>
+        <v>-985.1</v>
+      </c>
+      <c r="C28" s="40">
+        <f t="shared" si="8"/>
+        <v>-885.1</v>
+      </c>
+      <c r="D28" s="40">
+        <f t="shared" si="8"/>
+        <v>-785.1</v>
+      </c>
+      <c r="E28" s="40">
+        <f t="shared" si="8"/>
+        <v>-685.1</v>
+      </c>
+      <c r="F28" s="40">
+        <f t="shared" si="8"/>
+        <v>-585.1</v>
+      </c>
+      <c r="G28" s="40">
+        <f t="shared" si="8"/>
+        <v>-485.1</v>
+      </c>
+      <c r="H28" s="40">
+        <f t="shared" si="8"/>
+        <v>-385.1</v>
+      </c>
+      <c r="I28" s="40">
+        <f t="shared" si="8"/>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="J28" s="40">
+        <f t="shared" si="8"/>
+        <v>-185.10000000000002</v>
+      </c>
+      <c r="K28" s="40">
+        <f t="shared" si="8"/>
+        <v>-85.100000000000023</v>
+      </c>
+      <c r="L28" s="39"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="39">
+        <v>0</v>
+      </c>
+      <c r="C31" s="39">
+        <v>1</v>
+      </c>
+      <c r="D31" s="39">
+        <v>2</v>
+      </c>
+      <c r="E31" s="39">
+        <v>3</v>
+      </c>
+      <c r="F31" s="39">
+        <v>4</v>
+      </c>
+      <c r="G31" s="39">
+        <v>5</v>
+      </c>
+      <c r="H31" s="39">
+        <v>6</v>
+      </c>
+      <c r="I31" s="39">
+        <v>7</v>
+      </c>
+      <c r="J31" s="39">
+        <v>8</v>
+      </c>
+      <c r="K31" s="39">
+        <v>9</v>
+      </c>
+      <c r="L31" s="39"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>A14</f>
+        <v>Ref</v>
+      </c>
+      <c r="B32" s="40">
+        <f>$E14+B$31*ABS($E14-$F14)/9</f>
+        <v>-17719.163</v>
+      </c>
+      <c r="C32" s="40">
+        <f>$E14+C$31*ABS($E14-$F14)/9</f>
+        <v>-15987.985222222222</v>
+      </c>
+      <c r="D32" s="40">
+        <f>$E14+D$31*ABS($E14-$F14)/9</f>
+        <v>-14256.807444444445</v>
+      </c>
+      <c r="E32" s="40">
+        <f>$E14+E$31*ABS($E14-$F14)/9</f>
+        <v>-12525.629666666668</v>
+      </c>
+      <c r="F32" s="40">
+        <f>$E14+F$31*ABS($E14-$F14)/9</f>
+        <v>-10794.451888888889</v>
+      </c>
+      <c r="G32" s="40">
+        <f>$E14+G$31*ABS($E14-$F14)/9</f>
+        <v>-9063.2741111111118</v>
+      </c>
+      <c r="H32" s="40">
+        <f>$E14+H$31*ABS($E14-$F14)/9</f>
+        <v>-7332.096333333333</v>
+      </c>
+      <c r="I32" s="40">
+        <f>$E14+I$31*ABS($E14-$F14)/9</f>
+        <v>-5600.9185555555559</v>
+      </c>
+      <c r="J32" s="40">
+        <f>$E14+J$31*ABS($E14-$F14)/9</f>
+        <v>-3869.7407777777771</v>
+      </c>
+      <c r="K32" s="40">
+        <f>$E14+K$31*ABS($E14-$F14)/9</f>
+        <v>-2138.5630000000019</v>
+      </c>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>A15</f>
+        <v>20MWe</v>
+      </c>
+      <c r="B33" s="40">
+        <f>$E15+B$31*ABS($E15-$F15)/9</f>
+        <v>-5656.7629999999999</v>
+      </c>
+      <c r="C33" s="40">
+        <f>$E15+C$31*ABS($E15-$F15)/9</f>
+        <v>-5265.8518888888884</v>
+      </c>
+      <c r="D33" s="40">
+        <f>$E15+D$31*ABS($E15-$F15)/9</f>
+        <v>-4874.9407777777778</v>
+      </c>
+      <c r="E33" s="40">
+        <f>$E15+E$31*ABS($E15-$F15)/9</f>
+        <v>-4484.0296666666663</v>
+      </c>
+      <c r="F33" s="40">
+        <f>$E15+F$31*ABS($E15-$F15)/9</f>
+        <v>-4093.1185555555553</v>
+      </c>
+      <c r="G33" s="40">
+        <f>$E15+G$31*ABS($E15-$F15)/9</f>
+        <v>-3702.2074444444443</v>
+      </c>
+      <c r="H33" s="40">
+        <f>$E15+H$31*ABS($E15-$F15)/9</f>
+        <v>-3311.2963333333332</v>
+      </c>
+      <c r="I33" s="40">
+        <f>$E15+I$31*ABS($E15-$F15)/9</f>
+        <v>-2920.3852222222222</v>
+      </c>
+      <c r="J33" s="40">
+        <f>$E15+J$31*ABS($E15-$F15)/9</f>
+        <v>-2529.4741111111107</v>
+      </c>
+      <c r="K33" s="40">
+        <f>$E15+K$31*ABS($E15-$F15)/9</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="L33" s="40"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>A16</f>
+        <v>40MWe</v>
+      </c>
+      <c r="B34" s="40">
+        <f>$E16+B$31*ABS($E16-$F16)/9</f>
+        <v>-11687.963</v>
+      </c>
+      <c r="C34" s="40">
+        <f>$E16+C$31*ABS($E16-$F16)/9</f>
+        <v>-10626.918555555556</v>
+      </c>
+      <c r="D34" s="40">
+        <f>$E16+D$31*ABS($E16-$F16)/9</f>
+        <v>-9565.8741111111103</v>
+      </c>
+      <c r="E34" s="40">
+        <f>$E16+E$31*ABS($E16-$F16)/9</f>
+        <v>-8504.8296666666665</v>
+      </c>
+      <c r="F34" s="40">
+        <f>$E16+F$31*ABS($E16-$F16)/9</f>
+        <v>-7443.7852222222218</v>
+      </c>
+      <c r="G34" s="40">
+        <f>$E16+G$31*ABS($E16-$F16)/9</f>
+        <v>-6382.7407777777771</v>
+      </c>
+      <c r="H34" s="40">
+        <f>$E16+H$31*ABS($E16-$F16)/9</f>
+        <v>-5321.6963333333333</v>
+      </c>
+      <c r="I34" s="40">
+        <f>$E16+I$31*ABS($E16-$F16)/9</f>
+        <v>-4260.6518888888886</v>
+      </c>
+      <c r="J34" s="40">
+        <f>$E16+J$31*ABS($E16-$F16)/9</f>
+        <v>-3199.6074444444439</v>
+      </c>
+      <c r="K34" s="40">
+        <f>$E16+K$31*ABS($E16-$F16)/9</f>
+        <v>-2138.5630000000001</v>
+      </c>
+      <c r="L34" s="39"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f t="shared" ref="A35:A36" si="9">A17</f>
+        <v>80MWe</v>
+      </c>
+      <c r="B35" s="40">
+        <f t="shared" ref="B35:K35" si="10">$E17+B$31*ABS($E17-$F17)/9</f>
+        <v>-23750.363000000001</v>
+      </c>
+      <c r="C35" s="40">
+        <f t="shared" si="10"/>
+        <v>-21349.051888888891</v>
+      </c>
+      <c r="D35" s="40">
+        <f t="shared" si="10"/>
+        <v>-18947.740777777777</v>
+      </c>
+      <c r="E35" s="40">
+        <f t="shared" si="10"/>
+        <v>-16546.429666666667</v>
+      </c>
+      <c r="F35" s="40">
+        <f t="shared" si="10"/>
+        <v>-14145.118555555555</v>
+      </c>
+      <c r="G35" s="40">
+        <f t="shared" si="10"/>
+        <v>-11743.807444444445</v>
+      </c>
+      <c r="H35" s="40">
+        <f t="shared" si="10"/>
+        <v>-9342.4963333333326</v>
+      </c>
+      <c r="I35" s="40">
+        <f t="shared" si="10"/>
+        <v>-6941.1852222222187</v>
+      </c>
+      <c r="J35" s="40">
+        <f t="shared" si="10"/>
+        <v>-4539.8741111111085</v>
+      </c>
+      <c r="K35" s="40">
+        <f t="shared" si="10"/>
+        <v>-2138.5629999999983</v>
+      </c>
+      <c r="L35" s="39"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f t="shared" si="9"/>
+        <v>100MWe</v>
+      </c>
+      <c r="B36" s="40">
+        <f t="shared" ref="B36:K36" si="11">$E18+B$31*ABS($E18-$F18)/9</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="C36" s="40">
+        <f t="shared" si="11"/>
+        <v>-22242.562999999998</v>
+      </c>
+      <c r="D36" s="40">
+        <f t="shared" si="11"/>
+        <v>-19729.562999999998</v>
+      </c>
+      <c r="E36" s="40">
+        <f t="shared" si="11"/>
+        <v>-17216.562999999998</v>
+      </c>
+      <c r="F36" s="40">
+        <f t="shared" si="11"/>
+        <v>-14703.562999999998</v>
+      </c>
+      <c r="G36" s="40">
+        <f t="shared" si="11"/>
+        <v>-12190.562999999998</v>
+      </c>
+      <c r="H36" s="40">
+        <f t="shared" si="11"/>
+        <v>-9677.5629999999983</v>
+      </c>
+      <c r="I36" s="40">
+        <f t="shared" si="11"/>
+        <v>-7164.5629999999983</v>
+      </c>
+      <c r="J36" s="40">
+        <f t="shared" si="11"/>
+        <v>-4651.5629999999983</v>
+      </c>
+      <c r="K36" s="40">
+        <f t="shared" si="11"/>
+        <v>-2138.5629999999983</v>
+      </c>
+      <c r="L36" s="39"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="39"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" t="str">
+        <f>A14</f>
+        <v>Ref</v>
+      </c>
+      <c r="F39" t="str">
+        <f>A15</f>
+        <v>20MWe</v>
+      </c>
+      <c r="H39" t="str">
+        <f>A16</f>
+        <v>40MWe</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" t="s">
+        <v>189</v>
+      </c>
+      <c r="G40" t="s">
+        <v>190</v>
+      </c>
+      <c r="H40" t="s">
+        <v>189</v>
+      </c>
+      <c r="I40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="35">
+        <f t="shared" ref="B41:B43" si="12">ROUNDUP(C41*$B$45/$C$45,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C41" s="35">
+        <v>934</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="34">
+        <f>ABS($E$14)*24*B41</f>
+        <v>850519.82400000002</v>
+      </c>
+      <c r="F41" s="34">
+        <v>0</v>
+      </c>
+      <c r="G41" s="34">
+        <f>ABS($E$15)*24*$B41</f>
+        <v>271524.62400000001</v>
+      </c>
+      <c r="H41" s="34">
+        <v>0</v>
+      </c>
+      <c r="I41" s="34">
+        <f>ABS($E$16)*24*$B41</f>
+        <v>561022.22399999993</v>
+      </c>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" s="35">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="C42" s="35">
+        <v>4231</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="34">
+        <f>ABS($E$14)*24*B42</f>
+        <v>2976819.3840000001</v>
+      </c>
+      <c r="F42" s="34">
+        <v>0</v>
+      </c>
+      <c r="G42" s="34">
+        <f t="shared" ref="G42:G45" si="13">ABS($E$15)*24*$B42</f>
+        <v>950336.18400000001</v>
+      </c>
+      <c r="H42" s="34">
+        <v>0</v>
+      </c>
+      <c r="I42" s="34">
+        <f t="shared" ref="I42:I45" si="14">ABS($E$16)*24*$B42</f>
+        <v>1963577.7839999998</v>
+      </c>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="35">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C43" s="35">
+        <v>934</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="34">
+        <f>ABS($E$14)*24*B43</f>
+        <v>850519.82400000002</v>
+      </c>
+      <c r="F43" s="34">
+        <v>0</v>
+      </c>
+      <c r="G43" s="34">
+        <f t="shared" si="13"/>
+        <v>271524.62400000001</v>
+      </c>
+      <c r="H43" s="34">
+        <v>0</v>
+      </c>
+      <c r="I43" s="34">
+        <f t="shared" si="14"/>
+        <v>561022.22399999993</v>
+      </c>
+      <c r="J43" s="34"/>
+      <c r="K43" s="34"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="35">
+        <f>ROUNDUP(C44*$B$45/$C$45,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="35">
+        <v>97</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" s="34">
+        <f>ABS($E$14)*24*B44</f>
+        <v>425259.91200000001</v>
+      </c>
+      <c r="F44" s="34">
+        <v>0</v>
+      </c>
+      <c r="G44" s="34">
+        <f t="shared" si="13"/>
+        <v>135762.31200000001</v>
+      </c>
+      <c r="H44" s="34">
+        <v>0</v>
+      </c>
+      <c r="I44" s="34">
+        <f t="shared" si="14"/>
+        <v>280511.11199999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="35">
+        <v>14</v>
+      </c>
+      <c r="C45" s="35">
+        <v>8997</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="34">
+        <f>ABS($E$14)*24*B45</f>
+        <v>5953638.7680000002</v>
+      </c>
+      <c r="F45" s="34">
+        <v>0</v>
+      </c>
+      <c r="G45" s="34">
+        <f t="shared" si="13"/>
+        <v>1900672.368</v>
+      </c>
+      <c r="H45" s="34">
+        <v>0</v>
+      </c>
+      <c r="I45" s="34">
+        <f t="shared" si="14"/>
+        <v>3927155.5679999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" s="35">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" s="35">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47" s="35">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>6</v>
+      </c>
+      <c r="I47" s="35">
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <v>8</v>
+      </c>
+      <c r="K47" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f>A41</f>
+        <v>illinois</v>
+      </c>
+      <c r="B48" s="34">
+        <f>$D41+B$47*ABS($E41-$D41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="34">
+        <f>$D41+C$47*ABS($E41-$D41)/9</f>
+        <v>94502.202666666664</v>
+      </c>
+      <c r="D48" s="34">
+        <f t="shared" ref="C48:K48" si="15">$D41+D$47*ABS($E41-$D41)/9</f>
+        <v>189004.40533333333</v>
+      </c>
+      <c r="E48" s="34">
+        <f t="shared" si="15"/>
+        <v>283506.60800000001</v>
+      </c>
+      <c r="F48" s="34">
+        <f t="shared" si="15"/>
+        <v>378008.81066666666</v>
+      </c>
+      <c r="G48" s="34">
+        <f t="shared" si="15"/>
+        <v>472511.01333333337</v>
+      </c>
+      <c r="H48" s="34">
+        <f t="shared" si="15"/>
+        <v>567013.21600000001</v>
+      </c>
+      <c r="I48" s="34">
+        <f t="shared" si="15"/>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="J48" s="34">
+        <f t="shared" si="15"/>
+        <v>756017.62133333331</v>
+      </c>
+      <c r="K48" s="34">
+        <f t="shared" si="15"/>
+        <v>850519.82400000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f t="shared" ref="A49:A52" si="16">A42</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B49" s="34">
+        <f t="shared" ref="B49:K52" si="17">$D42+B$47*ABS($E42-$D42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="34">
+        <f t="shared" si="17"/>
+        <v>330757.70933333336</v>
+      </c>
+      <c r="D49" s="34">
+        <f t="shared" si="17"/>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="E49" s="34">
+        <f t="shared" si="17"/>
+        <v>992273.12800000003</v>
+      </c>
+      <c r="F49" s="34">
+        <f t="shared" si="17"/>
+        <v>1323030.8373333334</v>
+      </c>
+      <c r="G49" s="34">
+        <f t="shared" si="17"/>
+        <v>1653788.5466666666</v>
+      </c>
+      <c r="H49" s="34">
+        <f t="shared" si="17"/>
+        <v>1984546.2560000001</v>
+      </c>
+      <c r="I49" s="34">
+        <f t="shared" si="17"/>
+        <v>2315303.9653333332</v>
+      </c>
+      <c r="J49" s="34">
+        <f t="shared" si="17"/>
+        <v>2646061.6746666669</v>
+      </c>
+      <c r="K49" s="34">
+        <f t="shared" si="17"/>
+        <v>2976819.3840000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="str">
+        <f t="shared" si="16"/>
+        <v>ohio</v>
+      </c>
+      <c r="B50" s="34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="C50" s="34">
+        <f t="shared" si="17"/>
+        <v>94502.202666666664</v>
+      </c>
+      <c r="D50" s="34">
+        <f t="shared" si="17"/>
+        <v>189004.40533333333</v>
+      </c>
+      <c r="E50" s="34">
+        <f t="shared" si="17"/>
+        <v>283506.60800000001</v>
+      </c>
+      <c r="F50" s="34">
+        <f t="shared" si="17"/>
+        <v>378008.81066666666</v>
+      </c>
+      <c r="G50" s="34">
+        <f t="shared" si="17"/>
+        <v>472511.01333333337</v>
+      </c>
+      <c r="H50" s="34">
+        <f t="shared" si="17"/>
+        <v>567013.21600000001</v>
+      </c>
+      <c r="I50" s="34">
+        <f t="shared" si="17"/>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="J50" s="34">
+        <f t="shared" si="17"/>
+        <v>756017.62133333331</v>
+      </c>
+      <c r="K50" s="34">
+        <f t="shared" si="17"/>
+        <v>850519.82400000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f t="shared" si="16"/>
+        <v>minnesota</v>
+      </c>
+      <c r="B51" s="34">
+        <f>$D44+B$47*ABS($E44-$D44)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="34">
+        <f t="shared" si="17"/>
+        <v>47251.101333333332</v>
+      </c>
+      <c r="D51" s="34">
+        <f t="shared" si="17"/>
+        <v>94502.202666666664</v>
+      </c>
+      <c r="E51" s="34">
+        <f t="shared" si="17"/>
+        <v>141753.304</v>
+      </c>
+      <c r="F51" s="34">
+        <f t="shared" si="17"/>
+        <v>189004.40533333333</v>
+      </c>
+      <c r="G51" s="34">
+        <f t="shared" si="17"/>
+        <v>236255.50666666668</v>
+      </c>
+      <c r="H51" s="34">
+        <f t="shared" si="17"/>
+        <v>283506.60800000001</v>
+      </c>
+      <c r="I51" s="34">
+        <f t="shared" si="17"/>
+        <v>330757.70933333336</v>
+      </c>
+      <c r="J51" s="34">
+        <f t="shared" si="17"/>
+        <v>378008.81066666666</v>
+      </c>
+      <c r="K51" s="34">
+        <f t="shared" si="17"/>
+        <v>425259.91200000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="str">
+        <f t="shared" si="16"/>
+        <v>texas</v>
+      </c>
+      <c r="B52" s="34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="C52" s="34">
+        <f>$D45+C$47*ABS($E45-$D45)/9</f>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="D52" s="34">
+        <f t="shared" si="17"/>
+        <v>1323030.8373333334</v>
+      </c>
+      <c r="E52" s="34">
+        <f t="shared" si="17"/>
+        <v>1984546.2560000001</v>
+      </c>
+      <c r="F52" s="34">
+        <f t="shared" si="17"/>
+        <v>2646061.6746666669</v>
+      </c>
+      <c r="G52" s="34">
+        <f t="shared" si="17"/>
+        <v>3307577.0933333333</v>
+      </c>
+      <c r="H52" s="34">
+        <f t="shared" si="17"/>
+        <v>3969092.5120000001</v>
+      </c>
+      <c r="I52" s="34">
+        <f t="shared" si="17"/>
+        <v>4630607.9306666665</v>
+      </c>
+      <c r="J52" s="34">
+        <f t="shared" si="17"/>
+        <v>5292123.3493333338</v>
+      </c>
+      <c r="K52" s="34">
+        <f t="shared" si="17"/>
+        <v>5953638.7680000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54" s="35">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" s="35">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54" s="35">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>6</v>
+      </c>
+      <c r="I54" s="35">
+        <v>7</v>
+      </c>
+      <c r="J54">
+        <v>8</v>
+      </c>
+      <c r="K54" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="str">
+        <f>A48</f>
+        <v>illinois</v>
+      </c>
+      <c r="B55" s="34">
+        <f>$F41+B$47*ABS($G41-$F41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="34">
+        <f t="shared" ref="C55:K55" si="18">$F41+C$47*ABS($G41-$F41)/9</f>
+        <v>30169.402666666669</v>
+      </c>
+      <c r="D55" s="34">
+        <f t="shared" si="18"/>
+        <v>60338.805333333337</v>
+      </c>
+      <c r="E55" s="34">
+        <f t="shared" si="18"/>
+        <v>90508.207999999999</v>
+      </c>
+      <c r="F55" s="34">
+        <f t="shared" si="18"/>
+        <v>120677.61066666667</v>
+      </c>
+      <c r="G55" s="34">
+        <f t="shared" si="18"/>
+        <v>150847.01333333334</v>
+      </c>
+      <c r="H55" s="34">
+        <f t="shared" si="18"/>
+        <v>181016.416</v>
+      </c>
+      <c r="I55" s="34">
+        <f t="shared" si="18"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="J55" s="34">
+        <f t="shared" si="18"/>
+        <v>241355.22133333335</v>
+      </c>
+      <c r="K55" s="34">
+        <f t="shared" si="18"/>
+        <v>271524.62400000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="str">
+        <f t="shared" ref="A56:A59" si="19">A49</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B56" s="34">
+        <f t="shared" ref="B56:K59" si="20">$F42+B$47*ABS($G42-$F42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="34">
+        <f t="shared" si="20"/>
+        <v>105592.90933333333</v>
+      </c>
+      <c r="D56" s="34">
+        <f t="shared" si="20"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="E56" s="34">
+        <f t="shared" si="20"/>
+        <v>316778.728</v>
+      </c>
+      <c r="F56" s="34">
+        <f t="shared" si="20"/>
+        <v>422371.63733333332</v>
+      </c>
+      <c r="G56" s="34">
+        <f t="shared" si="20"/>
+        <v>527964.54666666663</v>
+      </c>
+      <c r="H56" s="34">
+        <f t="shared" si="20"/>
+        <v>633557.45600000001</v>
+      </c>
+      <c r="I56" s="34">
+        <f t="shared" si="20"/>
+        <v>739150.36533333326</v>
+      </c>
+      <c r="J56" s="34">
+        <f t="shared" si="20"/>
+        <v>844743.27466666664</v>
+      </c>
+      <c r="K56" s="34">
+        <f t="shared" si="20"/>
+        <v>950336.18399999989</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f t="shared" si="19"/>
+        <v>ohio</v>
+      </c>
+      <c r="B57" s="34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="C57" s="34">
+        <f t="shared" si="20"/>
+        <v>30169.402666666669</v>
+      </c>
+      <c r="D57" s="34">
+        <f t="shared" si="20"/>
+        <v>60338.805333333337</v>
+      </c>
+      <c r="E57" s="34">
+        <f t="shared" si="20"/>
+        <v>90508.207999999999</v>
+      </c>
+      <c r="F57" s="34">
+        <f t="shared" si="20"/>
+        <v>120677.61066666667</v>
+      </c>
+      <c r="G57" s="34">
+        <f t="shared" si="20"/>
+        <v>150847.01333333334</v>
+      </c>
+      <c r="H57" s="34">
+        <f t="shared" si="20"/>
+        <v>181016.416</v>
+      </c>
+      <c r="I57" s="34">
+        <f t="shared" si="20"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="J57" s="34">
+        <f t="shared" si="20"/>
+        <v>241355.22133333335</v>
+      </c>
+      <c r="K57" s="34">
+        <f t="shared" si="20"/>
+        <v>271524.62400000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="str">
+        <f t="shared" si="19"/>
+        <v>minnesota</v>
+      </c>
+      <c r="B58" s="34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="C58" s="34">
+        <f t="shared" si="20"/>
+        <v>15084.701333333334</v>
+      </c>
+      <c r="D58" s="34">
+        <f t="shared" si="20"/>
+        <v>30169.402666666669</v>
+      </c>
+      <c r="E58" s="34">
+        <f t="shared" si="20"/>
+        <v>45254.103999999999</v>
+      </c>
+      <c r="F58" s="34">
+        <f t="shared" si="20"/>
+        <v>60338.805333333337</v>
+      </c>
+      <c r="G58" s="34">
+        <f t="shared" si="20"/>
+        <v>75423.506666666668</v>
+      </c>
+      <c r="H58" s="34">
+        <f t="shared" si="20"/>
+        <v>90508.207999999999</v>
+      </c>
+      <c r="I58" s="34">
+        <f t="shared" si="20"/>
+        <v>105592.90933333333</v>
+      </c>
+      <c r="J58" s="34">
+        <f t="shared" si="20"/>
+        <v>120677.61066666667</v>
+      </c>
+      <c r="K58" s="34">
+        <f t="shared" si="20"/>
+        <v>135762.31200000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="str">
+        <f t="shared" si="19"/>
+        <v>texas</v>
+      </c>
+      <c r="B59" s="34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="C59" s="34">
+        <f t="shared" si="20"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="D59" s="34">
+        <f t="shared" si="20"/>
+        <v>422371.63733333332</v>
+      </c>
+      <c r="E59" s="34">
+        <f t="shared" si="20"/>
+        <v>633557.45600000001</v>
+      </c>
+      <c r="F59" s="34">
+        <f t="shared" si="20"/>
+        <v>844743.27466666664</v>
+      </c>
+      <c r="G59" s="34">
+        <f t="shared" si="20"/>
+        <v>1055929.0933333333</v>
+      </c>
+      <c r="H59" s="34">
+        <f t="shared" si="20"/>
+        <v>1267114.912</v>
+      </c>
+      <c r="I59" s="34">
+        <f t="shared" si="20"/>
+        <v>1478300.7306666665</v>
+      </c>
+      <c r="J59" s="34">
+        <f t="shared" si="20"/>
+        <v>1689486.5493333333</v>
+      </c>
+      <c r="K59" s="34">
+        <f t="shared" si="20"/>
+        <v>1900672.3679999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61" s="35">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="35">
+        <v>3</v>
+      </c>
+      <c r="F61">
+        <v>4</v>
+      </c>
+      <c r="G61" s="35">
+        <v>5</v>
+      </c>
+      <c r="H61">
+        <v>6</v>
+      </c>
+      <c r="I61" s="35">
+        <v>7</v>
+      </c>
+      <c r="J61">
+        <v>8</v>
+      </c>
+      <c r="K61" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="str">
+        <f>A55</f>
+        <v>illinois</v>
+      </c>
+      <c r="B62" s="34">
+        <f>$H41+B$47*ABS($I41-$H41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C62" s="34">
+        <f t="shared" ref="C62:K62" si="21">$H41+C$47*ABS($I41-$H41)/9</f>
+        <v>62335.802666666656</v>
+      </c>
+      <c r="D62" s="34">
+        <f t="shared" si="21"/>
+        <v>124671.60533333331</v>
+      </c>
+      <c r="E62" s="34">
+        <f t="shared" si="21"/>
+        <v>187007.40799999997</v>
+      </c>
+      <c r="F62" s="34">
+        <f t="shared" si="21"/>
+        <v>249343.21066666662</v>
+      </c>
+      <c r="G62" s="34">
+        <f t="shared" si="21"/>
+        <v>311679.01333333331</v>
+      </c>
+      <c r="H62" s="34">
+        <f t="shared" si="21"/>
+        <v>374014.81599999993</v>
+      </c>
+      <c r="I62" s="34">
+        <f t="shared" si="21"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="J62" s="34">
+        <f t="shared" si="21"/>
+        <v>498686.42133333324</v>
+      </c>
+      <c r="K62" s="34">
+        <f t="shared" si="21"/>
+        <v>561022.22399999993</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="str">
+        <f t="shared" ref="A63:A66" si="22">A56</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B63" s="34">
+        <f t="shared" ref="B63:K66" si="23">$H42+B$47*ABS($I42-$H42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="34">
+        <f t="shared" si="23"/>
+        <v>218175.30933333331</v>
+      </c>
+      <c r="D63" s="34">
+        <f t="shared" si="23"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="E63" s="34">
+        <f t="shared" si="23"/>
+        <v>654525.92799999984</v>
+      </c>
+      <c r="F63" s="34">
+        <f t="shared" si="23"/>
+        <v>872701.23733333324</v>
+      </c>
+      <c r="G63" s="34">
+        <f t="shared" si="23"/>
+        <v>1090876.5466666664</v>
+      </c>
+      <c r="H63" s="34">
+        <f t="shared" si="23"/>
+        <v>1309051.8559999997</v>
+      </c>
+      <c r="I63" s="34">
+        <f t="shared" si="23"/>
+        <v>1527227.1653333332</v>
+      </c>
+      <c r="J63" s="34">
+        <f t="shared" si="23"/>
+        <v>1745402.4746666665</v>
+      </c>
+      <c r="K63" s="34">
+        <f t="shared" si="23"/>
+        <v>1963577.7839999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f t="shared" si="22"/>
+        <v>ohio</v>
+      </c>
+      <c r="B64" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C64" s="34">
+        <f t="shared" si="23"/>
+        <v>62335.802666666656</v>
+      </c>
+      <c r="D64" s="34">
+        <f t="shared" si="23"/>
+        <v>124671.60533333331</v>
+      </c>
+      <c r="E64" s="34">
+        <f t="shared" si="23"/>
+        <v>187007.40799999997</v>
+      </c>
+      <c r="F64" s="34">
+        <f t="shared" si="23"/>
+        <v>249343.21066666662</v>
+      </c>
+      <c r="G64" s="34">
+        <f t="shared" si="23"/>
+        <v>311679.01333333331</v>
+      </c>
+      <c r="H64" s="34">
+        <f t="shared" si="23"/>
+        <v>374014.81599999993</v>
+      </c>
+      <c r="I64" s="34">
+        <f t="shared" si="23"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="J64" s="34">
+        <f t="shared" si="23"/>
+        <v>498686.42133333324</v>
+      </c>
+      <c r="K64" s="34">
+        <f t="shared" si="23"/>
+        <v>561022.22399999993</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f t="shared" si="22"/>
+        <v>minnesota</v>
+      </c>
+      <c r="B65" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C65" s="34">
+        <f t="shared" si="23"/>
+        <v>31167.901333333328</v>
+      </c>
+      <c r="D65" s="34">
+        <f t="shared" si="23"/>
+        <v>62335.802666666656</v>
+      </c>
+      <c r="E65" s="34">
+        <f t="shared" si="23"/>
+        <v>93503.703999999983</v>
+      </c>
+      <c r="F65" s="34">
+        <f t="shared" si="23"/>
+        <v>124671.60533333331</v>
+      </c>
+      <c r="G65" s="34">
+        <f t="shared" si="23"/>
+        <v>155839.50666666665</v>
+      </c>
+      <c r="H65" s="34">
+        <f t="shared" si="23"/>
+        <v>187007.40799999997</v>
+      </c>
+      <c r="I65" s="34">
+        <f t="shared" si="23"/>
+        <v>218175.30933333331</v>
+      </c>
+      <c r="J65" s="34">
+        <f t="shared" si="23"/>
+        <v>249343.21066666662</v>
+      </c>
+      <c r="K65" s="34">
+        <f t="shared" si="23"/>
+        <v>280511.11199999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="str">
+        <f t="shared" si="22"/>
+        <v>texas</v>
+      </c>
+      <c r="B66" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C66" s="34">
+        <f t="shared" si="23"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="D66" s="34">
+        <f t="shared" si="23"/>
+        <v>872701.23733333324</v>
+      </c>
+      <c r="E66" s="34">
+        <f t="shared" si="23"/>
+        <v>1309051.8559999997</v>
+      </c>
+      <c r="F66" s="34">
+        <f t="shared" si="23"/>
+        <v>1745402.4746666665</v>
+      </c>
+      <c r="G66" s="34">
+        <f t="shared" si="23"/>
+        <v>2181753.0933333328</v>
+      </c>
+      <c r="H66" s="34">
+        <f t="shared" si="23"/>
+        <v>2618103.7119999994</v>
+      </c>
+      <c r="I66" s="34">
+        <f t="shared" si="23"/>
+        <v>3054454.3306666664</v>
+      </c>
+      <c r="J66" s="34">
+        <f t="shared" si="23"/>
+        <v>3490804.9493333329</v>
+      </c>
+      <c r="K66" s="34">
+        <f t="shared" si="23"/>
+        <v>3927155.5679999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4300,10 +4457,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="38"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -4471,26 +4628,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4562,15 +4719,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4648,22 +4805,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4677,11 +4834,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -4937,7 +5094,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O2" s="25" t="s">
         <v>27</v>
@@ -4951,16 +5108,16 @@
         <v>80</v>
       </c>
       <c r="M3" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O3" s="22">
         <v>257800644</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4968,16 +5125,16 @@
         <v>105</v>
       </c>
       <c r="M4" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O4" s="22">
         <v>5156012.88</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -4992,13 +5149,13 @@
       </c>
       <c r="M5" s="28"/>
       <c r="N5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O5" s="22">
         <v>25780064.399999999</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -5022,13 +5179,13 @@
       </c>
       <c r="M6" s="28"/>
       <c r="N6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O6" s="22">
         <v>38670096.600000001</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -5052,13 +5209,13 @@
       </c>
       <c r="M7" s="28"/>
       <c r="N7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O7" s="22">
         <v>12251143</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -5084,13 +5241,13 @@
       </c>
       <c r="M8" s="28"/>
       <c r="N8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O8" s="22">
         <v>38670096.600000001</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -5116,13 +5273,13 @@
         <v>0.3979400086720376</v>
       </c>
       <c r="M9" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O9" s="22">
         <v>120527413.48</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5142,16 +5299,16 @@
         <v>8.4682380044363352</v>
       </c>
       <c r="M10" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O10" s="22">
         <v>550360</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5166,13 +5323,13 @@
         <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O11" s="23">
         <v>378878417.48000002</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -5190,16 +5347,16 @@
       </c>
       <c r="E12" s="14"/>
       <c r="M12" s="28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O12" s="22">
         <v>9607972</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -5211,16 +5368,16 @@
       </c>
       <c r="E13" s="14"/>
       <c r="M13" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O13" s="22">
         <v>1921594.4</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -5238,16 +5395,16 @@
       </c>
       <c r="E14" s="14"/>
       <c r="M14" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O14" s="22">
         <v>7577568.3499999996</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -5263,13 +5420,13 @@
       </c>
       <c r="E15" s="14"/>
       <c r="M15" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O15" s="22">
         <v>1049006</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -5282,13 +5439,13 @@
       <c r="C16" s="1"/>
       <c r="E16" s="14"/>
       <c r="M16" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O16" s="23">
         <v>20156140.75</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -5303,26 +5460,26 @@
       </c>
       <c r="E17" s="14"/>
       <c r="M17" s="28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="O17" s="22">
         <v>7085933</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="E18" s="14"/>
       <c r="M18" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O18" s="23">
         <v>7085933</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5334,7 +5491,7 @@
       </c>
       <c r="E19" s="14"/>
       <c r="M19" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N19" s="24" t="s">
         <v>4</v>
@@ -5551,7 +5708,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>133</v>
@@ -5568,7 +5725,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>136</v>
@@ -5586,7 +5743,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -5604,7 +5761,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
         <v>139</v>
@@ -5622,7 +5779,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
         <v>141</v>
@@ -5640,7 +5797,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>143</v>
@@ -5658,7 +5815,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
         <v>145</v>
@@ -5676,7 +5833,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
Calculate SA sweep values for SMR capacity cases
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC12F5-D4F6-1549-84CD-EAF3D73E4F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284A4D28-EA24-4B4F-AE20-B66E2235870D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37140" yWindow="1460" windowWidth="35980" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="35840" yWindow="-1600" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="SMR" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="214">
   <si>
     <t>Source</t>
   </si>
@@ -644,12 +644,6 @@
     <t>Location elec. Prices</t>
   </si>
   <si>
-    <t>6 units</t>
-  </si>
-  <si>
-    <t>18 units</t>
-  </si>
-  <si>
     <t>Find Abdalla's report citation</t>
   </si>
   <si>
@@ -687,6 +681,9 @@
   </si>
   <si>
     <t>100MWe</t>
+  </si>
+  <si>
+    <t>Ref (60MWe)</t>
   </si>
 </sst>
 </file>
@@ -769,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -946,6 +943,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -954,7 +975,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -991,17 +1012,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2427,15 +2493,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H2">
         <v>12</v>
@@ -2443,19 +2509,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
         <v>197</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -2475,19 +2541,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="36">
+        <v>202</v>
+      </c>
+      <c r="B4" s="34">
         <v>1802460</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="34">
         <v>5569000</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="34">
         <v>24646000</v>
       </c>
       <c r="G4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H4">
         <f>H3*$H$2</f>
@@ -2512,15 +2578,15 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" s="36">
+        <v>204</v>
+      </c>
+      <c r="B5" s="34">
         <v>3.71</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="34">
         <v>23.2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="34">
         <v>55.69</v>
       </c>
     </row>
@@ -2531,10 +2597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:K51"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2641,1786 +2707,2445 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38" t="s">
+      <c r="D12" s="47"/>
+      <c r="E12" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="14" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="45">
         <v>720</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="45">
         <f>MAX(-B14+$B$5, -1000+$B$5)</f>
         <v>-705.1</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="45">
         <f>-100+$B$5</f>
         <v>-85.1</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="45">
         <f>C14*25.13</f>
         <v>-17719.163</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="14">
         <f>D14*25.13</f>
         <v>-2138.5629999999996</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="45">
         <v>240</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="45">
         <f t="shared" ref="C15:C18" si="0">MAX(-B15+$B$5, -1000+$B$5)</f>
         <v>-225.1</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="45">
         <f t="shared" ref="D15:D18" si="1">-100+$B$5</f>
         <v>-85.1</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="45">
         <f t="shared" ref="E15:F15" si="2">C15*25.13</f>
         <v>-5656.7629999999999</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="14">
         <f t="shared" si="2"/>
         <v>-2138.5629999999996</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="45">
         <v>480</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="45">
         <f t="shared" si="0"/>
         <v>-465.1</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="45">
         <f t="shared" si="1"/>
         <v>-85.1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="45">
         <f>C16*25.13</f>
         <v>-11687.963</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="14">
         <f>D16*25.13</f>
         <v>-2138.5629999999996</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="45">
         <v>960</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="45">
         <f t="shared" si="0"/>
         <v>-945.1</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="45">
         <f t="shared" si="1"/>
         <v>-85.1</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="45">
         <f t="shared" ref="E17:E18" si="3">C17*25.13</f>
         <v>-23750.363000000001</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="14">
         <f t="shared" ref="F17:F18" si="4">D17*25.13</f>
         <v>-2138.5629999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>214</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="24">
         <v>1200</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="24">
         <f t="shared" si="0"/>
         <v>-985.1</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="24">
         <f t="shared" si="1"/>
         <v>-85.1</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="24">
         <f t="shared" si="3"/>
         <v>-24755.562999999998</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="17">
         <f t="shared" si="4"/>
         <v>-2138.5629999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="21" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+    </row>
+    <row r="22" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="36"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="B23" s="39">
+      <c r="B23" s="54">
         <v>0</v>
       </c>
-      <c r="C23" s="39">
+      <c r="C23" s="54">
         <v>1</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="54">
         <v>2</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="54">
         <v>3</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="54">
         <v>4</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="54">
         <v>5</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="54">
         <v>6</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="54">
         <v>7</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="54">
         <v>8</v>
       </c>
-      <c r="K23" s="39">
+      <c r="K23" s="55">
         <v>9</v>
       </c>
-      <c r="L23" s="39"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
+      <c r="A24" s="13" t="str">
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="50">
         <f>$C14+B$23*ABS($C14-$D14)/9</f>
         <v>-705.1</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="50">
         <f t="shared" ref="C24:K24" si="5">$C14+C$23*ABS($C14-$D14)/9</f>
         <v>-636.21111111111111</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="50">
         <f t="shared" si="5"/>
         <v>-567.32222222222231</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="50">
         <f t="shared" si="5"/>
         <v>-498.43333333333339</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="50">
         <f t="shared" si="5"/>
         <v>-429.54444444444448</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="50">
         <f t="shared" si="5"/>
         <v>-360.65555555555557</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="50">
         <f t="shared" si="5"/>
         <v>-291.76666666666671</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="50">
         <f t="shared" si="5"/>
         <v>-222.87777777777779</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="50">
         <f t="shared" si="5"/>
         <v>-153.98888888888894</v>
       </c>
-      <c r="K24" s="40">
+      <c r="K24" s="56">
         <f t="shared" si="5"/>
         <v>-85.100000000000023</v>
       </c>
-      <c r="L24" s="39"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
+      <c r="A25" s="13" t="str">
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="50">
         <f>$C15+B$23*ABS($C15-$D15)/9</f>
         <v>-225.1</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="50">
         <f t="shared" ref="C25:K25" si="6">$C15+C$23*ABS($C15-$D15)/9</f>
         <v>-209.54444444444445</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="50">
         <f t="shared" si="6"/>
         <v>-193.98888888888888</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="50">
         <f t="shared" si="6"/>
         <v>-178.43333333333334</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="50">
         <f t="shared" si="6"/>
         <v>-162.87777777777777</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="50">
         <f t="shared" si="6"/>
         <v>-147.32222222222222</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="50">
         <f t="shared" si="6"/>
         <v>-131.76666666666665</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="50">
         <f t="shared" si="6"/>
         <v>-116.21111111111111</v>
       </c>
-      <c r="J25" s="40">
+      <c r="J25" s="50">
         <f t="shared" si="6"/>
         <v>-100.65555555555555</v>
       </c>
-      <c r="K25" s="40">
+      <c r="K25" s="56">
         <f t="shared" si="6"/>
         <v>-85.1</v>
       </c>
-      <c r="L25" s="39"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
+      <c r="A26" s="13" t="str">
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="50">
         <f>$C16+B$23*ABS($C16-$D16)/9</f>
         <v>-465.1</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="50">
         <f>$C16+C$23*ABS($C16-$D16)/9</f>
         <v>-422.87777777777779</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="50">
         <f>$C16+D$23*ABS($C16-$D16)/9</f>
         <v>-380.65555555555557</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="50">
         <f>$C16+E$23*ABS($C16-$D16)/9</f>
         <v>-338.43333333333334</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="50">
         <f>$C16+F$23*ABS($C16-$D16)/9</f>
         <v>-296.21111111111111</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="50">
         <f>$C16+G$23*ABS($C16-$D16)/9</f>
         <v>-253.98888888888891</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="50">
         <f>$C16+H$23*ABS($C16-$D16)/9</f>
         <v>-211.76666666666668</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="50">
         <f>$C16+I$23*ABS($C16-$D16)/9</f>
         <v>-169.54444444444448</v>
       </c>
-      <c r="J26" s="40">
+      <c r="J26" s="50">
         <f>$C16+J$23*ABS($C16-$D16)/9</f>
         <v>-127.32222222222225</v>
       </c>
-      <c r="K26" s="40">
+      <c r="K26" s="56">
         <f>$C16+K$23*ABS($C16-$D16)/9</f>
         <v>-85.100000000000023</v>
       </c>
-      <c r="L26" s="39"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
+      <c r="A27" s="13" t="str">
         <f t="shared" ref="A27:A28" si="7">A17</f>
         <v>80MWe</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="50">
         <f>$C17+B$23*ABS($C17-$D17)/9</f>
         <v>-945.1</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="50">
         <f>$C17+C$23*ABS($C17-$D17)/9</f>
         <v>-849.54444444444448</v>
       </c>
-      <c r="D27" s="40">
+      <c r="D27" s="50">
         <f>$C17+D$23*ABS($C17-$D17)/9</f>
         <v>-753.98888888888894</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="50">
         <f>$C17+E$23*ABS($C17-$D17)/9</f>
         <v>-658.43333333333339</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="50">
         <f>$C17+F$23*ABS($C17-$D17)/9</f>
         <v>-562.87777777777774</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="50">
         <f>$C17+G$23*ABS($C17-$D17)/9</f>
         <v>-467.32222222222225</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="50">
         <f>$C17+H$23*ABS($C17-$D17)/9</f>
         <v>-371.76666666666665</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="50">
         <f>$C17+I$23*ABS($C17-$D17)/9</f>
         <v>-276.21111111111111</v>
       </c>
-      <c r="J27" s="40">
+      <c r="J27" s="50">
         <f>$C17+J$23*ABS($C17-$D17)/9</f>
         <v>-180.65555555555557</v>
       </c>
-      <c r="K27" s="40">
+      <c r="K27" s="56">
         <f>$C17+K$23*ABS($C17-$D17)/9</f>
         <v>-85.100000000000023</v>
       </c>
-      <c r="L27" s="39"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
+      <c r="L27" s="36"/>
+    </row>
+    <row r="28" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="str">
         <f t="shared" si="7"/>
         <v>100MWe</v>
       </c>
-      <c r="B28" s="40">
+      <c r="B28" s="57">
         <f t="shared" ref="B28:K28" si="8">$C18+B$23*ABS($C18-$D18)/9</f>
         <v>-985.1</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="57">
         <f t="shared" si="8"/>
         <v>-885.1</v>
       </c>
-      <c r="D28" s="40">
+      <c r="D28" s="57">
         <f t="shared" si="8"/>
         <v>-785.1</v>
       </c>
-      <c r="E28" s="40">
+      <c r="E28" s="57">
         <f t="shared" si="8"/>
         <v>-685.1</v>
       </c>
-      <c r="F28" s="40">
+      <c r="F28" s="57">
         <f t="shared" si="8"/>
         <v>-585.1</v>
       </c>
-      <c r="G28" s="40">
+      <c r="G28" s="57">
         <f t="shared" si="8"/>
         <v>-485.1</v>
       </c>
-      <c r="H28" s="40">
+      <c r="H28" s="57">
         <f t="shared" si="8"/>
         <v>-385.1</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="57">
         <f t="shared" si="8"/>
         <v>-285.10000000000002</v>
       </c>
-      <c r="J28" s="40">
+      <c r="J28" s="57">
         <f t="shared" si="8"/>
         <v>-185.10000000000002</v>
       </c>
-      <c r="K28" s="40">
+      <c r="K28" s="58">
         <f t="shared" si="8"/>
         <v>-85.100000000000023</v>
       </c>
-      <c r="L28" s="39"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="L28" s="36"/>
+    </row>
+    <row r="29" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+    </row>
+    <row r="30" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="36"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="54">
         <v>0</v>
       </c>
-      <c r="C31" s="39">
+      <c r="C31" s="54">
         <v>1</v>
       </c>
-      <c r="D31" s="39">
+      <c r="D31" s="54">
         <v>2</v>
       </c>
-      <c r="E31" s="39">
+      <c r="E31" s="54">
         <v>3</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="54">
         <v>4</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="54">
         <v>5</v>
       </c>
-      <c r="H31" s="39">
+      <c r="H31" s="54">
         <v>6</v>
       </c>
-      <c r="I31" s="39">
+      <c r="I31" s="54">
         <v>7</v>
       </c>
-      <c r="J31" s="39">
+      <c r="J31" s="54">
         <v>8</v>
       </c>
-      <c r="K31" s="39">
+      <c r="K31" s="55">
         <v>9</v>
       </c>
-      <c r="L31" s="39"/>
+      <c r="L31" s="36"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
+      <c r="A32" s="13" t="str">
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="50">
         <f>$E14+B$31*ABS($E14-$F14)/9</f>
         <v>-17719.163</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="50">
         <f>$E14+C$31*ABS($E14-$F14)/9</f>
         <v>-15987.985222222222</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="50">
         <f>$E14+D$31*ABS($E14-$F14)/9</f>
         <v>-14256.807444444445</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="50">
         <f>$E14+E$31*ABS($E14-$F14)/9</f>
         <v>-12525.629666666668</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="50">
         <f>$E14+F$31*ABS($E14-$F14)/9</f>
         <v>-10794.451888888889</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="50">
         <f>$E14+G$31*ABS($E14-$F14)/9</f>
         <v>-9063.2741111111118</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="50">
         <f>$E14+H$31*ABS($E14-$F14)/9</f>
         <v>-7332.096333333333</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="50">
         <f>$E14+I$31*ABS($E14-$F14)/9</f>
         <v>-5600.9185555555559</v>
       </c>
-      <c r="J32" s="40">
+      <c r="J32" s="50">
         <f>$E14+J$31*ABS($E14-$F14)/9</f>
         <v>-3869.7407777777771</v>
       </c>
-      <c r="K32" s="40">
+      <c r="K32" s="56">
         <f>$E14+K$31*ABS($E14-$F14)/9</f>
         <v>-2138.5630000000019</v>
       </c>
-      <c r="L32" s="39"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
+      <c r="L32" s="36"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="str">
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="B33" s="40">
+      <c r="B33" s="50">
         <f>$E15+B$31*ABS($E15-$F15)/9</f>
         <v>-5656.7629999999999</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="50">
         <f>$E15+C$31*ABS($E15-$F15)/9</f>
         <v>-5265.8518888888884</v>
       </c>
-      <c r="D33" s="40">
+      <c r="D33" s="50">
         <f>$E15+D$31*ABS($E15-$F15)/9</f>
         <v>-4874.9407777777778</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="50">
         <f>$E15+E$31*ABS($E15-$F15)/9</f>
         <v>-4484.0296666666663</v>
       </c>
-      <c r="F33" s="40">
+      <c r="F33" s="50">
         <f>$E15+F$31*ABS($E15-$F15)/9</f>
         <v>-4093.1185555555553</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G33" s="50">
         <f>$E15+G$31*ABS($E15-$F15)/9</f>
         <v>-3702.2074444444443</v>
       </c>
-      <c r="H33" s="40">
+      <c r="H33" s="50">
         <f>$E15+H$31*ABS($E15-$F15)/9</f>
         <v>-3311.2963333333332</v>
       </c>
-      <c r="I33" s="40">
+      <c r="I33" s="50">
         <f>$E15+I$31*ABS($E15-$F15)/9</f>
         <v>-2920.3852222222222</v>
       </c>
-      <c r="J33" s="40">
+      <c r="J33" s="50">
         <f>$E15+J$31*ABS($E15-$F15)/9</f>
         <v>-2529.4741111111107</v>
       </c>
-      <c r="K33" s="40">
+      <c r="K33" s="56">
         <f>$E15+K$31*ABS($E15-$F15)/9</f>
         <v>-2138.5629999999996</v>
       </c>
-      <c r="L33" s="40"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
+      <c r="L33" s="37"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="str">
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="B34" s="40">
+      <c r="B34" s="50">
         <f>$E16+B$31*ABS($E16-$F16)/9</f>
         <v>-11687.963</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="50">
         <f>$E16+C$31*ABS($E16-$F16)/9</f>
         <v>-10626.918555555556</v>
       </c>
-      <c r="D34" s="40">
+      <c r="D34" s="50">
         <f>$E16+D$31*ABS($E16-$F16)/9</f>
         <v>-9565.8741111111103</v>
       </c>
-      <c r="E34" s="40">
+      <c r="E34" s="50">
         <f>$E16+E$31*ABS($E16-$F16)/9</f>
         <v>-8504.8296666666665</v>
       </c>
-      <c r="F34" s="40">
+      <c r="F34" s="50">
         <f>$E16+F$31*ABS($E16-$F16)/9</f>
         <v>-7443.7852222222218</v>
       </c>
-      <c r="G34" s="40">
+      <c r="G34" s="50">
         <f>$E16+G$31*ABS($E16-$F16)/9</f>
         <v>-6382.7407777777771</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H34" s="50">
         <f>$E16+H$31*ABS($E16-$F16)/9</f>
         <v>-5321.6963333333333</v>
       </c>
-      <c r="I34" s="40">
+      <c r="I34" s="50">
         <f>$E16+I$31*ABS($E16-$F16)/9</f>
         <v>-4260.6518888888886</v>
       </c>
-      <c r="J34" s="40">
+      <c r="J34" s="50">
         <f>$E16+J$31*ABS($E16-$F16)/9</f>
         <v>-3199.6074444444439</v>
       </c>
-      <c r="K34" s="40">
+      <c r="K34" s="56">
         <f>$E16+K$31*ABS($E16-$F16)/9</f>
         <v>-2138.5630000000001</v>
       </c>
-      <c r="L34" s="39"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
+      <c r="L34" s="36"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="str">
         <f t="shared" ref="A35:A36" si="9">A17</f>
         <v>80MWe</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="50">
         <f t="shared" ref="B35:K35" si="10">$E17+B$31*ABS($E17-$F17)/9</f>
         <v>-23750.363000000001</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="50">
         <f t="shared" si="10"/>
         <v>-21349.051888888891</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="50">
         <f t="shared" si="10"/>
         <v>-18947.740777777777</v>
       </c>
-      <c r="E35" s="40">
+      <c r="E35" s="50">
         <f t="shared" si="10"/>
         <v>-16546.429666666667</v>
       </c>
-      <c r="F35" s="40">
+      <c r="F35" s="50">
         <f t="shared" si="10"/>
         <v>-14145.118555555555</v>
       </c>
-      <c r="G35" s="40">
+      <c r="G35" s="50">
         <f t="shared" si="10"/>
         <v>-11743.807444444445</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="50">
         <f t="shared" si="10"/>
         <v>-9342.4963333333326</v>
       </c>
-      <c r="I35" s="40">
+      <c r="I35" s="50">
         <f t="shared" si="10"/>
         <v>-6941.1852222222187</v>
       </c>
-      <c r="J35" s="40">
+      <c r="J35" s="50">
         <f t="shared" si="10"/>
         <v>-4539.8741111111085</v>
       </c>
-      <c r="K35" s="40">
+      <c r="K35" s="56">
         <f t="shared" si="10"/>
         <v>-2138.5629999999983</v>
       </c>
-      <c r="L35" s="39"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
+      <c r="L35" s="36"/>
+    </row>
+    <row r="36" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="str">
         <f t="shared" si="9"/>
         <v>100MWe</v>
       </c>
-      <c r="B36" s="40">
+      <c r="B36" s="57">
         <f t="shared" ref="B36:K36" si="11">$E18+B$31*ABS($E18-$F18)/9</f>
         <v>-24755.562999999998</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C36" s="57">
         <f t="shared" si="11"/>
         <v>-22242.562999999998</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36" s="57">
         <f t="shared" si="11"/>
         <v>-19729.562999999998</v>
       </c>
-      <c r="E36" s="40">
+      <c r="E36" s="57">
         <f t="shared" si="11"/>
         <v>-17216.562999999998</v>
       </c>
-      <c r="F36" s="40">
+      <c r="F36" s="57">
         <f t="shared" si="11"/>
         <v>-14703.562999999998</v>
       </c>
-      <c r="G36" s="40">
+      <c r="G36" s="57">
         <f t="shared" si="11"/>
         <v>-12190.562999999998</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="57">
         <f t="shared" si="11"/>
         <v>-9677.5629999999983</v>
       </c>
-      <c r="I36" s="40">
+      <c r="I36" s="57">
         <f t="shared" si="11"/>
         <v>-7164.5629999999983</v>
       </c>
-      <c r="J36" s="40">
+      <c r="J36" s="57">
         <f t="shared" si="11"/>
         <v>-4651.5629999999983</v>
       </c>
-      <c r="K36" s="40">
+      <c r="K36" s="58">
         <f t="shared" si="11"/>
         <v>-2138.5629999999983</v>
       </c>
-      <c r="L36" s="39"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="39"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="L36" s="36"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="36"/>
+    </row>
+    <row r="38" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="67" t="s">
         <v>198</v>
       </c>
-      <c r="D39" t="str">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="49" t="str">
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="F39" t="str">
+      <c r="E39" s="48"/>
+      <c r="F39" s="49" t="str">
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="H39" t="str">
+      <c r="G39" s="48"/>
+      <c r="H39" s="49" t="str">
         <f>A16</f>
         <v>40MWe</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="I39" s="48"/>
+      <c r="J39" s="49" t="str">
+        <f>A35</f>
+        <v>80MWe</v>
+      </c>
+      <c r="K39" s="48"/>
+      <c r="L39" s="47" t="str">
+        <f>A36</f>
+        <v>100MWe</v>
+      </c>
+      <c r="M39" s="48"/>
+    </row>
+    <row r="40" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="17" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="J40" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="35">
+      <c r="B41" s="44">
         <f t="shared" ref="B41:B43" si="12">ROUNDUP(C41*$B$45/$C$45,0)</f>
         <v>2</v>
       </c>
-      <c r="C41" s="35">
+      <c r="C41" s="44">
         <v>934</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="45">
         <v>0</v>
       </c>
-      <c r="E41" s="34">
+      <c r="E41" s="40">
         <f>ABS($E$14)*24*B41</f>
         <v>850519.82400000002</v>
       </c>
-      <c r="F41" s="34">
+      <c r="F41" s="40">
         <v>0</v>
       </c>
-      <c r="G41" s="34">
+      <c r="G41" s="40">
         <f>ABS($E$15)*24*$B41</f>
         <v>271524.62400000001</v>
       </c>
-      <c r="H41" s="34">
+      <c r="H41" s="40">
         <v>0</v>
       </c>
-      <c r="I41" s="34">
+      <c r="I41" s="40">
         <f>ABS($E$16)*24*$B41</f>
         <v>561022.22399999993</v>
       </c>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="J41" s="40">
+        <v>0</v>
+      </c>
+      <c r="K41" s="40">
+        <f>ABS($E$17)*24*$B41</f>
+        <v>1140017.4240000001</v>
+      </c>
+      <c r="L41" s="45">
+        <v>0</v>
+      </c>
+      <c r="M41" s="41">
+        <f>ABS($E$18*24*$B41)</f>
+        <v>1188267.024</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="35">
+      <c r="B42" s="44">
         <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="C42" s="35">
+      <c r="C42" s="44">
         <v>4231</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="45">
         <v>0</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="40">
         <f>ABS($E$14)*24*B42</f>
         <v>2976819.3840000001</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="40">
         <v>0</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="40">
         <f t="shared" ref="G42:G45" si="13">ABS($E$15)*24*$B42</f>
         <v>950336.18400000001</v>
       </c>
-      <c r="H42" s="34">
+      <c r="H42" s="40">
         <v>0</v>
       </c>
-      <c r="I42" s="34">
+      <c r="I42" s="40">
         <f t="shared" ref="I42:I45" si="14">ABS($E$16)*24*$B42</f>
         <v>1963577.7839999998</v>
       </c>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="J42" s="40">
+        <v>0</v>
+      </c>
+      <c r="K42" s="40">
+        <f t="shared" ref="K42:K45" si="15">ABS($E$17)*24*$B42</f>
+        <v>3990060.9840000002</v>
+      </c>
+      <c r="L42" s="45">
+        <v>0</v>
+      </c>
+      <c r="M42" s="41">
+        <f t="shared" ref="M42:M45" si="16">ABS($E$18*24*$B42)</f>
+        <v>4158934.5839999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B43" s="35">
+      <c r="B43" s="44">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="C43" s="35">
+      <c r="C43" s="44">
         <v>934</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="45">
         <v>0</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="40">
         <f>ABS($E$14)*24*B43</f>
         <v>850519.82400000002</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="40">
         <v>0</v>
       </c>
-      <c r="G43" s="34">
+      <c r="G43" s="40">
         <f t="shared" si="13"/>
         <v>271524.62400000001</v>
       </c>
-      <c r="H43" s="34">
+      <c r="H43" s="40">
         <v>0</v>
       </c>
-      <c r="I43" s="34">
+      <c r="I43" s="40">
         <f t="shared" si="14"/>
         <v>561022.22399999993</v>
       </c>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="J43" s="40">
+        <v>0</v>
+      </c>
+      <c r="K43" s="40">
+        <f t="shared" si="15"/>
+        <v>1140017.4240000001</v>
+      </c>
+      <c r="L43" s="45">
+        <v>0</v>
+      </c>
+      <c r="M43" s="41">
+        <f t="shared" si="16"/>
+        <v>1188267.024</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="B44" s="35">
+      <c r="B44" s="44">
         <f>ROUNDUP(C44*$B$45/$C$45,0)</f>
         <v>1</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="44">
         <v>97</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="45">
         <v>0</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E44" s="40">
         <f>ABS($E$14)*24*B44</f>
         <v>425259.91200000001</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44" s="40">
         <v>0</v>
       </c>
-      <c r="G44" s="34">
+      <c r="G44" s="40">
         <f t="shared" si="13"/>
         <v>135762.31200000001</v>
       </c>
-      <c r="H44" s="34">
+      <c r="H44" s="40">
         <v>0</v>
       </c>
-      <c r="I44" s="34">
+      <c r="I44" s="40">
         <f t="shared" si="14"/>
         <v>280511.11199999996</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="J44" s="40">
+        <v>0</v>
+      </c>
+      <c r="K44" s="40">
+        <f t="shared" si="15"/>
+        <v>570008.71200000006</v>
+      </c>
+      <c r="L44" s="45">
+        <v>0</v>
+      </c>
+      <c r="M44" s="41">
+        <f t="shared" si="16"/>
+        <v>594133.51199999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="35">
+      <c r="B45" s="46">
         <v>14</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="46">
         <v>8997</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="24">
         <v>0</v>
       </c>
-      <c r="E45" s="34">
+      <c r="E45" s="42">
         <f>ABS($E$14)*24*B45</f>
         <v>5953638.7680000002</v>
       </c>
-      <c r="F45" s="34">
+      <c r="F45" s="42">
         <v>0</v>
       </c>
-      <c r="G45" s="34">
+      <c r="G45" s="42">
         <f t="shared" si="13"/>
         <v>1900672.368</v>
       </c>
-      <c r="H45" s="34">
+      <c r="H45" s="42">
         <v>0</v>
       </c>
-      <c r="I45" s="34">
+      <c r="I45" s="42">
         <f t="shared" si="14"/>
         <v>3927155.5679999995</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>195</v>
-      </c>
-      <c r="B47">
+      <c r="J45" s="42">
         <v>0</v>
       </c>
-      <c r="C47" s="35">
+      <c r="K45" s="42">
+        <f t="shared" si="15"/>
+        <v>7980121.9680000003</v>
+      </c>
+      <c r="L45" s="24">
+        <v>0</v>
+      </c>
+      <c r="M45" s="43">
+        <f t="shared" si="16"/>
+        <v>8317869.1679999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="B47" s="30">
+        <v>0</v>
+      </c>
+      <c r="C47" s="38">
         <v>1</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="30">
         <v>2</v>
       </c>
-      <c r="E47" s="35">
+      <c r="E47" s="38">
         <v>3</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="30">
         <v>4</v>
       </c>
-      <c r="G47" s="35">
+      <c r="G47" s="38">
         <v>5</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="30">
         <v>6</v>
       </c>
-      <c r="I47" s="35">
+      <c r="I47" s="38">
         <v>7</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="30">
         <v>8</v>
       </c>
-      <c r="K47" s="35">
+      <c r="K47" s="39">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="str">
         <f>A41</f>
         <v>illinois</v>
       </c>
-      <c r="B48" s="34">
+      <c r="B48" s="40">
         <f>$D41+B$47*ABS($E41-$D41)/9</f>
         <v>0</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="40">
         <f>$D41+C$47*ABS($E41-$D41)/9</f>
         <v>94502.202666666664</v>
       </c>
-      <c r="D48" s="34">
-        <f t="shared" ref="C48:K48" si="15">$D41+D$47*ABS($E41-$D41)/9</f>
+      <c r="D48" s="40">
+        <f t="shared" ref="C48:K48" si="17">$D41+D$47*ABS($E41-$D41)/9</f>
         <v>189004.40533333333</v>
       </c>
-      <c r="E48" s="34">
-        <f t="shared" si="15"/>
+      <c r="E48" s="40">
+        <f t="shared" si="17"/>
         <v>283506.60800000001</v>
       </c>
-      <c r="F48" s="34">
-        <f t="shared" si="15"/>
+      <c r="F48" s="40">
+        <f t="shared" si="17"/>
         <v>378008.81066666666</v>
       </c>
-      <c r="G48" s="34">
-        <f t="shared" si="15"/>
+      <c r="G48" s="40">
+        <f t="shared" si="17"/>
         <v>472511.01333333337</v>
       </c>
-      <c r="H48" s="34">
-        <f t="shared" si="15"/>
+      <c r="H48" s="40">
+        <f t="shared" si="17"/>
         <v>567013.21600000001</v>
       </c>
-      <c r="I48" s="34">
-        <f t="shared" si="15"/>
-        <v>661515.41866666672</v>
-      </c>
-      <c r="J48" s="34">
-        <f t="shared" si="15"/>
-        <v>756017.62133333331</v>
-      </c>
-      <c r="K48" s="34">
-        <f t="shared" si="15"/>
-        <v>850519.82400000002</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f t="shared" ref="A49:A52" si="16">A42</f>
-        <v>nebraska</v>
-      </c>
-      <c r="B49" s="34">
-        <f t="shared" ref="B49:K52" si="17">$D42+B$47*ABS($E42-$D42)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="34">
-        <f t="shared" si="17"/>
-        <v>330757.70933333336</v>
-      </c>
-      <c r="D49" s="34">
+      <c r="I48" s="40">
         <f t="shared" si="17"/>
         <v>661515.41866666672</v>
       </c>
-      <c r="E49" s="34">
-        <f t="shared" si="17"/>
-        <v>992273.12800000003</v>
-      </c>
-      <c r="F49" s="34">
-        <f t="shared" si="17"/>
-        <v>1323030.8373333334</v>
-      </c>
-      <c r="G49" s="34">
-        <f t="shared" si="17"/>
-        <v>1653788.5466666666</v>
-      </c>
-      <c r="H49" s="34">
-        <f t="shared" si="17"/>
-        <v>1984546.2560000001</v>
-      </c>
-      <c r="I49" s="34">
-        <f t="shared" si="17"/>
-        <v>2315303.9653333332</v>
-      </c>
-      <c r="J49" s="34">
-        <f t="shared" si="17"/>
-        <v>2646061.6746666669</v>
-      </c>
-      <c r="K49" s="34">
-        <f t="shared" si="17"/>
-        <v>2976819.3840000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="16"/>
-        <v>ohio</v>
-      </c>
-      <c r="B50" s="34">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="C50" s="34">
-        <f t="shared" si="17"/>
-        <v>94502.202666666664</v>
-      </c>
-      <c r="D50" s="34">
-        <f t="shared" si="17"/>
-        <v>189004.40533333333</v>
-      </c>
-      <c r="E50" s="34">
-        <f t="shared" si="17"/>
-        <v>283506.60800000001</v>
-      </c>
-      <c r="F50" s="34">
-        <f t="shared" si="17"/>
-        <v>378008.81066666666</v>
-      </c>
-      <c r="G50" s="34">
-        <f t="shared" si="17"/>
-        <v>472511.01333333337</v>
-      </c>
-      <c r="H50" s="34">
-        <f t="shared" si="17"/>
-        <v>567013.21600000001</v>
-      </c>
-      <c r="I50" s="34">
-        <f t="shared" si="17"/>
-        <v>661515.41866666672</v>
-      </c>
-      <c r="J50" s="34">
+      <c r="J48" s="40">
         <f t="shared" si="17"/>
         <v>756017.62133333331</v>
       </c>
-      <c r="K50" s="34">
+      <c r="K48" s="41">
         <f t="shared" si="17"/>
         <v>850519.82400000002</v>
       </c>
     </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="str">
+        <f t="shared" ref="A49:A52" si="18">A42</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B49" s="40">
+        <f t="shared" ref="B49:K52" si="19">$D42+B$47*ABS($E42-$D42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="40">
+        <f t="shared" si="19"/>
+        <v>330757.70933333336</v>
+      </c>
+      <c r="D49" s="40">
+        <f t="shared" si="19"/>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="E49" s="40">
+        <f t="shared" si="19"/>
+        <v>992273.12800000003</v>
+      </c>
+      <c r="F49" s="40">
+        <f t="shared" si="19"/>
+        <v>1323030.8373333334</v>
+      </c>
+      <c r="G49" s="40">
+        <f t="shared" si="19"/>
+        <v>1653788.5466666666</v>
+      </c>
+      <c r="H49" s="40">
+        <f t="shared" si="19"/>
+        <v>1984546.2560000001</v>
+      </c>
+      <c r="I49" s="40">
+        <f t="shared" si="19"/>
+        <v>2315303.9653333332</v>
+      </c>
+      <c r="J49" s="40">
+        <f t="shared" si="19"/>
+        <v>2646061.6746666669</v>
+      </c>
+      <c r="K49" s="41">
+        <f t="shared" si="19"/>
+        <v>2976819.3840000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="str">
+        <f t="shared" si="18"/>
+        <v>ohio</v>
+      </c>
+      <c r="B50" s="40">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="C50" s="40">
+        <f t="shared" si="19"/>
+        <v>94502.202666666664</v>
+      </c>
+      <c r="D50" s="40">
+        <f t="shared" si="19"/>
+        <v>189004.40533333333</v>
+      </c>
+      <c r="E50" s="40">
+        <f t="shared" si="19"/>
+        <v>283506.60800000001</v>
+      </c>
+      <c r="F50" s="40">
+        <f t="shared" si="19"/>
+        <v>378008.81066666666</v>
+      </c>
+      <c r="G50" s="40">
+        <f t="shared" si="19"/>
+        <v>472511.01333333337</v>
+      </c>
+      <c r="H50" s="40">
+        <f t="shared" si="19"/>
+        <v>567013.21600000001</v>
+      </c>
+      <c r="I50" s="40">
+        <f t="shared" si="19"/>
+        <v>661515.41866666672</v>
+      </c>
+      <c r="J50" s="40">
+        <f t="shared" si="19"/>
+        <v>756017.62133333331</v>
+      </c>
+      <c r="K50" s="41">
+        <f t="shared" si="19"/>
+        <v>850519.82400000002</v>
+      </c>
+    </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="str">
-        <f t="shared" si="16"/>
+      <c r="A51" s="13" t="str">
+        <f t="shared" si="18"/>
         <v>minnesota</v>
       </c>
-      <c r="B51" s="34">
+      <c r="B51" s="40">
         <f>$D44+B$47*ABS($E44-$D44)/9</f>
         <v>0</v>
       </c>
-      <c r="C51" s="34">
-        <f t="shared" si="17"/>
+      <c r="C51" s="40">
+        <f t="shared" si="19"/>
         <v>47251.101333333332</v>
       </c>
-      <c r="D51" s="34">
-        <f t="shared" si="17"/>
+      <c r="D51" s="40">
+        <f t="shared" si="19"/>
         <v>94502.202666666664</v>
       </c>
-      <c r="E51" s="34">
-        <f t="shared" si="17"/>
+      <c r="E51" s="40">
+        <f t="shared" si="19"/>
         <v>141753.304</v>
       </c>
-      <c r="F51" s="34">
-        <f t="shared" si="17"/>
+      <c r="F51" s="40">
+        <f t="shared" si="19"/>
         <v>189004.40533333333</v>
       </c>
-      <c r="G51" s="34">
-        <f t="shared" si="17"/>
+      <c r="G51" s="40">
+        <f t="shared" si="19"/>
         <v>236255.50666666668</v>
       </c>
-      <c r="H51" s="34">
-        <f t="shared" si="17"/>
+      <c r="H51" s="40">
+        <f t="shared" si="19"/>
         <v>283506.60800000001</v>
       </c>
-      <c r="I51" s="34">
-        <f t="shared" si="17"/>
+      <c r="I51" s="40">
+        <f t="shared" si="19"/>
         <v>330757.70933333336</v>
       </c>
-      <c r="J51" s="34">
-        <f t="shared" si="17"/>
+      <c r="J51" s="40">
+        <f t="shared" si="19"/>
         <v>378008.81066666666</v>
       </c>
-      <c r="K51" s="34">
-        <f t="shared" si="17"/>
+      <c r="K51" s="41">
+        <f t="shared" si="19"/>
         <v>425259.91200000001</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f t="shared" si="16"/>
+    <row r="52" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="str">
+        <f t="shared" si="18"/>
         <v>texas</v>
       </c>
-      <c r="B52" s="34">
-        <f t="shared" si="17"/>
+      <c r="B52" s="42">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52" s="42">
         <f>$D45+C$47*ABS($E45-$D45)/9</f>
         <v>661515.41866666672</v>
       </c>
-      <c r="D52" s="34">
-        <f t="shared" si="17"/>
+      <c r="D52" s="42">
+        <f t="shared" si="19"/>
         <v>1323030.8373333334</v>
       </c>
-      <c r="E52" s="34">
-        <f t="shared" si="17"/>
+      <c r="E52" s="42">
+        <f t="shared" si="19"/>
         <v>1984546.2560000001</v>
       </c>
-      <c r="F52" s="34">
-        <f t="shared" si="17"/>
+      <c r="F52" s="42">
+        <f t="shared" si="19"/>
         <v>2646061.6746666669</v>
       </c>
-      <c r="G52" s="34">
-        <f t="shared" si="17"/>
+      <c r="G52" s="42">
+        <f t="shared" si="19"/>
         <v>3307577.0933333333</v>
       </c>
-      <c r="H52" s="34">
-        <f t="shared" si="17"/>
+      <c r="H52" s="42">
+        <f t="shared" si="19"/>
         <v>3969092.5120000001</v>
       </c>
-      <c r="I52" s="34">
-        <f t="shared" si="17"/>
+      <c r="I52" s="42">
+        <f t="shared" si="19"/>
         <v>4630607.9306666665</v>
       </c>
-      <c r="J52" s="34">
-        <f t="shared" si="17"/>
+      <c r="J52" s="42">
+        <f t="shared" si="19"/>
         <v>5292123.3493333338</v>
       </c>
-      <c r="K52" s="34">
-        <f t="shared" si="17"/>
+      <c r="K52" s="43">
+        <f t="shared" si="19"/>
         <v>5953638.7680000002</v>
       </c>
     </row>
+    <row r="53" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54">
+      <c r="A54" s="63" t="str">
+        <f>F39</f>
+        <v>20MWe</v>
+      </c>
+      <c r="B54" s="30">
         <v>0</v>
       </c>
-      <c r="C54" s="35">
+      <c r="C54" s="38">
         <v>1</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="30">
         <v>2</v>
       </c>
-      <c r="E54" s="35">
+      <c r="E54" s="38">
         <v>3</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="30">
         <v>4</v>
       </c>
-      <c r="G54" s="35">
+      <c r="G54" s="38">
         <v>5</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="30">
         <v>6</v>
       </c>
-      <c r="I54" s="35">
+      <c r="I54" s="38">
         <v>7</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="30">
         <v>8</v>
       </c>
-      <c r="K54" s="35">
+      <c r="K54" s="39">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" t="str">
+      <c r="A55" s="13" t="str">
         <f>A48</f>
         <v>illinois</v>
       </c>
-      <c r="B55" s="34">
+      <c r="B55" s="40">
         <f>$F41+B$47*ABS($G41-$F41)/9</f>
         <v>0</v>
       </c>
-      <c r="C55" s="34">
-        <f t="shared" ref="C55:K55" si="18">$F41+C$47*ABS($G41-$F41)/9</f>
+      <c r="C55" s="40">
+        <f>$F41+C$47*ABS($G41-$F41)/9</f>
         <v>30169.402666666669</v>
       </c>
-      <c r="D55" s="34">
-        <f t="shared" si="18"/>
+      <c r="D55" s="40">
+        <f t="shared" ref="C55:K55" si="20">$F41+D$47*ABS($G41-$F41)/9</f>
         <v>60338.805333333337</v>
       </c>
-      <c r="E55" s="34">
-        <f t="shared" si="18"/>
+      <c r="E55" s="40">
+        <f t="shared" si="20"/>
         <v>90508.207999999999</v>
       </c>
-      <c r="F55" s="34">
-        <f t="shared" si="18"/>
+      <c r="F55" s="40">
+        <f t="shared" si="20"/>
         <v>120677.61066666667</v>
       </c>
-      <c r="G55" s="34">
-        <f t="shared" si="18"/>
+      <c r="G55" s="40">
+        <f t="shared" si="20"/>
         <v>150847.01333333334</v>
       </c>
-      <c r="H55" s="34">
-        <f t="shared" si="18"/>
+      <c r="H55" s="40">
+        <f t="shared" si="20"/>
         <v>181016.416</v>
       </c>
-      <c r="I55" s="34">
-        <f t="shared" si="18"/>
-        <v>211185.81866666666</v>
-      </c>
-      <c r="J55" s="34">
-        <f t="shared" si="18"/>
-        <v>241355.22133333335</v>
-      </c>
-      <c r="K55" s="34">
-        <f t="shared" si="18"/>
-        <v>271524.62400000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f t="shared" ref="A56:A59" si="19">A49</f>
-        <v>nebraska</v>
-      </c>
-      <c r="B56" s="34">
-        <f t="shared" ref="B56:K59" si="20">$F42+B$47*ABS($G42-$F42)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="34">
-        <f t="shared" si="20"/>
-        <v>105592.90933333333</v>
-      </c>
-      <c r="D56" s="34">
+      <c r="I55" s="40">
         <f t="shared" si="20"/>
         <v>211185.81866666666</v>
       </c>
-      <c r="E56" s="34">
-        <f t="shared" si="20"/>
-        <v>316778.728</v>
-      </c>
-      <c r="F56" s="34">
-        <f t="shared" si="20"/>
-        <v>422371.63733333332</v>
-      </c>
-      <c r="G56" s="34">
-        <f t="shared" si="20"/>
-        <v>527964.54666666663</v>
-      </c>
-      <c r="H56" s="34">
-        <f t="shared" si="20"/>
-        <v>633557.45600000001</v>
-      </c>
-      <c r="I56" s="34">
-        <f t="shared" si="20"/>
-        <v>739150.36533333326</v>
-      </c>
-      <c r="J56" s="34">
-        <f t="shared" si="20"/>
-        <v>844743.27466666664</v>
-      </c>
-      <c r="K56" s="34">
-        <f t="shared" si="20"/>
-        <v>950336.18399999989</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" t="str">
-        <f t="shared" si="19"/>
-        <v>ohio</v>
-      </c>
-      <c r="B57" s="34">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="C57" s="34">
-        <f t="shared" si="20"/>
-        <v>30169.402666666669</v>
-      </c>
-      <c r="D57" s="34">
-        <f t="shared" si="20"/>
-        <v>60338.805333333337</v>
-      </c>
-      <c r="E57" s="34">
-        <f t="shared" si="20"/>
-        <v>90508.207999999999</v>
-      </c>
-      <c r="F57" s="34">
-        <f t="shared" si="20"/>
-        <v>120677.61066666667</v>
-      </c>
-      <c r="G57" s="34">
-        <f t="shared" si="20"/>
-        <v>150847.01333333334</v>
-      </c>
-      <c r="H57" s="34">
-        <f t="shared" si="20"/>
-        <v>181016.416</v>
-      </c>
-      <c r="I57" s="34">
-        <f t="shared" si="20"/>
-        <v>211185.81866666666</v>
-      </c>
-      <c r="J57" s="34">
+      <c r="J55" s="40">
         <f t="shared" si="20"/>
         <v>241355.22133333335</v>
       </c>
-      <c r="K57" s="34">
+      <c r="K55" s="41">
         <f t="shared" si="20"/>
         <v>271524.62400000001</v>
       </c>
     </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="str">
+        <f t="shared" ref="A56:A59" si="21">A49</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B56" s="40">
+        <f t="shared" ref="B56:K59" si="22">$F42+B$47*ABS($G42-$F42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="40">
+        <f t="shared" si="22"/>
+        <v>105592.90933333333</v>
+      </c>
+      <c r="D56" s="40">
+        <f t="shared" si="22"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="E56" s="40">
+        <f t="shared" si="22"/>
+        <v>316778.728</v>
+      </c>
+      <c r="F56" s="40">
+        <f t="shared" si="22"/>
+        <v>422371.63733333332</v>
+      </c>
+      <c r="G56" s="40">
+        <f t="shared" si="22"/>
+        <v>527964.54666666663</v>
+      </c>
+      <c r="H56" s="40">
+        <f t="shared" si="22"/>
+        <v>633557.45600000001</v>
+      </c>
+      <c r="I56" s="40">
+        <f t="shared" si="22"/>
+        <v>739150.36533333326</v>
+      </c>
+      <c r="J56" s="40">
+        <f t="shared" si="22"/>
+        <v>844743.27466666664</v>
+      </c>
+      <c r="K56" s="41">
+        <f t="shared" si="22"/>
+        <v>950336.18399999989</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="str">
+        <f t="shared" si="21"/>
+        <v>ohio</v>
+      </c>
+      <c r="B57" s="40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="C57" s="40">
+        <f t="shared" si="22"/>
+        <v>30169.402666666669</v>
+      </c>
+      <c r="D57" s="40">
+        <f t="shared" si="22"/>
+        <v>60338.805333333337</v>
+      </c>
+      <c r="E57" s="40">
+        <f t="shared" si="22"/>
+        <v>90508.207999999999</v>
+      </c>
+      <c r="F57" s="40">
+        <f t="shared" si="22"/>
+        <v>120677.61066666667</v>
+      </c>
+      <c r="G57" s="40">
+        <f t="shared" si="22"/>
+        <v>150847.01333333334</v>
+      </c>
+      <c r="H57" s="40">
+        <f t="shared" si="22"/>
+        <v>181016.416</v>
+      </c>
+      <c r="I57" s="40">
+        <f t="shared" si="22"/>
+        <v>211185.81866666666</v>
+      </c>
+      <c r="J57" s="40">
+        <f t="shared" si="22"/>
+        <v>241355.22133333335</v>
+      </c>
+      <c r="K57" s="41">
+        <f t="shared" si="22"/>
+        <v>271524.62400000001</v>
+      </c>
+    </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" t="str">
-        <f t="shared" si="19"/>
+      <c r="A58" s="13" t="str">
+        <f t="shared" si="21"/>
         <v>minnesota</v>
       </c>
-      <c r="B58" s="34">
-        <f t="shared" si="20"/>
+      <c r="B58" s="40">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="C58" s="34">
-        <f t="shared" si="20"/>
+      <c r="C58" s="40">
+        <f>$F44+C$47*ABS($G44-$F44)/9</f>
         <v>15084.701333333334</v>
       </c>
-      <c r="D58" s="34">
-        <f t="shared" si="20"/>
+      <c r="D58" s="40">
+        <f t="shared" si="22"/>
         <v>30169.402666666669</v>
       </c>
-      <c r="E58" s="34">
-        <f t="shared" si="20"/>
+      <c r="E58" s="40">
+        <f t="shared" si="22"/>
         <v>45254.103999999999</v>
       </c>
-      <c r="F58" s="34">
-        <f t="shared" si="20"/>
+      <c r="F58" s="40">
+        <f t="shared" si="22"/>
         <v>60338.805333333337</v>
       </c>
-      <c r="G58" s="34">
-        <f t="shared" si="20"/>
+      <c r="G58" s="40">
+        <f t="shared" si="22"/>
         <v>75423.506666666668</v>
       </c>
-      <c r="H58" s="34">
-        <f t="shared" si="20"/>
+      <c r="H58" s="40">
+        <f t="shared" si="22"/>
         <v>90508.207999999999</v>
       </c>
-      <c r="I58" s="34">
-        <f t="shared" si="20"/>
+      <c r="I58" s="40">
+        <f t="shared" si="22"/>
         <v>105592.90933333333</v>
       </c>
-      <c r="J58" s="34">
-        <f t="shared" si="20"/>
+      <c r="J58" s="40">
+        <f t="shared" si="22"/>
         <v>120677.61066666667</v>
       </c>
-      <c r="K58" s="34">
-        <f t="shared" si="20"/>
+      <c r="K58" s="41">
+        <f t="shared" si="22"/>
         <v>135762.31200000001</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" t="str">
-        <f t="shared" si="19"/>
+    <row r="59" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="str">
+        <f t="shared" si="21"/>
         <v>texas</v>
       </c>
-      <c r="B59" s="34">
-        <f t="shared" si="20"/>
+      <c r="B59" s="42">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="C59" s="34">
-        <f t="shared" si="20"/>
+      <c r="C59" s="42">
+        <f t="shared" si="22"/>
         <v>211185.81866666666</v>
       </c>
-      <c r="D59" s="34">
-        <f t="shared" si="20"/>
+      <c r="D59" s="42">
+        <f t="shared" si="22"/>
         <v>422371.63733333332</v>
       </c>
-      <c r="E59" s="34">
-        <f t="shared" si="20"/>
+      <c r="E59" s="42">
+        <f t="shared" si="22"/>
         <v>633557.45600000001</v>
       </c>
-      <c r="F59" s="34">
-        <f t="shared" si="20"/>
+      <c r="F59" s="42">
+        <f t="shared" si="22"/>
         <v>844743.27466666664</v>
       </c>
-      <c r="G59" s="34">
-        <f t="shared" si="20"/>
+      <c r="G59" s="42">
+        <f t="shared" si="22"/>
         <v>1055929.0933333333</v>
       </c>
-      <c r="H59" s="34">
-        <f t="shared" si="20"/>
+      <c r="H59" s="42">
+        <f t="shared" si="22"/>
         <v>1267114.912</v>
       </c>
-      <c r="I59" s="34">
-        <f t="shared" si="20"/>
+      <c r="I59" s="42">
+        <f t="shared" si="22"/>
         <v>1478300.7306666665</v>
       </c>
-      <c r="J59" s="34">
-        <f t="shared" si="20"/>
+      <c r="J59" s="42">
+        <f t="shared" si="22"/>
         <v>1689486.5493333333</v>
       </c>
-      <c r="K59" s="34">
-        <f t="shared" si="20"/>
+      <c r="K59" s="43">
+        <f t="shared" si="22"/>
         <v>1900672.3679999998</v>
       </c>
     </row>
+    <row r="60" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61">
+      <c r="A61" s="63" t="str">
+        <f>H39</f>
+        <v>40MWe</v>
+      </c>
+      <c r="B61" s="30">
         <v>0</v>
       </c>
-      <c r="C61" s="35">
+      <c r="C61" s="38">
         <v>1</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="30">
         <v>2</v>
       </c>
-      <c r="E61" s="35">
+      <c r="E61" s="38">
         <v>3</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="30">
         <v>4</v>
       </c>
-      <c r="G61" s="35">
+      <c r="G61" s="38">
         <v>5</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="30">
         <v>6</v>
       </c>
-      <c r="I61" s="35">
+      <c r="I61" s="38">
         <v>7</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="30">
         <v>8</v>
       </c>
-      <c r="K61" s="35">
+      <c r="K61" s="39">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
+      <c r="A62" s="13" t="str">
         <f>A55</f>
         <v>illinois</v>
       </c>
-      <c r="B62" s="34">
+      <c r="B62" s="40">
         <f>$H41+B$47*ABS($I41-$H41)/9</f>
         <v>0</v>
       </c>
-      <c r="C62" s="34">
-        <f t="shared" ref="C62:K62" si="21">$H41+C$47*ABS($I41-$H41)/9</f>
+      <c r="C62" s="40">
+        <f t="shared" ref="C62:K62" si="23">$H41+C$47*ABS($I41-$H41)/9</f>
         <v>62335.802666666656</v>
       </c>
-      <c r="D62" s="34">
-        <f t="shared" si="21"/>
+      <c r="D62" s="40">
+        <f t="shared" si="23"/>
         <v>124671.60533333331</v>
       </c>
-      <c r="E62" s="34">
-        <f t="shared" si="21"/>
+      <c r="E62" s="40">
+        <f t="shared" si="23"/>
         <v>187007.40799999997</v>
       </c>
-      <c r="F62" s="34">
-        <f t="shared" si="21"/>
+      <c r="F62" s="40">
+        <f t="shared" si="23"/>
         <v>249343.21066666662</v>
       </c>
-      <c r="G62" s="34">
-        <f t="shared" si="21"/>
+      <c r="G62" s="40">
+        <f t="shared" si="23"/>
         <v>311679.01333333331</v>
       </c>
-      <c r="H62" s="34">
-        <f t="shared" si="21"/>
+      <c r="H62" s="40">
+        <f t="shared" si="23"/>
         <v>374014.81599999993</v>
       </c>
-      <c r="I62" s="34">
-        <f t="shared" si="21"/>
-        <v>436350.61866666662</v>
-      </c>
-      <c r="J62" s="34">
-        <f t="shared" si="21"/>
-        <v>498686.42133333324</v>
-      </c>
-      <c r="K62" s="34">
-        <f t="shared" si="21"/>
-        <v>561022.22399999993</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" t="str">
-        <f t="shared" ref="A63:A66" si="22">A56</f>
-        <v>nebraska</v>
-      </c>
-      <c r="B63" s="34">
-        <f t="shared" ref="B63:K66" si="23">$H42+B$47*ABS($I42-$H42)/9</f>
-        <v>0</v>
-      </c>
-      <c r="C63" s="34">
-        <f t="shared" si="23"/>
-        <v>218175.30933333331</v>
-      </c>
-      <c r="D63" s="34">
+      <c r="I62" s="40">
         <f t="shared" si="23"/>
         <v>436350.61866666662</v>
       </c>
-      <c r="E63" s="34">
-        <f t="shared" si="23"/>
-        <v>654525.92799999984</v>
-      </c>
-      <c r="F63" s="34">
-        <f t="shared" si="23"/>
-        <v>872701.23733333324</v>
-      </c>
-      <c r="G63" s="34">
-        <f t="shared" si="23"/>
-        <v>1090876.5466666664</v>
-      </c>
-      <c r="H63" s="34">
-        <f t="shared" si="23"/>
-        <v>1309051.8559999997</v>
-      </c>
-      <c r="I63" s="34">
-        <f t="shared" si="23"/>
-        <v>1527227.1653333332</v>
-      </c>
-      <c r="J63" s="34">
-        <f t="shared" si="23"/>
-        <v>1745402.4746666665</v>
-      </c>
-      <c r="K63" s="34">
-        <f t="shared" si="23"/>
-        <v>1963577.7839999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" t="str">
-        <f t="shared" si="22"/>
-        <v>ohio</v>
-      </c>
-      <c r="B64" s="34">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="C64" s="34">
-        <f t="shared" si="23"/>
-        <v>62335.802666666656</v>
-      </c>
-      <c r="D64" s="34">
-        <f t="shared" si="23"/>
-        <v>124671.60533333331</v>
-      </c>
-      <c r="E64" s="34">
-        <f t="shared" si="23"/>
-        <v>187007.40799999997</v>
-      </c>
-      <c r="F64" s="34">
-        <f t="shared" si="23"/>
-        <v>249343.21066666662</v>
-      </c>
-      <c r="G64" s="34">
-        <f t="shared" si="23"/>
-        <v>311679.01333333331</v>
-      </c>
-      <c r="H64" s="34">
-        <f t="shared" si="23"/>
-        <v>374014.81599999993</v>
-      </c>
-      <c r="I64" s="34">
-        <f t="shared" si="23"/>
-        <v>436350.61866666662</v>
-      </c>
-      <c r="J64" s="34">
+      <c r="J62" s="40">
         <f t="shared" si="23"/>
         <v>498686.42133333324</v>
       </c>
-      <c r="K64" s="34">
+      <c r="K62" s="41">
         <f t="shared" si="23"/>
         <v>561022.22399999993</v>
       </c>
     </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="str">
+        <f t="shared" ref="A63:A66" si="24">A56</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B63" s="40">
+        <f t="shared" ref="B63:K66" si="25">$H42+B$47*ABS($I42-$H42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="40">
+        <f t="shared" si="25"/>
+        <v>218175.30933333331</v>
+      </c>
+      <c r="D63" s="40">
+        <f t="shared" si="25"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="E63" s="40">
+        <f t="shared" si="25"/>
+        <v>654525.92799999984</v>
+      </c>
+      <c r="F63" s="40">
+        <f t="shared" si="25"/>
+        <v>872701.23733333324</v>
+      </c>
+      <c r="G63" s="40">
+        <f t="shared" si="25"/>
+        <v>1090876.5466666664</v>
+      </c>
+      <c r="H63" s="40">
+        <f t="shared" si="25"/>
+        <v>1309051.8559999997</v>
+      </c>
+      <c r="I63" s="40">
+        <f t="shared" si="25"/>
+        <v>1527227.1653333332</v>
+      </c>
+      <c r="J63" s="40">
+        <f t="shared" si="25"/>
+        <v>1745402.4746666665</v>
+      </c>
+      <c r="K63" s="41">
+        <f t="shared" si="25"/>
+        <v>1963577.7839999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="13" t="str">
+        <f t="shared" si="24"/>
+        <v>ohio</v>
+      </c>
+      <c r="B64" s="40">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="C64" s="40">
+        <f>$H43+C$47*ABS($I43-$H43)/9</f>
+        <v>62335.802666666656</v>
+      </c>
+      <c r="D64" s="40">
+        <f t="shared" si="25"/>
+        <v>124671.60533333331</v>
+      </c>
+      <c r="E64" s="40">
+        <f t="shared" si="25"/>
+        <v>187007.40799999997</v>
+      </c>
+      <c r="F64" s="40">
+        <f t="shared" si="25"/>
+        <v>249343.21066666662</v>
+      </c>
+      <c r="G64" s="40">
+        <f t="shared" si="25"/>
+        <v>311679.01333333331</v>
+      </c>
+      <c r="H64" s="40">
+        <f t="shared" si="25"/>
+        <v>374014.81599999993</v>
+      </c>
+      <c r="I64" s="40">
+        <f t="shared" si="25"/>
+        <v>436350.61866666662</v>
+      </c>
+      <c r="J64" s="40">
+        <f t="shared" si="25"/>
+        <v>498686.42133333324</v>
+      </c>
+      <c r="K64" s="41">
+        <f t="shared" si="25"/>
+        <v>561022.22399999993</v>
+      </c>
+    </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f t="shared" si="22"/>
+      <c r="A65" s="13" t="str">
+        <f t="shared" si="24"/>
         <v>minnesota</v>
       </c>
-      <c r="B65" s="34">
-        <f t="shared" si="23"/>
+      <c r="B65" s="40">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="C65" s="34">
-        <f t="shared" si="23"/>
+      <c r="C65" s="40">
+        <f t="shared" si="25"/>
         <v>31167.901333333328</v>
       </c>
-      <c r="D65" s="34">
-        <f t="shared" si="23"/>
+      <c r="D65" s="40">
+        <f t="shared" si="25"/>
         <v>62335.802666666656</v>
       </c>
-      <c r="E65" s="34">
-        <f t="shared" si="23"/>
+      <c r="E65" s="40">
+        <f t="shared" si="25"/>
         <v>93503.703999999983</v>
       </c>
-      <c r="F65" s="34">
-        <f t="shared" si="23"/>
+      <c r="F65" s="40">
+        <f t="shared" si="25"/>
         <v>124671.60533333331</v>
       </c>
-      <c r="G65" s="34">
-        <f t="shared" si="23"/>
+      <c r="G65" s="40">
+        <f t="shared" si="25"/>
         <v>155839.50666666665</v>
       </c>
-      <c r="H65" s="34">
-        <f t="shared" si="23"/>
+      <c r="H65" s="40">
+        <f t="shared" si="25"/>
         <v>187007.40799999997</v>
       </c>
-      <c r="I65" s="34">
-        <f t="shared" si="23"/>
+      <c r="I65" s="40">
+        <f t="shared" si="25"/>
         <v>218175.30933333331</v>
       </c>
-      <c r="J65" s="34">
-        <f t="shared" si="23"/>
+      <c r="J65" s="40">
+        <f t="shared" si="25"/>
         <v>249343.21066666662</v>
       </c>
-      <c r="K65" s="34">
-        <f t="shared" si="23"/>
+      <c r="K65" s="41">
+        <f t="shared" si="25"/>
         <v>280511.11199999996</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" t="str">
-        <f t="shared" si="22"/>
+    <row r="66" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="str">
+        <f t="shared" si="24"/>
         <v>texas</v>
       </c>
-      <c r="B66" s="34">
-        <f t="shared" si="23"/>
+      <c r="B66" s="42">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="C66" s="34">
-        <f t="shared" si="23"/>
+      <c r="C66" s="42">
+        <f t="shared" si="25"/>
         <v>436350.61866666662</v>
       </c>
-      <c r="D66" s="34">
-        <f t="shared" si="23"/>
+      <c r="D66" s="42">
+        <f t="shared" si="25"/>
         <v>872701.23733333324</v>
       </c>
-      <c r="E66" s="34">
-        <f t="shared" si="23"/>
+      <c r="E66" s="42">
+        <f t="shared" si="25"/>
         <v>1309051.8559999997</v>
       </c>
-      <c r="F66" s="34">
-        <f t="shared" si="23"/>
+      <c r="F66" s="42">
+        <f t="shared" si="25"/>
         <v>1745402.4746666665</v>
       </c>
-      <c r="G66" s="34">
-        <f t="shared" si="23"/>
+      <c r="G66" s="42">
+        <f t="shared" si="25"/>
         <v>2181753.0933333328</v>
       </c>
-      <c r="H66" s="34">
-        <f t="shared" si="23"/>
+      <c r="H66" s="42">
+        <f t="shared" si="25"/>
         <v>2618103.7119999994</v>
       </c>
-      <c r="I66" s="34">
-        <f t="shared" si="23"/>
+      <c r="I66" s="42">
+        <f t="shared" si="25"/>
         <v>3054454.3306666664</v>
       </c>
-      <c r="J66" s="34">
-        <f t="shared" si="23"/>
+      <c r="J66" s="42">
+        <f t="shared" si="25"/>
         <v>3490804.9493333329</v>
       </c>
-      <c r="K66" s="34">
-        <f t="shared" si="23"/>
+      <c r="K66" s="43">
+        <f t="shared" si="25"/>
         <v>3927155.5679999995</v>
       </c>
     </row>
+    <row r="67" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="63" t="str">
+        <f>J39</f>
+        <v>80MWe</v>
+      </c>
+      <c r="B68" s="51">
+        <f>B47</f>
+        <v>0</v>
+      </c>
+      <c r="C68" s="51">
+        <f t="shared" ref="C68:K68" si="26">C47</f>
+        <v>1</v>
+      </c>
+      <c r="D68" s="51">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="E68" s="51">
+        <f t="shared" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="F68" s="51">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="G68" s="51">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="H68" s="51">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="I68" s="51">
+        <f t="shared" si="26"/>
+        <v>7</v>
+      </c>
+      <c r="J68" s="51">
+        <f t="shared" si="26"/>
+        <v>8</v>
+      </c>
+      <c r="K68" s="52">
+        <f t="shared" si="26"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="str">
+        <f>A41</f>
+        <v>illinois</v>
+      </c>
+      <c r="B69" s="40">
+        <f>$J41+B$47*ABS($K41-$J41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="40">
+        <f t="shared" ref="C69:K69" si="27">$J41+C$47*ABS($K41-$J41)/9</f>
+        <v>126668.60266666667</v>
+      </c>
+      <c r="D69" s="40">
+        <f t="shared" si="27"/>
+        <v>253337.20533333335</v>
+      </c>
+      <c r="E69" s="40">
+        <f t="shared" si="27"/>
+        <v>380005.80800000002</v>
+      </c>
+      <c r="F69" s="40">
+        <f t="shared" si="27"/>
+        <v>506674.41066666669</v>
+      </c>
+      <c r="G69" s="40">
+        <f t="shared" si="27"/>
+        <v>633343.01333333342</v>
+      </c>
+      <c r="H69" s="40">
+        <f t="shared" si="27"/>
+        <v>760011.61600000004</v>
+      </c>
+      <c r="I69" s="40">
+        <f t="shared" si="27"/>
+        <v>886680.21866666665</v>
+      </c>
+      <c r="J69" s="40">
+        <f t="shared" si="27"/>
+        <v>1013348.8213333334</v>
+      </c>
+      <c r="K69" s="41">
+        <f t="shared" si="27"/>
+        <v>1140017.4240000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="str">
+        <f t="shared" ref="A70:A73" si="28">A42</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B70" s="40">
+        <f t="shared" ref="B70:K70" si="29">$J42+B$47*ABS($K42-$J42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C70" s="40">
+        <f>$J42+C$47*ABS($K42-$J42)/9</f>
+        <v>443340.10933333333</v>
+      </c>
+      <c r="D70" s="40">
+        <f t="shared" si="29"/>
+        <v>886680.21866666665</v>
+      </c>
+      <c r="E70" s="40">
+        <f t="shared" si="29"/>
+        <v>1330020.328</v>
+      </c>
+      <c r="F70" s="40">
+        <f t="shared" si="29"/>
+        <v>1773360.4373333333</v>
+      </c>
+      <c r="G70" s="40">
+        <f t="shared" si="29"/>
+        <v>2216700.5466666669</v>
+      </c>
+      <c r="H70" s="40">
+        <f t="shared" si="29"/>
+        <v>2660040.656</v>
+      </c>
+      <c r="I70" s="40">
+        <f t="shared" si="29"/>
+        <v>3103380.7653333335</v>
+      </c>
+      <c r="J70" s="40">
+        <f t="shared" si="29"/>
+        <v>3546720.8746666666</v>
+      </c>
+      <c r="K70" s="41">
+        <f t="shared" si="29"/>
+        <v>3990060.9839999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="str">
+        <f t="shared" si="28"/>
+        <v>ohio</v>
+      </c>
+      <c r="B71" s="40">
+        <f t="shared" ref="B71:K71" si="30">$J43+B$47*ABS($K43-$J43)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="40">
+        <f t="shared" si="30"/>
+        <v>126668.60266666667</v>
+      </c>
+      <c r="D71" s="40">
+        <f t="shared" si="30"/>
+        <v>253337.20533333335</v>
+      </c>
+      <c r="E71" s="40">
+        <f t="shared" si="30"/>
+        <v>380005.80800000002</v>
+      </c>
+      <c r="F71" s="40">
+        <f t="shared" si="30"/>
+        <v>506674.41066666669</v>
+      </c>
+      <c r="G71" s="40">
+        <f t="shared" si="30"/>
+        <v>633343.01333333342</v>
+      </c>
+      <c r="H71" s="40">
+        <f t="shared" si="30"/>
+        <v>760011.61600000004</v>
+      </c>
+      <c r="I71" s="40">
+        <f t="shared" si="30"/>
+        <v>886680.21866666665</v>
+      </c>
+      <c r="J71" s="40">
+        <f t="shared" si="30"/>
+        <v>1013348.8213333334</v>
+      </c>
+      <c r="K71" s="41">
+        <f t="shared" si="30"/>
+        <v>1140017.4240000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="13" t="str">
+        <f t="shared" si="28"/>
+        <v>minnesota</v>
+      </c>
+      <c r="B72" s="40">
+        <f t="shared" ref="B72:K72" si="31">$J44+B$47*ABS($K44-$J44)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C72" s="40">
+        <f t="shared" si="31"/>
+        <v>63334.301333333337</v>
+      </c>
+      <c r="D72" s="40">
+        <f t="shared" si="31"/>
+        <v>126668.60266666667</v>
+      </c>
+      <c r="E72" s="40">
+        <f t="shared" si="31"/>
+        <v>190002.90400000001</v>
+      </c>
+      <c r="F72" s="40">
+        <f>$J44+F$47*ABS($K44-$J44)/9</f>
+        <v>253337.20533333335</v>
+      </c>
+      <c r="G72" s="40">
+        <f t="shared" si="31"/>
+        <v>316671.50666666671</v>
+      </c>
+      <c r="H72" s="40">
+        <f t="shared" si="31"/>
+        <v>380005.80800000002</v>
+      </c>
+      <c r="I72" s="40">
+        <f t="shared" si="31"/>
+        <v>443340.10933333333</v>
+      </c>
+      <c r="J72" s="40">
+        <f t="shared" si="31"/>
+        <v>506674.41066666669</v>
+      </c>
+      <c r="K72" s="41">
+        <f t="shared" si="31"/>
+        <v>570008.71200000006</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>texas</v>
+      </c>
+      <c r="B73" s="42">
+        <f t="shared" ref="B73:K73" si="32">$J45+B$47*ABS($K45-$J45)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C73" s="42">
+        <f t="shared" si="32"/>
+        <v>886680.21866666665</v>
+      </c>
+      <c r="D73" s="42">
+        <f t="shared" si="32"/>
+        <v>1773360.4373333333</v>
+      </c>
+      <c r="E73" s="42">
+        <f t="shared" si="32"/>
+        <v>2660040.656</v>
+      </c>
+      <c r="F73" s="42">
+        <f t="shared" si="32"/>
+        <v>3546720.8746666666</v>
+      </c>
+      <c r="G73" s="42">
+        <f t="shared" si="32"/>
+        <v>4433401.0933333337</v>
+      </c>
+      <c r="H73" s="42">
+        <f t="shared" si="32"/>
+        <v>5320081.3119999999</v>
+      </c>
+      <c r="I73" s="42">
+        <f t="shared" si="32"/>
+        <v>6206761.530666667</v>
+      </c>
+      <c r="J73" s="42">
+        <f t="shared" si="32"/>
+        <v>7093441.7493333332</v>
+      </c>
+      <c r="K73" s="43">
+        <f t="shared" si="32"/>
+        <v>7980121.9679999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="63" t="str">
+        <f>L39</f>
+        <v>100MWe</v>
+      </c>
+      <c r="B75" s="51">
+        <f>B47</f>
+        <v>0</v>
+      </c>
+      <c r="C75" s="51">
+        <f t="shared" ref="C75:K75" si="33">C47</f>
+        <v>1</v>
+      </c>
+      <c r="D75" s="51">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="E75" s="51">
+        <f t="shared" si="33"/>
+        <v>3</v>
+      </c>
+      <c r="F75" s="51">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="G75" s="51">
+        <f t="shared" si="33"/>
+        <v>5</v>
+      </c>
+      <c r="H75" s="51">
+        <f t="shared" si="33"/>
+        <v>6</v>
+      </c>
+      <c r="I75" s="51">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="J75" s="51">
+        <f t="shared" si="33"/>
+        <v>8</v>
+      </c>
+      <c r="K75" s="52">
+        <f t="shared" si="33"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="13" t="str">
+        <f>A41</f>
+        <v>illinois</v>
+      </c>
+      <c r="B76" s="40">
+        <f>$L41+B$47*ABS($M41-$L41)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C76" s="40">
+        <f t="shared" ref="C76:K76" si="34">$L41+C$47*ABS($M41-$L41)/9</f>
+        <v>132029.66933333332</v>
+      </c>
+      <c r="D76" s="40">
+        <f t="shared" si="34"/>
+        <v>264059.33866666665</v>
+      </c>
+      <c r="E76" s="40">
+        <f t="shared" si="34"/>
+        <v>396089.00799999997</v>
+      </c>
+      <c r="F76" s="40">
+        <f t="shared" si="34"/>
+        <v>528118.6773333333</v>
+      </c>
+      <c r="G76" s="40">
+        <f t="shared" si="34"/>
+        <v>660148.34666666668</v>
+      </c>
+      <c r="H76" s="40">
+        <f t="shared" si="34"/>
+        <v>792178.01599999995</v>
+      </c>
+      <c r="I76" s="40">
+        <f t="shared" si="34"/>
+        <v>924207.68533333333</v>
+      </c>
+      <c r="J76" s="40">
+        <f t="shared" si="34"/>
+        <v>1056237.3546666666</v>
+      </c>
+      <c r="K76" s="41">
+        <f t="shared" si="34"/>
+        <v>1188267.024</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="13" t="str">
+        <f t="shared" ref="A77:A80" si="35">A42</f>
+        <v>nebraska</v>
+      </c>
+      <c r="B77" s="40">
+        <f t="shared" ref="B77:K77" si="36">$L42+B$47*ABS($M42-$L42)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C77" s="40">
+        <f t="shared" si="36"/>
+        <v>462103.84266666666</v>
+      </c>
+      <c r="D77" s="40">
+        <f t="shared" si="36"/>
+        <v>924207.68533333333</v>
+      </c>
+      <c r="E77" s="40">
+        <f t="shared" si="36"/>
+        <v>1386311.5279999999</v>
+      </c>
+      <c r="F77" s="40">
+        <f t="shared" si="36"/>
+        <v>1848415.3706666667</v>
+      </c>
+      <c r="G77" s="40">
+        <f t="shared" si="36"/>
+        <v>2310519.2133333329</v>
+      </c>
+      <c r="H77" s="40">
+        <f t="shared" si="36"/>
+        <v>2772623.0559999999</v>
+      </c>
+      <c r="I77" s="40">
+        <f t="shared" si="36"/>
+        <v>3234726.8986666668</v>
+      </c>
+      <c r="J77" s="40">
+        <f t="shared" si="36"/>
+        <v>3696830.7413333333</v>
+      </c>
+      <c r="K77" s="41">
+        <f t="shared" si="36"/>
+        <v>4158934.5839999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="13" t="str">
+        <f t="shared" si="35"/>
+        <v>ohio</v>
+      </c>
+      <c r="B78" s="40">
+        <f t="shared" ref="B78:K78" si="37">$L43+B$47*ABS($M43-$L43)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C78" s="40">
+        <f t="shared" si="37"/>
+        <v>132029.66933333332</v>
+      </c>
+      <c r="D78" s="40">
+        <f t="shared" si="37"/>
+        <v>264059.33866666665</v>
+      </c>
+      <c r="E78" s="40">
+        <f t="shared" si="37"/>
+        <v>396089.00799999997</v>
+      </c>
+      <c r="F78" s="40">
+        <f t="shared" si="37"/>
+        <v>528118.6773333333</v>
+      </c>
+      <c r="G78" s="40">
+        <f t="shared" si="37"/>
+        <v>660148.34666666668</v>
+      </c>
+      <c r="H78" s="40">
+        <f t="shared" si="37"/>
+        <v>792178.01599999995</v>
+      </c>
+      <c r="I78" s="40">
+        <f t="shared" si="37"/>
+        <v>924207.68533333333</v>
+      </c>
+      <c r="J78" s="40">
+        <f t="shared" si="37"/>
+        <v>1056237.3546666666</v>
+      </c>
+      <c r="K78" s="41">
+        <f t="shared" si="37"/>
+        <v>1188267.024</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="13" t="str">
+        <f t="shared" si="35"/>
+        <v>minnesota</v>
+      </c>
+      <c r="B79" s="40">
+        <f t="shared" ref="B79:K79" si="38">$L44+B$47*ABS($M44-$L44)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C79" s="40">
+        <f t="shared" si="38"/>
+        <v>66014.834666666662</v>
+      </c>
+      <c r="D79" s="40">
+        <f t="shared" si="38"/>
+        <v>132029.66933333332</v>
+      </c>
+      <c r="E79" s="40">
+        <f t="shared" si="38"/>
+        <v>198044.50399999999</v>
+      </c>
+      <c r="F79" s="40">
+        <f t="shared" si="38"/>
+        <v>264059.33866666665</v>
+      </c>
+      <c r="G79" s="40">
+        <f t="shared" si="38"/>
+        <v>330074.17333333334</v>
+      </c>
+      <c r="H79" s="40">
+        <f t="shared" si="38"/>
+        <v>396089.00799999997</v>
+      </c>
+      <c r="I79" s="40">
+        <f t="shared" si="38"/>
+        <v>462103.84266666666</v>
+      </c>
+      <c r="J79" s="40">
+        <f t="shared" si="38"/>
+        <v>528118.6773333333</v>
+      </c>
+      <c r="K79" s="41">
+        <f t="shared" si="38"/>
+        <v>594133.51199999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v>texas</v>
+      </c>
+      <c r="B80" s="42">
+        <f t="shared" ref="B80:K80" si="39">$L45+B$47*ABS($M45-$L45)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C80" s="42">
+        <f t="shared" si="39"/>
+        <v>924207.68533333333</v>
+      </c>
+      <c r="D80" s="42">
+        <f t="shared" si="39"/>
+        <v>1848415.3706666667</v>
+      </c>
+      <c r="E80" s="42">
+        <f t="shared" si="39"/>
+        <v>2772623.0559999999</v>
+      </c>
+      <c r="F80" s="42">
+        <f t="shared" si="39"/>
+        <v>3696830.7413333333</v>
+      </c>
+      <c r="G80" s="42">
+        <f t="shared" si="39"/>
+        <v>4621038.4266666658</v>
+      </c>
+      <c r="H80" s="42">
+        <f t="shared" si="39"/>
+        <v>5545246.1119999997</v>
+      </c>
+      <c r="I80" s="42">
+        <f t="shared" si="39"/>
+        <v>6469453.7973333336</v>
+      </c>
+      <c r="J80" s="42">
+        <f t="shared" si="39"/>
+        <v>7393661.4826666666</v>
+      </c>
+      <c r="K80" s="43">
+        <f t="shared" si="39"/>
+        <v>8317869.1679999996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:D12"/>
@@ -4457,10 +5182,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="35"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -4628,26 +5353,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4719,15 +5444,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4805,22 +5530,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4834,11 +5559,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">

</xml_diff>

<commit_message>
ITC and PTC calculations
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76249CF-CCC6-0F4A-8CCF-7D769B1AFEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF6F3B-9FAD-3146-A6A7-2F8CF1903596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="35840" yWindow="-1600" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="SMR" sheetId="13" r:id="rId1"/>
     <sheet name="Boundaries" sheetId="10" r:id="rId2"/>
-    <sheet name="MACRS" sheetId="1" r:id="rId3"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId4"/>
-    <sheet name="HTSE" sheetId="2" r:id="rId5"/>
-    <sheet name="FT" sheetId="11" r:id="rId6"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId7"/>
-    <sheet name="Tax rates" sheetId="12" r:id="rId8"/>
+    <sheet name="PTC vs. ITC" sheetId="14" r:id="rId3"/>
+    <sheet name="MACRS" sheetId="1" r:id="rId4"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId5"/>
+    <sheet name="HTSE" sheetId="2" r:id="rId6"/>
+    <sheet name="FT" sheetId="11" r:id="rId7"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId8"/>
+    <sheet name="Tax rates" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="226">
   <si>
     <t>Source</t>
   </si>
@@ -687,6 +688,39 @@
   </si>
   <si>
     <t>For SA inputs</t>
+  </si>
+  <si>
+    <t>SMR Capacity (MWe)</t>
+  </si>
+  <si>
+    <t>ITC (%)</t>
+  </si>
+  <si>
+    <t>PTC ($/Mwh)</t>
+  </si>
+  <si>
+    <t>CAPEX ($/MW)</t>
+  </si>
+  <si>
+    <t>Added revenues</t>
+  </si>
+  <si>
+    <t>ITC</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>First 10 years of operations</t>
+  </si>
+  <si>
+    <t>20% of total CAPEX costs</t>
+  </si>
+  <si>
+    <t>25 $/MWh for 10 years</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
   </si>
 </sst>
 </file>
@@ -764,7 +798,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,6 +813,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1007,7 +1053,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1058,22 +1104,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="18" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1091,8 +1127,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="3" borderId="18" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="5" builtinId="22"/>
@@ -2625,7 +2673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
@@ -2735,26 +2783,26 @@
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53" t="s">
+      <c r="D12" s="50"/>
+      <c r="E12" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="55"/>
-      <c r="B13" s="57"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="55"/>
       <c r="C13" t="s">
         <v>189</v>
       </c>
@@ -2889,25 +2937,25 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="49" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="59"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
@@ -2949,7 +2997,7 @@
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="B24" s="59">
+      <c r="B24" s="48">
         <f>$C14+B$23*ABS($C14-$D14)/9</f>
         <v>-705.1</v>
       </c>
@@ -2957,7 +3005,7 @@
         <f t="shared" ref="C24:K24" si="5">$C14+C$23*ABS($C14-$D14)/9</f>
         <v>-636.21111111111111</v>
       </c>
-      <c r="D24" s="59">
+      <c r="D24" s="48">
         <f t="shared" si="5"/>
         <v>-567.32222222222231</v>
       </c>
@@ -2965,7 +3013,7 @@
         <f t="shared" si="5"/>
         <v>-498.43333333333339</v>
       </c>
-      <c r="F24" s="59">
+      <c r="F24" s="48">
         <f t="shared" si="5"/>
         <v>-429.54444444444448</v>
       </c>
@@ -2973,7 +3021,7 @@
         <f t="shared" si="5"/>
         <v>-360.65555555555557</v>
       </c>
-      <c r="H24" s="59">
+      <c r="H24" s="48">
         <f t="shared" si="5"/>
         <v>-291.76666666666671</v>
       </c>
@@ -2981,7 +3029,7 @@
         <f t="shared" si="5"/>
         <v>-222.87777777777779</v>
       </c>
-      <c r="J24" s="59">
+      <c r="J24" s="48">
         <f t="shared" si="5"/>
         <v>-153.98888888888894</v>
       </c>
@@ -2995,7 +3043,7 @@
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="B25" s="59">
+      <c r="B25" s="48">
         <f>$C15+B$23*ABS($C15-$D15)/9</f>
         <v>-225.1</v>
       </c>
@@ -3003,7 +3051,7 @@
         <f t="shared" ref="C25:K25" si="6">$C15+C$23*ABS($C15-$D15)/9</f>
         <v>-209.54444444444445</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="48">
         <f t="shared" si="6"/>
         <v>-193.98888888888888</v>
       </c>
@@ -3011,7 +3059,7 @@
         <f t="shared" si="6"/>
         <v>-178.43333333333334</v>
       </c>
-      <c r="F25" s="59">
+      <c r="F25" s="48">
         <f t="shared" si="6"/>
         <v>-162.87777777777777</v>
       </c>
@@ -3019,7 +3067,7 @@
         <f t="shared" si="6"/>
         <v>-147.32222222222222</v>
       </c>
-      <c r="H25" s="59">
+      <c r="H25" s="48">
         <f t="shared" si="6"/>
         <v>-131.76666666666665</v>
       </c>
@@ -3027,7 +3075,7 @@
         <f t="shared" si="6"/>
         <v>-116.21111111111111</v>
       </c>
-      <c r="J25" s="59">
+      <c r="J25" s="48">
         <f t="shared" si="6"/>
         <v>-100.65555555555555</v>
       </c>
@@ -3041,7 +3089,7 @@
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="B26" s="59">
+      <c r="B26" s="48">
         <f>$C16+B$23*ABS($C16-$D16)/9</f>
         <v>-465.1</v>
       </c>
@@ -3049,7 +3097,7 @@
         <f t="shared" ref="C26:K26" si="7">$C16+C$23*ABS($C16-$D16)/9</f>
         <v>-422.87777777777779</v>
       </c>
-      <c r="D26" s="59">
+      <c r="D26" s="48">
         <f t="shared" si="7"/>
         <v>-380.65555555555557</v>
       </c>
@@ -3057,7 +3105,7 @@
         <f t="shared" si="7"/>
         <v>-338.43333333333334</v>
       </c>
-      <c r="F26" s="59">
+      <c r="F26" s="48">
         <f t="shared" si="7"/>
         <v>-296.21111111111111</v>
       </c>
@@ -3065,7 +3113,7 @@
         <f t="shared" si="7"/>
         <v>-253.98888888888891</v>
       </c>
-      <c r="H26" s="59">
+      <c r="H26" s="48">
         <f t="shared" si="7"/>
         <v>-211.76666666666668</v>
       </c>
@@ -3073,7 +3121,7 @@
         <f t="shared" si="7"/>
         <v>-169.54444444444448</v>
       </c>
-      <c r="J26" s="59">
+      <c r="J26" s="48">
         <f t="shared" si="7"/>
         <v>-127.32222222222225</v>
       </c>
@@ -3087,7 +3135,7 @@
         <f t="shared" ref="A27:A28" si="8">A17</f>
         <v>80MWe</v>
       </c>
-      <c r="B27" s="59">
+      <c r="B27" s="48">
         <f>$C17+B$23*ABS($C17-$D17)/9</f>
         <v>-945.1</v>
       </c>
@@ -3095,7 +3143,7 @@
         <f t="shared" ref="C27:K27" si="9">$C17+C$23*ABS($C17-$D17)/9</f>
         <v>-849.54444444444448</v>
       </c>
-      <c r="D27" s="59">
+      <c r="D27" s="48">
         <f t="shared" si="9"/>
         <v>-753.98888888888894</v>
       </c>
@@ -3103,7 +3151,7 @@
         <f t="shared" si="9"/>
         <v>-658.43333333333339</v>
       </c>
-      <c r="F27" s="59">
+      <c r="F27" s="48">
         <f t="shared" si="9"/>
         <v>-562.87777777777774</v>
       </c>
@@ -3111,7 +3159,7 @@
         <f t="shared" si="9"/>
         <v>-467.32222222222225</v>
       </c>
-      <c r="H27" s="59">
+      <c r="H27" s="48">
         <f t="shared" si="9"/>
         <v>-371.76666666666665</v>
       </c>
@@ -3119,7 +3167,7 @@
         <f t="shared" si="9"/>
         <v>-276.21111111111111</v>
       </c>
-      <c r="J27" s="59">
+      <c r="J27" s="48">
         <f t="shared" si="9"/>
         <v>-180.65555555555557</v>
       </c>
@@ -3133,7 +3181,7 @@
         <f t="shared" si="8"/>
         <v>100MWe</v>
       </c>
-      <c r="B28" s="59">
+      <c r="B28" s="48">
         <f t="shared" ref="B28:K28" si="10">$C18+B$23*ABS($C18-$D18)/9</f>
         <v>-985.1</v>
       </c>
@@ -3141,7 +3189,7 @@
         <f t="shared" si="10"/>
         <v>-885.1</v>
       </c>
-      <c r="D28" s="59">
+      <c r="D28" s="48">
         <f t="shared" si="10"/>
         <v>-785.1</v>
       </c>
@@ -3149,7 +3197,7 @@
         <f t="shared" si="10"/>
         <v>-685.1</v>
       </c>
-      <c r="F28" s="59">
+      <c r="F28" s="48">
         <f t="shared" si="10"/>
         <v>-585.1</v>
       </c>
@@ -3157,7 +3205,7 @@
         <f t="shared" si="10"/>
         <v>-485.1</v>
       </c>
-      <c r="H28" s="59">
+      <c r="H28" s="48">
         <f t="shared" si="10"/>
         <v>-385.1</v>
       </c>
@@ -3165,7 +3213,7 @@
         <f t="shared" si="10"/>
         <v>-285.10000000000002</v>
       </c>
-      <c r="J28" s="59">
+      <c r="J28" s="48">
         <f t="shared" si="10"/>
         <v>-185.10000000000002</v>
       </c>
@@ -3176,19 +3224,19 @@
     </row>
     <row r="29" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="50"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="59"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="45" t="s">
@@ -3230,7 +3278,7 @@
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="B32" s="59">
+      <c r="B32" s="48">
         <f t="shared" ref="B32:K32" si="11">$E14+B$31*ABS($E14-$F14)/9</f>
         <v>-17719.163</v>
       </c>
@@ -3238,7 +3286,7 @@
         <f t="shared" si="11"/>
         <v>-15987.985222222222</v>
       </c>
-      <c r="D32" s="59">
+      <c r="D32" s="48">
         <f t="shared" si="11"/>
         <v>-14256.807444444445</v>
       </c>
@@ -3246,7 +3294,7 @@
         <f t="shared" si="11"/>
         <v>-12525.629666666668</v>
       </c>
-      <c r="F32" s="59">
+      <c r="F32" s="48">
         <f t="shared" si="11"/>
         <v>-10794.451888888889</v>
       </c>
@@ -3254,7 +3302,7 @@
         <f t="shared" si="11"/>
         <v>-9063.2741111111118</v>
       </c>
-      <c r="H32" s="59">
+      <c r="H32" s="48">
         <f t="shared" si="11"/>
         <v>-7332.096333333333</v>
       </c>
@@ -3262,7 +3310,7 @@
         <f t="shared" si="11"/>
         <v>-5600.9185555555559</v>
       </c>
-      <c r="J32" s="59">
+      <c r="J32" s="48">
         <f t="shared" si="11"/>
         <v>-3869.7407777777771</v>
       </c>
@@ -3276,7 +3324,7 @@
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="B33" s="59">
+      <c r="B33" s="48">
         <f t="shared" ref="B33:K33" si="12">$E15+B$31*ABS($E15-$F15)/9</f>
         <v>-5656.7629999999999</v>
       </c>
@@ -3284,7 +3332,7 @@
         <f t="shared" si="12"/>
         <v>-5265.8518888888884</v>
       </c>
-      <c r="D33" s="59">
+      <c r="D33" s="48">
         <f t="shared" si="12"/>
         <v>-4874.9407777777778</v>
       </c>
@@ -3292,7 +3340,7 @@
         <f t="shared" si="12"/>
         <v>-4484.0296666666663</v>
       </c>
-      <c r="F33" s="59">
+      <c r="F33" s="48">
         <f t="shared" si="12"/>
         <v>-4093.1185555555553</v>
       </c>
@@ -3300,7 +3348,7 @@
         <f t="shared" si="12"/>
         <v>-3702.2074444444443</v>
       </c>
-      <c r="H33" s="59">
+      <c r="H33" s="48">
         <f t="shared" si="12"/>
         <v>-3311.2963333333332</v>
       </c>
@@ -3308,7 +3356,7 @@
         <f t="shared" si="12"/>
         <v>-2920.3852222222222</v>
       </c>
-      <c r="J33" s="59">
+      <c r="J33" s="48">
         <f t="shared" si="12"/>
         <v>-2529.4741111111107</v>
       </c>
@@ -3323,7 +3371,7 @@
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="B34" s="59">
+      <c r="B34" s="48">
         <f t="shared" ref="B34:K34" si="13">$E16+B$31*ABS($E16-$F16)/9</f>
         <v>-11687.963</v>
       </c>
@@ -3331,7 +3379,7 @@
         <f t="shared" si="13"/>
         <v>-10626.918555555556</v>
       </c>
-      <c r="D34" s="59">
+      <c r="D34" s="48">
         <f t="shared" si="13"/>
         <v>-9565.8741111111103</v>
       </c>
@@ -3339,7 +3387,7 @@
         <f t="shared" si="13"/>
         <v>-8504.8296666666665</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="48">
         <f t="shared" si="13"/>
         <v>-7443.7852222222218</v>
       </c>
@@ -3347,7 +3395,7 @@
         <f t="shared" si="13"/>
         <v>-6382.7407777777771</v>
       </c>
-      <c r="H34" s="59">
+      <c r="H34" s="48">
         <f t="shared" si="13"/>
         <v>-5321.6963333333333</v>
       </c>
@@ -3355,7 +3403,7 @@
         <f t="shared" si="13"/>
         <v>-4260.6518888888886</v>
       </c>
-      <c r="J34" s="59">
+      <c r="J34" s="48">
         <f t="shared" si="13"/>
         <v>-3199.6074444444439</v>
       </c>
@@ -3369,7 +3417,7 @@
         <f t="shared" ref="A35:A36" si="14">A17</f>
         <v>80MWe</v>
       </c>
-      <c r="B35" s="59">
+      <c r="B35" s="48">
         <f t="shared" ref="B35:K35" si="15">$E17+B$31*ABS($E17-$F17)/9</f>
         <v>-23750.363000000001</v>
       </c>
@@ -3377,7 +3425,7 @@
         <f t="shared" si="15"/>
         <v>-21349.051888888891</v>
       </c>
-      <c r="D35" s="59">
+      <c r="D35" s="48">
         <f t="shared" si="15"/>
         <v>-18947.740777777777</v>
       </c>
@@ -3385,7 +3433,7 @@
         <f t="shared" si="15"/>
         <v>-16546.429666666667</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="48">
         <f t="shared" si="15"/>
         <v>-14145.118555555555</v>
       </c>
@@ -3393,7 +3441,7 @@
         <f t="shared" si="15"/>
         <v>-11743.807444444445</v>
       </c>
-      <c r="H35" s="59">
+      <c r="H35" s="48">
         <f t="shared" si="15"/>
         <v>-9342.4963333333326</v>
       </c>
@@ -3401,7 +3449,7 @@
         <f t="shared" si="15"/>
         <v>-6941.1852222222187</v>
       </c>
-      <c r="J35" s="59">
+      <c r="J35" s="48">
         <f t="shared" si="15"/>
         <v>-4539.8741111111085</v>
       </c>
@@ -3415,7 +3463,7 @@
         <f t="shared" si="14"/>
         <v>100MWe</v>
       </c>
-      <c r="B36" s="59">
+      <c r="B36" s="48">
         <f t="shared" ref="B36:K36" si="16">$E18+B$31*ABS($E18-$F18)/9</f>
         <v>-24755.562999999998</v>
       </c>
@@ -3423,7 +3471,7 @@
         <f t="shared" si="16"/>
         <v>-22242.562999999998</v>
       </c>
-      <c r="D36" s="59">
+      <c r="D36" s="48">
         <f t="shared" si="16"/>
         <v>-19729.562999999998</v>
       </c>
@@ -3431,7 +3479,7 @@
         <f t="shared" si="16"/>
         <v>-17216.562999999998</v>
       </c>
-      <c r="F36" s="59">
+      <c r="F36" s="48">
         <f t="shared" si="16"/>
         <v>-14703.562999999998</v>
       </c>
@@ -3439,7 +3487,7 @@
         <f t="shared" si="16"/>
         <v>-12190.562999999998</v>
       </c>
-      <c r="H36" s="59">
+      <c r="H36" s="48">
         <f t="shared" si="16"/>
         <v>-9677.5629999999983</v>
       </c>
@@ -3447,7 +3495,7 @@
         <f t="shared" si="16"/>
         <v>-7164.5629999999983</v>
       </c>
-      <c r="J36" s="59">
+      <c r="J36" s="48">
         <f t="shared" si="16"/>
         <v>-4651.5629999999983</v>
       </c>
@@ -3475,31 +3523,31 @@
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
-      <c r="D39" s="51" t="str">
+      <c r="D39" s="60" t="str">
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="E39" s="52"/>
-      <c r="F39" s="51" t="str">
+      <c r="E39" s="51"/>
+      <c r="F39" s="60" t="str">
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="G39" s="52"/>
-      <c r="H39" s="51" t="str">
+      <c r="G39" s="51"/>
+      <c r="H39" s="60" t="str">
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="I39" s="52"/>
-      <c r="J39" s="51" t="str">
+      <c r="I39" s="51"/>
+      <c r="J39" s="60" t="str">
         <f>A35</f>
         <v>80MWe</v>
       </c>
-      <c r="K39" s="52"/>
-      <c r="L39" s="53" t="str">
+      <c r="K39" s="51"/>
+      <c r="L39" s="50" t="str">
         <f>A36</f>
         <v>100MWe</v>
       </c>
-      <c r="M39" s="52"/>
+      <c r="M39" s="51"/>
     </row>
     <row r="40" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
@@ -4084,7 +4132,7 @@
         <f>A48</f>
         <v>illinois</v>
       </c>
-      <c r="B55" s="59">
+      <c r="B55" s="48">
         <f>$F41+B$47*ABS($G41-$F41)/9</f>
         <v>0</v>
       </c>
@@ -4092,7 +4140,7 @@
         <f>$F41+C$47*ABS($G41-$F41)/9</f>
         <v>30169.402666666669</v>
       </c>
-      <c r="D55" s="59">
+      <c r="D55" s="48">
         <f t="shared" ref="D55:K55" si="25">$F41+D$47*ABS($G41-$F41)/9</f>
         <v>60338.805333333337</v>
       </c>
@@ -4100,7 +4148,7 @@
         <f t="shared" si="25"/>
         <v>90508.207999999999</v>
       </c>
-      <c r="F55" s="59">
+      <c r="F55" s="48">
         <f t="shared" si="25"/>
         <v>120677.61066666667</v>
       </c>
@@ -4108,7 +4156,7 @@
         <f t="shared" si="25"/>
         <v>150847.01333333334</v>
       </c>
-      <c r="H55" s="59">
+      <c r="H55" s="48">
         <f t="shared" si="25"/>
         <v>181016.416</v>
       </c>
@@ -4116,7 +4164,7 @@
         <f t="shared" si="25"/>
         <v>211185.81866666666</v>
       </c>
-      <c r="J55" s="59">
+      <c r="J55" s="48">
         <f t="shared" si="25"/>
         <v>241355.22133333335</v>
       </c>
@@ -4130,7 +4178,7 @@
         <f t="shared" ref="A56:A59" si="26">A49</f>
         <v>nebraska</v>
       </c>
-      <c r="B56" s="59">
+      <c r="B56" s="48">
         <f t="shared" ref="B56:K59" si="27">$F42+B$47*ABS($G42-$F42)/9</f>
         <v>0</v>
       </c>
@@ -4138,7 +4186,7 @@
         <f t="shared" si="27"/>
         <v>105592.90933333333</v>
       </c>
-      <c r="D56" s="59">
+      <c r="D56" s="48">
         <f t="shared" si="27"/>
         <v>211185.81866666666</v>
       </c>
@@ -4146,7 +4194,7 @@
         <f t="shared" si="27"/>
         <v>316778.728</v>
       </c>
-      <c r="F56" s="59">
+      <c r="F56" s="48">
         <f t="shared" si="27"/>
         <v>422371.63733333332</v>
       </c>
@@ -4154,7 +4202,7 @@
         <f t="shared" si="27"/>
         <v>527964.54666666663</v>
       </c>
-      <c r="H56" s="59">
+      <c r="H56" s="48">
         <f t="shared" si="27"/>
         <v>633557.45600000001</v>
       </c>
@@ -4162,7 +4210,7 @@
         <f t="shared" si="27"/>
         <v>739150.36533333326</v>
       </c>
-      <c r="J56" s="59">
+      <c r="J56" s="48">
         <f t="shared" si="27"/>
         <v>844743.27466666664</v>
       </c>
@@ -4176,7 +4224,7 @@
         <f t="shared" si="26"/>
         <v>ohio</v>
       </c>
-      <c r="B57" s="59">
+      <c r="B57" s="48">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -4184,7 +4232,7 @@
         <f t="shared" si="27"/>
         <v>30169.402666666669</v>
       </c>
-      <c r="D57" s="59">
+      <c r="D57" s="48">
         <f t="shared" si="27"/>
         <v>60338.805333333337</v>
       </c>
@@ -4192,7 +4240,7 @@
         <f t="shared" si="27"/>
         <v>90508.207999999999</v>
       </c>
-      <c r="F57" s="59">
+      <c r="F57" s="48">
         <f t="shared" si="27"/>
         <v>120677.61066666667</v>
       </c>
@@ -4200,7 +4248,7 @@
         <f t="shared" si="27"/>
         <v>150847.01333333334</v>
       </c>
-      <c r="H57" s="59">
+      <c r="H57" s="48">
         <f t="shared" si="27"/>
         <v>181016.416</v>
       </c>
@@ -4208,7 +4256,7 @@
         <f t="shared" si="27"/>
         <v>211185.81866666666</v>
       </c>
-      <c r="J57" s="59">
+      <c r="J57" s="48">
         <f t="shared" si="27"/>
         <v>241355.22133333335</v>
       </c>
@@ -4222,7 +4270,7 @@
         <f t="shared" si="26"/>
         <v>minnesota</v>
       </c>
-      <c r="B58" s="59">
+      <c r="B58" s="48">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -4230,7 +4278,7 @@
         <f>$F44+C$47*ABS($G44-$F44)/9</f>
         <v>15084.701333333334</v>
       </c>
-      <c r="D58" s="59">
+      <c r="D58" s="48">
         <f t="shared" si="27"/>
         <v>30169.402666666669</v>
       </c>
@@ -4238,7 +4286,7 @@
         <f t="shared" si="27"/>
         <v>45254.103999999999</v>
       </c>
-      <c r="F58" s="59">
+      <c r="F58" s="48">
         <f t="shared" si="27"/>
         <v>60338.805333333337</v>
       </c>
@@ -4246,7 +4294,7 @@
         <f t="shared" si="27"/>
         <v>75423.506666666668</v>
       </c>
-      <c r="H58" s="59">
+      <c r="H58" s="48">
         <f t="shared" si="27"/>
         <v>90508.207999999999</v>
       </c>
@@ -4254,7 +4302,7 @@
         <f t="shared" si="27"/>
         <v>105592.90933333333</v>
       </c>
-      <c r="J58" s="59">
+      <c r="J58" s="48">
         <f t="shared" si="27"/>
         <v>120677.61066666667</v>
       </c>
@@ -4268,7 +4316,7 @@
         <f t="shared" si="26"/>
         <v>texas</v>
       </c>
-      <c r="B59" s="59">
+      <c r="B59" s="48">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -4276,7 +4324,7 @@
         <f t="shared" si="27"/>
         <v>211185.81866666666</v>
       </c>
-      <c r="D59" s="59">
+      <c r="D59" s="48">
         <f t="shared" si="27"/>
         <v>422371.63733333332</v>
       </c>
@@ -4284,7 +4332,7 @@
         <f t="shared" si="27"/>
         <v>633557.45600000001</v>
       </c>
-      <c r="F59" s="59">
+      <c r="F59" s="48">
         <f t="shared" si="27"/>
         <v>844743.27466666664</v>
       </c>
@@ -4292,7 +4340,7 @@
         <f t="shared" si="27"/>
         <v>1055929.0933333333</v>
       </c>
-      <c r="H59" s="59">
+      <c r="H59" s="48">
         <f t="shared" si="27"/>
         <v>1267114.912</v>
       </c>
@@ -4300,7 +4348,7 @@
         <f t="shared" si="27"/>
         <v>1478300.7306666665</v>
       </c>
-      <c r="J59" s="59">
+      <c r="J59" s="48">
         <f t="shared" si="27"/>
         <v>1689486.5493333333</v>
       </c>
@@ -4905,7 +4953,7 @@
         <f>A41</f>
         <v>illinois</v>
       </c>
-      <c r="B76" s="59">
+      <c r="B76" s="48">
         <f>$L41+B$47*ABS($M41-$L41)/9</f>
         <v>0</v>
       </c>
@@ -4913,7 +4961,7 @@
         <f t="shared" ref="C76:K76" si="39">$L41+C$47*ABS($M41-$L41)/9</f>
         <v>132029.66933333332</v>
       </c>
-      <c r="D76" s="59">
+      <c r="D76" s="48">
         <f t="shared" si="39"/>
         <v>264059.33866666665</v>
       </c>
@@ -4921,7 +4969,7 @@
         <f t="shared" si="39"/>
         <v>396089.00799999997</v>
       </c>
-      <c r="F76" s="59">
+      <c r="F76" s="48">
         <f t="shared" si="39"/>
         <v>528118.6773333333</v>
       </c>
@@ -4929,7 +4977,7 @@
         <f t="shared" si="39"/>
         <v>660148.34666666668</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="48">
         <f t="shared" si="39"/>
         <v>792178.01599999995</v>
       </c>
@@ -4937,7 +4985,7 @@
         <f t="shared" si="39"/>
         <v>924207.68533333333</v>
       </c>
-      <c r="J76" s="59">
+      <c r="J76" s="48">
         <f t="shared" si="39"/>
         <v>1056237.3546666666</v>
       </c>
@@ -4951,7 +4999,7 @@
         <f t="shared" ref="A77:A80" si="40">A42</f>
         <v>nebraska</v>
       </c>
-      <c r="B77" s="59">
+      <c r="B77" s="48">
         <f t="shared" ref="B77:K77" si="41">$L42+B$47*ABS($M42-$L42)/9</f>
         <v>0</v>
       </c>
@@ -4959,7 +5007,7 @@
         <f t="shared" si="41"/>
         <v>462103.84266666666</v>
       </c>
-      <c r="D77" s="59">
+      <c r="D77" s="48">
         <f t="shared" si="41"/>
         <v>924207.68533333333</v>
       </c>
@@ -4967,7 +5015,7 @@
         <f t="shared" si="41"/>
         <v>1386311.5279999999</v>
       </c>
-      <c r="F77" s="59">
+      <c r="F77" s="48">
         <f t="shared" si="41"/>
         <v>1848415.3706666667</v>
       </c>
@@ -4975,7 +5023,7 @@
         <f t="shared" si="41"/>
         <v>2310519.2133333329</v>
       </c>
-      <c r="H77" s="59">
+      <c r="H77" s="48">
         <f t="shared" si="41"/>
         <v>2772623.0559999999</v>
       </c>
@@ -4983,7 +5031,7 @@
         <f t="shared" si="41"/>
         <v>3234726.8986666668</v>
       </c>
-      <c r="J77" s="59">
+      <c r="J77" s="48">
         <f t="shared" si="41"/>
         <v>3696830.7413333333</v>
       </c>
@@ -4997,7 +5045,7 @@
         <f t="shared" si="40"/>
         <v>ohio</v>
       </c>
-      <c r="B78" s="59">
+      <c r="B78" s="48">
         <f t="shared" ref="B78:K78" si="42">$L43+B$47*ABS($M43-$L43)/9</f>
         <v>0</v>
       </c>
@@ -5005,7 +5053,7 @@
         <f t="shared" si="42"/>
         <v>132029.66933333332</v>
       </c>
-      <c r="D78" s="59">
+      <c r="D78" s="48">
         <f t="shared" si="42"/>
         <v>264059.33866666665</v>
       </c>
@@ -5013,7 +5061,7 @@
         <f t="shared" si="42"/>
         <v>396089.00799999997</v>
       </c>
-      <c r="F78" s="59">
+      <c r="F78" s="48">
         <f t="shared" si="42"/>
         <v>528118.6773333333</v>
       </c>
@@ -5021,7 +5069,7 @@
         <f t="shared" si="42"/>
         <v>660148.34666666668</v>
       </c>
-      <c r="H78" s="59">
+      <c r="H78" s="48">
         <f t="shared" si="42"/>
         <v>792178.01599999995</v>
       </c>
@@ -5029,7 +5077,7 @@
         <f t="shared" si="42"/>
         <v>924207.68533333333</v>
       </c>
-      <c r="J78" s="59">
+      <c r="J78" s="48">
         <f t="shared" si="42"/>
         <v>1056237.3546666666</v>
       </c>
@@ -5043,7 +5091,7 @@
         <f t="shared" si="40"/>
         <v>minnesota</v>
       </c>
-      <c r="B79" s="59">
+      <c r="B79" s="48">
         <f t="shared" ref="B79:K79" si="43">$L44+B$47*ABS($M44-$L44)/9</f>
         <v>0</v>
       </c>
@@ -5051,7 +5099,7 @@
         <f t="shared" si="43"/>
         <v>66014.834666666662</v>
       </c>
-      <c r="D79" s="59">
+      <c r="D79" s="48">
         <f t="shared" si="43"/>
         <v>132029.66933333332</v>
       </c>
@@ -5059,7 +5107,7 @@
         <f t="shared" si="43"/>
         <v>198044.50399999999</v>
       </c>
-      <c r="F79" s="59">
+      <c r="F79" s="48">
         <f t="shared" si="43"/>
         <v>264059.33866666665</v>
       </c>
@@ -5067,7 +5115,7 @@
         <f t="shared" si="43"/>
         <v>330074.17333333334</v>
       </c>
-      <c r="H79" s="59">
+      <c r="H79" s="48">
         <f t="shared" si="43"/>
         <v>396089.00799999997</v>
       </c>
@@ -5075,7 +5123,7 @@
         <f t="shared" si="43"/>
         <v>462103.84266666666</v>
       </c>
-      <c r="J79" s="59">
+      <c r="J79" s="48">
         <f t="shared" si="43"/>
         <v>528118.6773333333</v>
       </c>
@@ -5089,7 +5137,7 @@
         <f t="shared" si="40"/>
         <v>texas</v>
       </c>
-      <c r="B80" s="59">
+      <c r="B80" s="48">
         <f t="shared" ref="B80:K80" si="44">$L45+B$47*ABS($M45-$L45)/9</f>
         <v>0</v>
       </c>
@@ -5097,7 +5145,7 @@
         <f t="shared" si="44"/>
         <v>924207.68533333333</v>
       </c>
-      <c r="D80" s="59">
+      <c r="D80" s="48">
         <f t="shared" si="44"/>
         <v>1848415.3706666667</v>
       </c>
@@ -5105,7 +5153,7 @@
         <f t="shared" si="44"/>
         <v>2772623.0559999999</v>
       </c>
-      <c r="F80" s="59">
+      <c r="F80" s="48">
         <f t="shared" si="44"/>
         <v>3696830.7413333333</v>
       </c>
@@ -5113,7 +5161,7 @@
         <f t="shared" si="44"/>
         <v>4621038.4266666658</v>
       </c>
-      <c r="H80" s="59">
+      <c r="H80" s="48">
         <f t="shared" si="44"/>
         <v>5545246.1119999997</v>
       </c>
@@ -5121,7 +5169,7 @@
         <f t="shared" si="44"/>
         <v>6469453.7973333336</v>
       </c>
-      <c r="J80" s="59">
+      <c r="J80" s="48">
         <f t="shared" si="44"/>
         <v>7393661.4826666666</v>
       </c>
@@ -5131,7 +5179,7 @@
       </c>
     </row>
     <row r="81" spans="4:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="D81" s="60"/>
+      <c r="D81" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5153,6 +5201,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1763D785-0BD3-214B-94B7-2A4B796A3A87}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5">
+        <v>5569000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="20">
+        <v>0</v>
+      </c>
+      <c r="C9" s="34">
+        <f>C2*C5*C1/100</f>
+        <v>1202904000</v>
+      </c>
+      <c r="D9" s="34">
+        <f>C3*C1*(365*24*10)</f>
+        <v>1576800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="61">
+        <f>C9</f>
+        <v>1202904000</v>
+      </c>
+      <c r="D10" s="62">
+        <f>C3*C1*(365*24)*(1-POWER(1/(1+B10),10))/(1-(1/(1+B10)))</f>
+        <v>1065762875.3502659</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17762179-2135-43B7-98DA-D4A6A7868310}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -5178,10 +5330,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58"/>
+      <c r="B2" s="56"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -5309,7 +5461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -5349,26 +5501,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5440,15 +5592,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5526,22 +5678,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -5555,11 +5707,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -5600,7 +5752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -5775,7 +5927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D919D22-7A01-ED42-B8B2-84358A3D7717}">
   <dimension ref="A1:P25"/>
   <sheetViews>
@@ -6282,7 +6434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -6414,7 +6566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
   <dimension ref="A1:E10"/>
   <sheetViews>

</xml_diff>

<commit_message>
ITC and ptc calculations for advanced nuclear
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF6F3B-9FAD-3146-A6A7-2F8CF1903596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E886DE9-EBB4-2B41-8A96-8F6D19EF26E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-1600" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="35840" yWindow="-1100" windowWidth="38400" windowHeight="23500" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="SMR" sheetId="13" r:id="rId1"/>
@@ -1106,6 +1106,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="3" borderId="18" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="5"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1139,8 +1141,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="5" builtinId="22"/>
@@ -2783,26 +2783,26 @@
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="C13" t="s">
         <v>189</v>
       </c>
@@ -2943,19 +2943,19 @@
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="61"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
@@ -3224,19 +3224,19 @@
     </row>
     <row r="29" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="61"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="45" t="s">
@@ -3523,31 +3523,31 @@
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
-      <c r="D39" s="60" t="str">
+      <c r="D39" s="62" t="str">
         <f>A14</f>
         <v>Ref</v>
       </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="60" t="str">
+      <c r="E39" s="53"/>
+      <c r="F39" s="62" t="str">
         <f>A15</f>
         <v>20MWe</v>
       </c>
-      <c r="G39" s="51"/>
-      <c r="H39" s="60" t="str">
+      <c r="G39" s="53"/>
+      <c r="H39" s="62" t="str">
         <f>A16</f>
         <v>40MWe</v>
       </c>
-      <c r="I39" s="51"/>
-      <c r="J39" s="60" t="str">
+      <c r="I39" s="53"/>
+      <c r="J39" s="62" t="str">
         <f>A35</f>
         <v>80MWe</v>
       </c>
-      <c r="K39" s="51"/>
-      <c r="L39" s="50" t="str">
+      <c r="K39" s="53"/>
+      <c r="L39" s="52" t="str">
         <f>A36</f>
         <v>100MWe</v>
       </c>
-      <c r="M39" s="51"/>
+      <c r="M39" s="53"/>
     </row>
     <row r="40" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
@@ -5290,11 +5290,11 @@
       <c r="B10" s="20">
         <v>0.1</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="50">
         <f>C9</f>
         <v>1202904000</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="51">
         <f>C3*C1*(365*24)*(1-POWER(1/(1+B10),10))/(1-(1/(1+B10)))</f>
         <v>1065762875.3502659</v>
       </c>
@@ -5330,10 +5330,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="58"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -5501,26 +5501,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5592,15 +5592,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5678,22 +5678,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -5707,11 +5707,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">

</xml_diff>